<commit_message>
Reduced number of items through versioning to avoid Payload bug
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\Dropbox\Personal\Minecraft\Minecraft Raw Data Share\06.07.2014 - alpha launch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\GitHub\polycraft\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="15270" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="17" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9113" uniqueCount="8736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9111" uniqueCount="8736">
   <si>
     <t>Uuo</t>
   </si>
@@ -35257,11 +35257,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:N116"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -36157,6 +36157,7 @@
       <c r="F41" s="8" t="b">
         <v>0</v>
       </c>
+      <c r="G41" s="32"/>
       <c r="H41" s="8" t="str">
         <f>Enums!$A$38</f>
         <v>polyester</v>
@@ -36168,16 +36169,15 @@
         <v>1.0.0</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G42" s="32"/>
+        <v>1</v>
+      </c>
       <c r="H42" s="8" t="str">
         <f>Enums!$A$38</f>
         <v>polyester</v>
@@ -36189,18 +36189,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" s="8" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
+        <v>0</v>
+      </c>
+      <c r="H43" s="32" t="str">
+        <f>Enums!$A$36</f>
+        <v>polycarbonate</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -36209,18 +36209,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H44" s="32" t="str">
-        <f>Enums!$A$36</f>
-        <v>polycarbonate</v>
+      <c r="H44" s="8" t="str">
+        <f>Enums!$A$50</f>
+        <v>synthetic rubber</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -36229,11 +36229,12 @@
         <v>1.0.0</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>1289</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>1288</v>
-      </c>
+        <v>1287</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D45" s="32"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="b">
         <v>0</v>
@@ -36245,23 +36246,22 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>1287</v>
-      </c>
-      <c r="C46" s="32" t="s">
-        <v>1286</v>
-      </c>
-      <c r="D46" s="32"/>
+        <v>1285</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1284</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H46" s="8" t="str">
-        <f>Enums!$A$50</f>
-        <v>synthetic rubber</v>
+        <f>Enums!$A$49</f>
+        <v>silicone</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -36270,18 +36270,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H47" s="8" t="str">
-        <f>Enums!$A$49</f>
-        <v>silicone</v>
+        <f>Enums!$A$35</f>
+        <v>polyamide</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -36290,18 +36290,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>1283</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>1282</v>
-      </c>
+        <v>1281</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D48" s="32"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H48" s="8" t="str">
-        <f>Enums!$A$35</f>
-        <v>polyamide</v>
+        <f>Enums!$A$40</f>
+        <v>polyimide</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -36310,19 +36311,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>1281</v>
-      </c>
-      <c r="C49" s="32" t="s">
-        <v>1280</v>
-      </c>
-      <c r="D49" s="32"/>
+        <v>1279</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1277</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H49" s="8" t="str">
-        <f>Enums!$A$40</f>
-        <v>polyimide</v>
+      <c r="H49" s="32" t="str">
+        <f>Enums!$A$32</f>
+        <v>polyacrylate</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -36331,18 +36331,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C50" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C50" s="32" t="s">
         <v>1277</v>
       </c>
+      <c r="D50" s="32"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" s="32" t="str">
-        <f>Enums!$A$32</f>
-        <v>polyacrylate</v>
+        <v>1</v>
+      </c>
+      <c r="H50" s="8" t="str">
+        <f>Enums!$A$38</f>
+        <v>polyester</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -36351,62 +36352,61 @@
         <v>1.0.0</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C51" s="32" t="s">
-        <v>1277</v>
-      </c>
-      <c r="D51" s="32"/>
+        <v>1276</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1275</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H51" s="8" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="H51" s="32" t="str">
+        <f>Enums!$A$39</f>
+        <v>polyether</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G52" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="H52" s="32" t="str">
-        <f>Enums!$A$39</f>
-        <v>polyether</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H52" s="8" t="str">
+        <f>Enums!$A$46</f>
+        <v>polyurethane</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H53" s="8" t="str">
-        <f>Enums!$A$46</f>
-        <v>polyurethane</v>
+        <f>Enums!$A$38</f>
+        <v>polyester</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -36415,18 +36415,22 @@
         <v>1.0.0</v>
       </c>
       <c r="B54" s="33" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>1271</v>
-      </c>
+        <v>1270</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D54" s="32"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H54" s="8" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
+      <c r="G54" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="H54" s="1" t="str">
+        <f>Enums!$A$39</f>
+        <v>polyether</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -36435,22 +36439,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C55" s="32" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D55" s="32"/>
+        <v>1268</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1267</v>
+      </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G55" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="H55" s="1" t="str">
-        <f>Enums!$A$39</f>
-        <v>polyether</v>
+      <c r="H55" s="8" t="str">
+        <f>Enums!$A$34</f>
+        <v>polyalkene sulfide</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -36459,55 +36459,55 @@
         <v>1.0.0</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H56" s="8" t="str">
-        <f>Enums!$A$34</f>
-        <v>polyalkene sulfide</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G56" s="32"/>
+      <c r="H56" s="1" t="str">
+        <f>Enums!$A$38</f>
+        <v>polyester</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G57" s="32"/>
       <c r="H57" s="1" t="str">
         <f>Enums!$A$38</f>
         <v>polyester</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="1" t="str">
         <f>Enums!$A$38</f>
@@ -36520,18 +36520,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B59" s="33" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>1261</v>
-      </c>
+        <v>1260</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H59" s="1" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
+        <v>0</v>
+      </c>
+      <c r="H59" s="32" t="str">
+        <f>Enums!$A$35</f>
+        <v>polyamide</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -36540,10 +36541,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
@@ -36561,31 +36562,31 @@
         <v>1.0.0</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>1257</v>
-      </c>
-      <c r="D61" s="8"/>
+        <v>1256</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D61" s="32"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H61" s="32" t="str">
-        <f>Enums!$A$35</f>
-        <v>polyamide</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="str">
+        <f>Enums!$A$38</f>
+        <v>polyester</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B62" s="33" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="D62" s="32"/>
       <c r="E62" s="8"/>
@@ -36597,25 +36598,24 @@
         <v>polyester</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C63" s="32" t="s">
-        <v>1253</v>
-      </c>
-      <c r="D63" s="32"/>
+        <v>1252</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>1251</v>
+      </c>
       <c r="E63" s="8"/>
       <c r="F63" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H63" s="1" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
+        <v>0</v>
+      </c>
+      <c r="H63" s="8" t="str">
+        <f>Enums!$A$35</f>
+        <v>polyamide</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -36624,18 +36624,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H64" s="8" t="str">
-        <f>Enums!$A$35</f>
-        <v>polyamide</v>
+      <c r="H64" s="1" t="str">
+        <f>Enums!$A$32</f>
+        <v>polyacrylate</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -36644,10 +36644,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="8" t="b">
@@ -36664,18 +36664,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H66" s="1" t="str">
-        <f>Enums!$A$32</f>
-        <v>polyacrylate</v>
+      <c r="H66" s="32" t="str">
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -36684,18 +36684,21 @@
         <v>1.0.0</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>1246</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>1245</v>
-      </c>
-      <c r="E67" s="8"/>
+        <v>1244</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D67" s="8">
+        <v>1</v>
+      </c>
+      <c r="E67" s="32"/>
       <c r="F67" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H67" s="32" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
+      <c r="H67" s="8" t="str">
+        <f>Enums!$A$31</f>
+        <v>natural rubber</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -36704,21 +36707,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B68" s="33" t="s">
-        <v>1244</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D68" s="8">
+        <v>1242</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" s="8" t="str">
-        <f>Enums!$A$31</f>
-        <v>natural rubber</v>
+      <c r="H68" s="32" t="str">
+        <f>Enums!$A$38</f>
+        <v>polyester</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -36727,10 +36727,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="8" t="b">
@@ -36747,18 +36747,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B70" s="33" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" s="32" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
+        <f>Enums!$A$32</f>
+        <v>polyacrylate</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -36767,10 +36767,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B71" s="33" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="8" t="b">
@@ -36787,10 +36787,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B72" s="33" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="8" t="b">
@@ -36807,18 +36807,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B73" s="33" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H73" s="32" t="str">
-        <f>Enums!$A$32</f>
-        <v>polyacrylate</v>
+      <c r="H73" s="1" t="str">
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -36827,18 +36827,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B74" s="33" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>1231</v>
-      </c>
+        <v>1230</v>
+      </c>
+      <c r="C74" s="32" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D74" s="32"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
+        <f>Enums!$A$43</f>
+        <v>polyphenol</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -36847,19 +36848,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C75" s="32" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D75" s="32"/>
+        <v>1228</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1227</v>
+      </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H75" s="1" t="str">
-        <f>Enums!$A$43</f>
-        <v>polyphenol</v>
+      <c r="H75" s="32" t="str">
+        <f>Enums!$A$32</f>
+        <v>polyacrylate</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -36868,60 +36868,60 @@
         <v>1.0.0</v>
       </c>
       <c r="B76" s="33" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H76" s="32" t="str">
-        <f>Enums!$A$32</f>
-        <v>polyacrylate</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H76" s="1" t="str">
+        <f>Enums!$A$39</f>
+        <v>polyether</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B77" s="33" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="E77" s="8"/>
       <c r="F77" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H77" s="1" t="str">
-        <f>Enums!$A$39</f>
-        <v>polyether</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H77" s="8" t="str">
+        <f>Enums!$A$46</f>
+        <v>polyurethane</v>
+      </c>
+      <c r="I77" s="32"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B78" s="33" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1223</v>
+        <v>1211</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H78" s="8" t="str">
-        <f>Enums!$A$46</f>
-        <v>polyurethane</v>
-      </c>
-      <c r="I78" s="32"/>
+        <f>Enums!$A$43</f>
+        <v>polyphenol</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="str">
@@ -36929,10 +36929,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B79" s="33" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1211</v>
+        <v>1220</v>
       </c>
       <c r="E79" s="8"/>
       <c r="F79" s="8" t="b">
@@ -36949,18 +36949,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B80" s="33" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>1220</v>
-      </c>
+        <v>1219</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D80" s="8"/>
       <c r="E80" s="8"/>
       <c r="F80" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H80" s="8" t="str">
-        <f>Enums!$A$43</f>
-        <v>polyphenol</v>
+        <f>Enums!$A$30</f>
+        <v>inorganic-organic polymer</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -36969,19 +36970,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B81" s="33" t="s">
-        <v>1219</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D81" s="8"/>
+        <v>1217</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1216</v>
+      </c>
       <c r="E81" s="8"/>
       <c r="F81" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H81" s="8" t="str">
-        <f>Enums!$A$30</f>
-        <v>inorganic-organic polymer</v>
+      <c r="H81" s="1" t="str">
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -36990,18 +36990,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B82" s="33" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="E82" s="8"/>
       <c r="F82" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
+        <f>Enums!$A$43</f>
+        <v>polyphenol</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -37010,10 +37010,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B83" s="33" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="8" t="b">
@@ -37030,18 +37030,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B84" s="33" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>Enums!$A$43</f>
-        <v>polyphenol</v>
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -37050,18 +37050,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B85" s="33" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
+        <f>Enums!$A$39</f>
+        <v>polyether</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -37070,10 +37070,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B86" s="33" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="8" t="b">
@@ -37090,18 +37090,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B87" s="33" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>Enums!$A$39</f>
-        <v>polyether</v>
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -37110,18 +37110,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B88" s="33" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H88" s="1" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
+      <c r="H88" s="32" t="str">
+        <f>Enums!$A$32</f>
+        <v>polyacrylate</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -37130,18 +37130,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B89" s="33" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>1201</v>
-      </c>
+        <v>1200</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H89" s="32" t="str">
-        <f>Enums!$A$32</f>
-        <v>polyacrylate</v>
+      <c r="H89" s="8" t="str">
+        <f>Enums!$A$28</f>
+        <v>fluoropolymer</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -37150,19 +37151,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B90" s="33" t="s">
-        <v>1200</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>1199</v>
-      </c>
-      <c r="D90" s="8"/>
+        <v>1198</v>
+      </c>
+      <c r="C90" s="32" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D90" s="32"/>
       <c r="E90" s="8"/>
       <c r="F90" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H90" s="8" t="str">
-        <f>Enums!$A$28</f>
-        <v>fluoropolymer</v>
+      <c r="H90" s="1" t="str">
+        <f>Enums!$A$39</f>
+        <v>polyether</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -37171,12 +37172,11 @@
         <v>1.0.0</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>1198</v>
-      </c>
-      <c r="C91" s="32" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D91" s="32"/>
+        <v>1196</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>1195</v>
+      </c>
       <c r="E91" s="8"/>
       <c r="F91" s="8" t="b">
         <v>0</v>
@@ -37192,18 +37192,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H92" s="1" t="str">
-        <f>Enums!$A$39</f>
-        <v>polyether</v>
+      <c r="H92" s="8" t="str">
+        <f>Enums!$A$29</f>
+        <v>inorganic polymer</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -37212,18 +37212,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B93" s="33" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="E93" s="8"/>
       <c r="F93" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H93" s="8" t="str">
-        <f>Enums!$A$29</f>
-        <v>inorganic polymer</v>
+        <f>Enums!$A$38</f>
+        <v>polyester</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -37232,18 +37232,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B94" s="33" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>1191</v>
-      </c>
+        <v>1190</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D94" s="8"/>
       <c r="E94" s="8"/>
       <c r="F94" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H94" s="8" t="str">
-        <f>Enums!$A$38</f>
-        <v>polyester</v>
+        <f>Enums!$A$46</f>
+        <v>polyurethane</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -37252,19 +37253,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>1189</v>
-      </c>
-      <c r="D95" s="8"/>
+        <v>1188</v>
+      </c>
+      <c r="C95" s="32" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D95" s="32"/>
       <c r="E95" s="8"/>
       <c r="F95" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H95" s="8" t="str">
-        <f>Enums!$A$46</f>
-        <v>polyurethane</v>
+        <f>Enums!$A$48</f>
+        <v>polyvinyl ester</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -37273,19 +37274,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B96" s="33" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C96" s="32" t="s">
-        <v>1187</v>
-      </c>
-      <c r="D96" s="32"/>
+        <v>1186</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1185</v>
+      </c>
       <c r="E96" s="8"/>
       <c r="F96" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96" s="8" t="str">
-        <f>Enums!$A$48</f>
-        <v>polyvinyl ester</v>
+        <f>Enums!$A$47</f>
+        <v>polyvinyl</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -37294,17 +37294,17 @@
         <v>1.0.0</v>
       </c>
       <c r="B97" s="33" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" s="8" t="str">
-        <f>Enums!$A$47</f>
+        <f>[1]Enums!$A$47</f>
         <v>polyvinyl</v>
       </c>
     </row>
@@ -37314,18 +37314,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B98" s="33" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H98" s="8" t="str">
-        <f>[1]Enums!$A$47</f>
-        <v>polyvinyl</v>
+      <c r="H98" s="1" t="str">
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -37334,18 +37334,19 @@
         <v>1.0.0</v>
       </c>
       <c r="B99" s="33" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>1181</v>
-      </c>
+        <v>1180</v>
+      </c>
+      <c r="C99" s="32" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D99" s="32"/>
       <c r="E99" s="8"/>
       <c r="F99" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H99" s="1" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
+      <c r="H99" s="8" t="str">
+        <f>Enums!$A$48</f>
+        <v>polyvinyl ester</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -37354,19 +37355,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B100" s="33" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C100" s="32" t="s">
-        <v>1179</v>
-      </c>
-      <c r="D100" s="32"/>
+        <v>1178</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1177</v>
+      </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H100" s="8" t="str">
-        <f>Enums!$A$48</f>
-        <v>polyvinyl ester</v>
+        <f>Enums!$A$28</f>
+        <v>fluoropolymer</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -37375,18 +37375,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B101" s="33" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H101" s="8" t="str">
-        <f>Enums!$A$28</f>
-        <v>fluoropolymer</v>
+        <f>[1]Enums!$A$47</f>
+        <v>polyvinyl</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -37395,10 +37395,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B102" s="33" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8" t="b">
@@ -37415,10 +37415,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B103" s="33" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="8" t="b">
@@ -37435,30 +37435,30 @@
         <v>1.0.0</v>
       </c>
       <c r="B104" s="33" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H104" s="8" t="str">
-        <f>[1]Enums!$A$47</f>
-        <v>polyvinyl</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+        <f>Enums!$A$28</f>
+        <v>fluoropolymer</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B105" s="33" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="8" t="b">
@@ -37469,24 +37469,24 @@
         <v>fluoropolymer</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B106" s="33" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E106" s="8"/>
+        <v>1165</v>
+      </c>
+      <c r="E106" s="32"/>
       <c r="F106" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H106" s="8" t="str">
-        <f>Enums!$A$28</f>
-        <v>fluoropolymer</v>
+        <f>Enums!$A$50</f>
+        <v>synthetic rubber</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -37495,12 +37495,11 @@
         <v>1.0.0</v>
       </c>
       <c r="B107" s="33" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E107" s="32"/>
+        <v>1163</v>
+      </c>
       <c r="F107" s="8" t="b">
         <v>0</v>
       </c>
@@ -37515,10 +37514,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B108" s="33" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="F108" s="8" t="b">
         <v>0</v>
@@ -37534,10 +37533,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B109" s="33" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="F109" s="8" t="b">
         <v>0</v>
@@ -37553,11 +37552,12 @@
         <v>1.0.0</v>
       </c>
       <c r="B110" s="33" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1159</v>
-      </c>
+        <v>1157</v>
+      </c>
+      <c r="E110" s="32"/>
       <c r="F110" s="8" t="b">
         <v>0</v>
       </c>
@@ -37566,71 +37566,71 @@
         <v>synthetic rubber</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B111" s="33" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1157</v>
-      </c>
-      <c r="E111" s="32"/>
+        <v>1155</v>
+      </c>
+      <c r="E111" s="8"/>
       <c r="F111" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H111" s="8" t="str">
-        <f>Enums!$A$50</f>
-        <v>synthetic rubber</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H111" s="1" t="str">
+        <f>Enums!$A$42</f>
+        <v>polyolefin</v>
+      </c>
+      <c r="I111" s="32"/>
+      <c r="J111" s="32"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B112" s="33" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E112" s="8"/>
+        <v>1153</v>
+      </c>
+      <c r="E112" s="32"/>
       <c r="F112" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H112" s="1" t="str">
+      <c r="H112" s="32" t="str">
+        <f>Enums!$A$33</f>
+        <v>polyaldehyde</v>
+      </c>
+      <c r="I112" s="8" t="str">
+        <f>Enums!$A$35</f>
+        <v>polyamide</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B113" s="33" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" s="1" t="str">
         <f>Enums!$A$42</f>
         <v>polyolefin</v>
       </c>
-      <c r="I112" s="32"/>
-      <c r="J112" s="32"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B113" s="33" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>1153</v>
-      </c>
-      <c r="E113" s="32"/>
-      <c r="F113" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H113" s="32" t="str">
-        <f>Enums!$A$33</f>
-        <v>polyaldehyde</v>
-      </c>
-      <c r="I113" s="8" t="str">
-        <f>Enums!$A$35</f>
-        <v>polyamide</v>
-      </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="str">
@@ -37638,54 +37638,34 @@
         <v>1.0.0</v>
       </c>
       <c r="B114" s="33" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1151</v>
-      </c>
-      <c r="E114" s="8"/>
+        <v>1149</v>
+      </c>
+      <c r="E114" s="32"/>
       <c r="F114" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H114" s="1" t="str">
-        <f>Enums!$A$42</f>
-        <v>polyolefin</v>
-      </c>
+      <c r="H114" s="8" t="str">
+        <f>Enums!$A$32</f>
+        <v>polyacrylate</v>
+      </c>
+      <c r="I114" s="8" t="str">
+        <f>Enums!$A$47</f>
+        <v>polyvinyl</v>
+      </c>
+      <c r="J114" s="8"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B115" s="33" t="s">
-        <v>1150</v>
+      <c r="B115" s="1" t="s">
+        <v>8734</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1149</v>
-      </c>
-      <c r="E115" s="32"/>
-      <c r="F115" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H115" s="8" t="str">
-        <f>Enums!$A$32</f>
-        <v>polyacrylate</v>
-      </c>
-      <c r="I115" s="8" t="str">
-        <f>Enums!$A$47</f>
-        <v>polyvinyl</v>
-      </c>
-      <c r="J115" s="8"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>8734</v>
-      </c>
-      <c r="C116" s="1" t="s">
         <v>8733</v>
       </c>
     </row>
@@ -41759,7 +41739,7 @@
   </sheetPr>
   <dimension ref="A1:K6104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Playable version from 7.6.14 - major brick bug
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9099" uniqueCount="8724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9097" uniqueCount="8722">
   <si>
     <t>Uuo</t>
   </si>
@@ -26447,12 +26447,6 @@
   </si>
   <si>
     <t>State</t>
-  </si>
-  <si>
-    <t>5m</t>
-  </si>
-  <si>
-    <t>5j</t>
   </si>
   <si>
     <t>59</t>
@@ -27697,10 +27691,10 @@
   <dimension ref="A1:J338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C164" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C152" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E327" sqref="E327"/>
+      <selection pane="bottomRight" activeCell="C169" sqref="A1:H337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31026,10 +31020,6 @@
       <c r="H147" s="18"/>
     </row>
     <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
       <c r="B148" s="8" t="s">
         <v>742</v>
       </c>
@@ -31164,10 +31154,6 @@
       </c>
     </row>
     <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
       <c r="B154" s="1" t="s">
         <v>726</v>
       </c>
@@ -32486,10 +32472,6 @@
       <c r="H212" s="18"/>
     </row>
     <row r="213" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A213" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
       <c r="B213" s="8" t="s">
         <v>595</v>
       </c>
@@ -32551,7 +32533,7 @@
       <c r="G215" s="12"/>
       <c r="H215" s="12"/>
     </row>
-    <row r="216" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
@@ -32618,10 +32600,7 @@
       </c>
     </row>
     <row r="219" spans="1:8" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A219" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
+      <c r="A219" s="1"/>
       <c r="B219" s="19" t="s">
         <v>577</v>
       </c>
@@ -34868,7 +34847,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>8583</v>
+        <v>8581</v>
       </c>
       <c r="C318" s="14"/>
       <c r="D318" s="12" t="str">
@@ -35224,8 +35203,8 @@
   <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B109" sqref="A1:N115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -37627,10 +37606,17 @@
         <v>1.0.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>8722</v>
+        <v>8720</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>8721</v>
+        <v>8719</v>
+      </c>
+      <c r="F115" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" s="8" t="str">
+        <f>Enums!$A$35</f>
+        <v>polyamide</v>
       </c>
     </row>
   </sheetData>
@@ -37797,7 +37783,7 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
@@ -37805,9 +37791,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
@@ -37864,7 +37850,7 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -37892,7 +37878,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>200</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -37920,7 +37906,7 @@
         <v>20</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -37929,7 +37915,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" ref="B5:B7" si="1">D5</f>
+        <f t="shared" ref="B5:B18" si="1">D5</f>
         <v>Methane</v>
       </c>
       <c r="C5" t="str">
@@ -37941,21 +37927,379 @@
         <v>Methane</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E7" si="2" xml:space="preserve"> E4 + 1</f>
+        <f t="shared" ref="E5:E18" si="2" xml:space="preserve"> E4 + 1</f>
         <v>3</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="1"/>
+        <v>Diesel</v>
+      </c>
+      <c r="C6" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D6" t="str">
+        <f>Compounds!B116</f>
+        <v>Diesel</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="1"/>
+        <v>Kerosene</v>
+      </c>
+      <c r="C7" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D7" t="str">
+        <f>Compounds!B163</f>
+        <v>Kerosene</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="1"/>
+        <v>Liquified Natural Gas</v>
+      </c>
+      <c r="C8" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D8" t="str">
+        <f>Compounds!B171</f>
+        <v>Liquified Natural Gas</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F8">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="G8">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="1"/>
+        <v>Naphtha</v>
+      </c>
+      <c r="C9" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D9" t="str">
+        <f>Compounds!B208</f>
+        <v>Naphtha</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="1"/>
+        <v>Naphthalene</v>
+      </c>
+      <c r="C10" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D10" t="str">
+        <f>Compounds!B209</f>
+        <v>Naphthalene</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="1"/>
+        <v>Propane</v>
+      </c>
+      <c r="C11" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D11" t="str">
+        <f>Compounds!B246</f>
+        <v>Propane</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>Ethane</v>
+      </c>
+      <c r="C12" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D12" t="str">
+        <f>Compounds!B125</f>
+        <v>Ethane</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>Sweet Butane Fuel</v>
+      </c>
+      <c r="C13" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D13" t="str">
+        <f>Compounds!B279</f>
+        <v>Sweet Butane Fuel</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>Sweet Propane Fuel</v>
+      </c>
+      <c r="C14" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D14" t="str">
+        <f>Compounds!B280</f>
+        <v>Sweet Propane Fuel</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>Sweet Light Naphtha</v>
+      </c>
+      <c r="C15" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D15" t="str">
+        <f>Compounds!B281</f>
+        <v>Sweet Light Naphtha</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>Town Gas</v>
+      </c>
+      <c r="C16" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D16" t="str">
+        <f>Compounds!B292</f>
+        <v>Town Gas</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>Light Naphtha</v>
+      </c>
+      <c r="C17" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D17" t="str">
+        <f>Compounds!B167</f>
+        <v>Light Naphtha</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="1"/>
+        <v>Light Naphthenes</v>
+      </c>
+      <c r="C18" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D18" t="str">
+        <f>Compounds!B168</f>
+        <v>Light Naphthenes</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -38777,7 +39121,7 @@
         <v>1375</v>
       </c>
       <c r="F91" s="64" t="s">
-        <v>8591</v>
+        <v>8589</v>
       </c>
       <c r="G91" s="64" t="s">
         <v>1377</v>
@@ -38786,25 +39130,25 @@
         <v>1414</v>
       </c>
       <c r="I91" s="64" t="s">
-        <v>8592</v>
+        <v>8590</v>
       </c>
       <c r="J91" s="64" t="s">
-        <v>8593</v>
+        <v>8591</v>
       </c>
       <c r="K91" s="64" t="s">
         <v>1374</v>
       </c>
       <c r="L91" s="64" t="s">
-        <v>8594</v>
+        <v>8592</v>
       </c>
       <c r="M91" s="64" t="s">
         <v>1373</v>
       </c>
       <c r="N91" s="64" t="s">
-        <v>8595</v>
+        <v>8593</v>
       </c>
       <c r="O91" s="64" t="s">
-        <v>8596</v>
+        <v>8594</v>
       </c>
       <c r="P91" s="64" t="s">
         <v>1372</v>
@@ -38819,67 +39163,67 @@
         <v>1369</v>
       </c>
       <c r="T91" s="64" t="s">
+        <v>8595</v>
+      </c>
+      <c r="U91" s="64" t="s">
+        <v>8596</v>
+      </c>
+      <c r="V91" s="64" t="s">
         <v>8597</v>
       </c>
-      <c r="U91" s="64" t="s">
+      <c r="W91" s="64" t="s">
         <v>8598</v>
       </c>
-      <c r="V91" s="64" t="s">
+      <c r="X91" s="64" t="s">
         <v>8599</v>
       </c>
-      <c r="W91" s="64" t="s">
+      <c r="Y91" s="64" t="s">
         <v>8600</v>
       </c>
-      <c r="X91" s="64" t="s">
+      <c r="Z91" s="64" t="s">
         <v>8601</v>
       </c>
-      <c r="Y91" s="64" t="s">
+      <c r="AA91" s="64" t="s">
         <v>8602</v>
       </c>
-      <c r="Z91" s="64" t="s">
+      <c r="AB91" s="64" t="s">
         <v>8603</v>
       </c>
-      <c r="AA91" s="64" t="s">
+      <c r="AC91" s="64" t="s">
         <v>8604</v>
       </c>
-      <c r="AB91" s="64" t="s">
+      <c r="AD91" s="64" t="s">
         <v>8605</v>
       </c>
-      <c r="AC91" s="64" t="s">
+      <c r="AE91" s="64" t="s">
         <v>8606</v>
       </c>
-      <c r="AD91" s="64" t="s">
+      <c r="AF91" s="64" t="s">
         <v>8607</v>
       </c>
-      <c r="AE91" s="64" t="s">
+      <c r="AG91" s="64" t="s">
         <v>8608</v>
       </c>
-      <c r="AF91" s="64" t="s">
+      <c r="AH91" s="64" t="s">
         <v>8609</v>
       </c>
-      <c r="AG91" s="64" t="s">
+      <c r="AI91" s="64" t="s">
         <v>8610</v>
       </c>
-      <c r="AH91" s="64" t="s">
+      <c r="AJ91" s="64" t="s">
         <v>8611</v>
       </c>
-      <c r="AI91" s="64" t="s">
+      <c r="AK91" s="64" t="s">
         <v>8612</v>
       </c>
-      <c r="AJ91" s="64" t="s">
+      <c r="AL91" s="64" t="s">
         <v>8613</v>
       </c>
-      <c r="AK91" s="64" t="s">
+      <c r="AM91" s="64" t="s">
         <v>8614</v>
       </c>
-      <c r="AL91" s="64" t="s">
+      <c r="AN91" s="64" t="s">
         <v>8615</v>
-      </c>
-      <c r="AM91" s="64" t="s">
-        <v>8616</v>
-      </c>
-      <c r="AN91" s="64" t="s">
-        <v>8617</v>
       </c>
     </row>
     <row r="92" spans="1:40" ht="39" x14ac:dyDescent="0.25">
@@ -38888,13 +39232,13 @@
         <v>1</v>
       </c>
       <c r="F92" s="66" t="s">
-        <v>8618</v>
+        <v>8616</v>
       </c>
       <c r="G92" s="67" t="s">
         <v>1265</v>
       </c>
       <c r="H92" s="67" t="s">
-        <v>8619</v>
+        <v>8617</v>
       </c>
       <c r="I92" s="66" t="str">
         <f>"Fiber ("&amp;F92&amp;")"</f>
@@ -38916,40 +39260,40 @@
         <v>4</v>
       </c>
       <c r="P92" s="67" t="s">
+        <v>8618</v>
+      </c>
+      <c r="Q92" s="67" t="s">
+        <v>8619</v>
+      </c>
+      <c r="R92" s="67" t="s">
         <v>8620</v>
       </c>
-      <c r="Q92" s="67" t="s">
+      <c r="S92" s="67" t="s">
         <v>8621</v>
       </c>
-      <c r="R92" s="67" t="s">
+      <c r="T92" s="67" t="s">
         <v>8622</v>
       </c>
-      <c r="S92" s="67" t="s">
+      <c r="U92" s="67" t="s">
         <v>8623</v>
       </c>
-      <c r="T92" s="67" t="s">
+      <c r="V92" s="67" t="s">
         <v>8624</v>
       </c>
-      <c r="U92" s="67" t="s">
+      <c r="W92" s="67" t="s">
         <v>8625</v>
       </c>
-      <c r="V92" s="67" t="s">
+      <c r="X92" s="67" t="s">
         <v>8626</v>
       </c>
-      <c r="W92" s="67" t="s">
+      <c r="Y92" s="67" t="s">
         <v>8627</v>
       </c>
-      <c r="X92" s="67" t="s">
+      <c r="Z92" s="67" t="s">
         <v>8628</v>
       </c>
-      <c r="Y92" s="67" t="s">
+      <c r="AA92" s="67" t="s">
         <v>8629</v>
-      </c>
-      <c r="Z92" s="67" t="s">
-        <v>8630</v>
-      </c>
-      <c r="AA92" s="67" t="s">
-        <v>8631</v>
       </c>
       <c r="AB92"/>
       <c r="AC92"/>
@@ -38971,13 +39315,13 @@
         <v>2</v>
       </c>
       <c r="F93" s="66" t="s">
-        <v>8632</v>
+        <v>8630</v>
       </c>
       <c r="G93" s="67" t="s">
         <v>1339</v>
       </c>
       <c r="H93" s="67" t="s">
-        <v>8633</v>
+        <v>8631</v>
       </c>
       <c r="I93" s="66" t="str">
         <f t="shared" ref="I93:I102" si="1">"Fiber ("&amp;F93&amp;")"</f>
@@ -38999,34 +39343,34 @@
         <v>4</v>
       </c>
       <c r="P93" s="67" t="s">
+        <v>8632</v>
+      </c>
+      <c r="Q93" s="67" t="s">
+        <v>8633</v>
+      </c>
+      <c r="R93" s="67" t="s">
         <v>8634</v>
       </c>
-      <c r="Q93" s="67" t="s">
+      <c r="S93" s="67" t="s">
         <v>8635</v>
       </c>
-      <c r="R93" s="67" t="s">
+      <c r="T93" s="67" t="s">
         <v>8636</v>
       </c>
-      <c r="S93" s="67" t="s">
+      <c r="U93" s="67" t="s">
         <v>8637</v>
       </c>
-      <c r="T93" s="67" t="s">
+      <c r="V93" s="67" t="s">
         <v>8638</v>
       </c>
-      <c r="U93" s="67" t="s">
+      <c r="W93" s="67" t="s">
         <v>8639</v>
       </c>
-      <c r="V93" s="67" t="s">
+      <c r="X93" s="67" t="s">
         <v>8640</v>
       </c>
-      <c r="W93" s="67" t="s">
+      <c r="Y93" s="67" t="s">
         <v>8641</v>
-      </c>
-      <c r="X93" s="67" t="s">
-        <v>8642</v>
-      </c>
-      <c r="Y93" s="67" t="s">
-        <v>8643</v>
       </c>
       <c r="Z93"/>
       <c r="AA93"/>
@@ -39056,7 +39400,7 @@
         <v>1181</v>
       </c>
       <c r="H94" s="67" t="s">
-        <v>8633</v>
+        <v>8631</v>
       </c>
       <c r="I94" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39078,34 +39422,34 @@
         <v>4</v>
       </c>
       <c r="P94" s="67" t="s">
+        <v>8642</v>
+      </c>
+      <c r="Q94" s="67" t="s">
+        <v>8643</v>
+      </c>
+      <c r="R94" s="67" t="s">
         <v>8644</v>
       </c>
-      <c r="Q94" s="67" t="s">
+      <c r="S94" s="67" t="s">
         <v>8645</v>
       </c>
-      <c r="R94" s="67" t="s">
+      <c r="T94" s="67" t="s">
         <v>8646</v>
       </c>
-      <c r="S94" s="67" t="s">
+      <c r="U94" s="67" t="s">
         <v>8647</v>
       </c>
-      <c r="T94" s="67" t="s">
+      <c r="V94" s="67" t="s">
         <v>8648</v>
       </c>
-      <c r="U94" s="67" t="s">
+      <c r="W94" s="67" t="s">
         <v>8649</v>
       </c>
-      <c r="V94" s="67" t="s">
+      <c r="X94" s="67" t="s">
         <v>8650</v>
       </c>
-      <c r="W94" s="67" t="s">
+      <c r="Y94" s="67" t="s">
         <v>8651</v>
-      </c>
-      <c r="X94" s="67" t="s">
-        <v>8652</v>
-      </c>
-      <c r="Y94" s="67" t="s">
-        <v>8653</v>
       </c>
       <c r="Z94"/>
       <c r="AA94"/>
@@ -39129,13 +39473,13 @@
         <v>4</v>
       </c>
       <c r="F95" s="66" t="s">
-        <v>8654</v>
+        <v>8652</v>
       </c>
       <c r="G95" s="67" t="s">
         <v>1327</v>
       </c>
       <c r="H95" s="67" t="s">
-        <v>8633</v>
+        <v>8631</v>
       </c>
       <c r="I95" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39160,19 +39504,19 @@
         <v>8445</v>
       </c>
       <c r="Q95" s="67" t="s">
+        <v>8653</v>
+      </c>
+      <c r="R95" s="67" t="s">
+        <v>8654</v>
+      </c>
+      <c r="S95" s="67" t="s">
         <v>8655</v>
-      </c>
-      <c r="R95" s="67" t="s">
-        <v>8656</v>
-      </c>
-      <c r="S95" s="67" t="s">
-        <v>8657</v>
       </c>
       <c r="T95" s="67" t="s">
         <v>8471</v>
       </c>
       <c r="U95" s="67" t="s">
-        <v>8658</v>
+        <v>8656</v>
       </c>
       <c r="V95"/>
       <c r="W95"/>
@@ -39206,7 +39550,7 @@
         <v>1209</v>
       </c>
       <c r="H96" s="67" t="s">
-        <v>8633</v>
+        <v>8631</v>
       </c>
       <c r="I96" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39228,61 +39572,61 @@
         <v>4</v>
       </c>
       <c r="P96" s="67" t="s">
-        <v>8647</v>
+        <v>8645</v>
       </c>
       <c r="Q96" s="67" t="s">
         <v>8445</v>
       </c>
       <c r="R96" s="67" t="s">
-        <v>8656</v>
+        <v>8654</v>
       </c>
       <c r="S96" s="67" t="s">
+        <v>8657</v>
+      </c>
+      <c r="T96" s="67" t="s">
+        <v>8658</v>
+      </c>
+      <c r="U96" s="67" t="s">
         <v>8659</v>
       </c>
-      <c r="T96" s="67" t="s">
+      <c r="V96" s="67" t="s">
         <v>8660</v>
       </c>
-      <c r="U96" s="67" t="s">
+      <c r="W96" s="67" t="s">
         <v>8661</v>
       </c>
-      <c r="V96" s="67" t="s">
+      <c r="X96" s="67" t="s">
         <v>8662</v>
       </c>
-      <c r="W96" s="67" t="s">
+      <c r="Y96" s="67" t="s">
         <v>8663</v>
       </c>
-      <c r="X96" s="67" t="s">
+      <c r="Z96" s="67" t="s">
         <v>8664</v>
       </c>
-      <c r="Y96" s="67" t="s">
+      <c r="AA96" s="67" t="s">
         <v>8665</v>
       </c>
-      <c r="Z96" s="67" t="s">
+      <c r="AB96" s="67" t="s">
         <v>8666</v>
       </c>
-      <c r="AA96" s="67" t="s">
+      <c r="AC96" s="67" t="s">
         <v>8667</v>
       </c>
-      <c r="AB96" s="67" t="s">
+      <c r="AD96" s="67" t="s">
         <v>8668</v>
       </c>
-      <c r="AC96" s="67" t="s">
+      <c r="AE96" s="67" t="s">
         <v>8669</v>
       </c>
-      <c r="AD96" s="67" t="s">
+      <c r="AF96" s="67" t="s">
         <v>8670</v>
       </c>
-      <c r="AE96" s="67" t="s">
+      <c r="AG96" s="67" t="s">
         <v>8671</v>
       </c>
-      <c r="AF96" s="67" t="s">
+      <c r="AH96" s="67" t="s">
         <v>8672</v>
-      </c>
-      <c r="AG96" s="67" t="s">
-        <v>8673</v>
-      </c>
-      <c r="AH96" s="67" t="s">
-        <v>8674</v>
       </c>
       <c r="AI96"/>
       <c r="AJ96"/>
@@ -39303,7 +39647,7 @@
         <v>1203</v>
       </c>
       <c r="H97" s="67" t="s">
-        <v>8633</v>
+        <v>8631</v>
       </c>
       <c r="I97" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39327,28 +39671,28 @@
         <v>4</v>
       </c>
       <c r="P97" s="67" t="s">
-        <v>8675</v>
+        <v>8673</v>
       </c>
       <c r="Q97" s="67" t="s">
-        <v>8676</v>
+        <v>8674</v>
       </c>
       <c r="R97" s="67" t="s">
         <v>8457</v>
       </c>
       <c r="S97" s="67" t="s">
+        <v>8675</v>
+      </c>
+      <c r="T97" s="67" t="s">
+        <v>8676</v>
+      </c>
+      <c r="U97" s="67" t="s">
         <v>8677</v>
       </c>
-      <c r="T97" s="67" t="s">
+      <c r="V97" s="67" t="s">
         <v>8678</v>
       </c>
-      <c r="U97" s="67" t="s">
+      <c r="W97" s="67" t="s">
         <v>8679</v>
-      </c>
-      <c r="V97" s="67" t="s">
-        <v>8680</v>
-      </c>
-      <c r="W97" s="67" t="s">
-        <v>8681</v>
       </c>
       <c r="X97"/>
       <c r="Y97"/>
@@ -39380,7 +39724,7 @@
         <v>220</v>
       </c>
       <c r="H98" s="67" t="s">
-        <v>8682</v>
+        <v>8680</v>
       </c>
       <c r="I98" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39404,50 +39748,50 @@
         <v>4</v>
       </c>
       <c r="P98" s="67" t="s">
+        <v>8681</v>
+      </c>
+      <c r="Q98" s="67" t="s">
+        <v>8682</v>
+      </c>
+      <c r="R98" s="67" t="s">
         <v>8683</v>
       </c>
-      <c r="Q98" s="67" t="s">
+      <c r="S98" s="67" t="s">
         <v>8684</v>
-      </c>
-      <c r="R98" s="67" t="s">
-        <v>8685</v>
-      </c>
-      <c r="S98" s="67" t="s">
-        <v>8686</v>
       </c>
       <c r="T98" s="67"/>
       <c r="U98" s="67" t="s">
+        <v>8685</v>
+      </c>
+      <c r="V98" s="67" t="s">
+        <v>8686</v>
+      </c>
+      <c r="W98" s="67" t="s">
         <v>8687</v>
       </c>
-      <c r="V98" s="67" t="s">
+      <c r="X98" s="67" t="s">
         <v>8688</v>
       </c>
-      <c r="W98" s="67" t="s">
+      <c r="Y98" s="67" t="s">
         <v>8689</v>
       </c>
-      <c r="X98" s="67" t="s">
+      <c r="Z98" s="67" t="s">
         <v>8690</v>
       </c>
-      <c r="Y98" s="67" t="s">
+      <c r="AA98" s="67" t="s">
         <v>8691</v>
       </c>
-      <c r="Z98" s="67" t="s">
+      <c r="AB98" s="67" t="s">
         <v>8692</v>
       </c>
-      <c r="AA98" s="67" t="s">
+      <c r="AC98" s="67" t="s">
         <v>8693</v>
       </c>
-      <c r="AB98" s="67" t="s">
+      <c r="AD98" s="67" t="s">
         <v>8694</v>
       </c>
-      <c r="AC98" s="67" t="s">
+      <c r="AE98" s="67" t="s">
         <v>8695</v>
-      </c>
-      <c r="AD98" s="67" t="s">
-        <v>8696</v>
-      </c>
-      <c r="AE98" s="67" t="s">
-        <v>8697</v>
       </c>
       <c r="AF98"/>
       <c r="AG98"/>
@@ -39471,7 +39815,7 @@
         <v>220</v>
       </c>
       <c r="H99" s="67" t="s">
-        <v>8698</v>
+        <v>8696</v>
       </c>
       <c r="I99" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39493,29 +39837,29 @@
         <v>4</v>
       </c>
       <c r="P99" s="67" t="s">
+        <v>8697</v>
+      </c>
+      <c r="Q99" s="67" t="s">
+        <v>8698</v>
+      </c>
+      <c r="R99" s="67" t="s">
         <v>8699</v>
       </c>
-      <c r="Q99" s="67" t="s">
+      <c r="S99" s="67" t="s">
         <v>8700</v>
       </c>
-      <c r="R99" s="67" t="s">
+      <c r="T99" s="67" t="s">
         <v>8701</v>
       </c>
-      <c r="S99" s="67" t="s">
+      <c r="U99" s="67" t="s">
         <v>8702</v>
       </c>
-      <c r="T99" s="67" t="s">
+      <c r="V99" s="67" t="s">
         <v>8703</v>
-      </c>
-      <c r="U99" s="67" t="s">
-        <v>8704</v>
-      </c>
-      <c r="V99" s="67" t="s">
-        <v>8705</v>
       </c>
       <c r="W99" s="67"/>
       <c r="X99" s="67" t="s">
-        <v>8706</v>
+        <v>8704</v>
       </c>
       <c r="Y99"/>
       <c r="Z99"/>
@@ -39540,13 +39884,13 @@
         <v>0</v>
       </c>
       <c r="F100" s="66" t="s">
-        <v>8707</v>
+        <v>8705</v>
       </c>
       <c r="G100" s="67" t="s">
         <v>7529</v>
       </c>
       <c r="H100" s="67" t="s">
-        <v>8708</v>
+        <v>8706</v>
       </c>
       <c r="I100" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39568,25 +39912,25 @@
         <v>4</v>
       </c>
       <c r="P100" s="67" t="s">
+        <v>8707</v>
+      </c>
+      <c r="Q100" s="67" t="s">
+        <v>8708</v>
+      </c>
+      <c r="R100" s="67" t="s">
         <v>8709</v>
       </c>
-      <c r="Q100" s="67" t="s">
+      <c r="S100" s="67" t="s">
         <v>8710</v>
       </c>
-      <c r="R100" s="67" t="s">
+      <c r="T100" s="67" t="s">
         <v>8711</v>
       </c>
-      <c r="S100" s="67" t="s">
+      <c r="U100" s="67" t="s">
         <v>8712</v>
       </c>
-      <c r="T100" s="67" t="s">
+      <c r="V100" s="67" t="s">
         <v>8713</v>
-      </c>
-      <c r="U100" s="67" t="s">
-        <v>8714</v>
-      </c>
-      <c r="V100" s="67" t="s">
-        <v>8715</v>
       </c>
       <c r="W100"/>
       <c r="X100"/>
@@ -39613,13 +39957,13 @@
         <v>10</v>
       </c>
       <c r="F101" s="66" t="s">
-        <v>8716</v>
+        <v>8714</v>
       </c>
       <c r="G101" s="67" t="s">
         <v>7530</v>
       </c>
       <c r="H101" s="67" t="s">
-        <v>8708</v>
+        <v>8706</v>
       </c>
       <c r="I101" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39675,13 +40019,13 @@
         <v>0</v>
       </c>
       <c r="F102" s="66" t="s">
-        <v>8717</v>
+        <v>8715</v>
       </c>
       <c r="G102" s="67" t="s">
-        <v>8718</v>
+        <v>8716</v>
       </c>
       <c r="H102" s="67" t="s">
-        <v>8717</v>
+        <v>8715</v>
       </c>
       <c r="I102" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39703,10 +40047,10 @@
         <v>4</v>
       </c>
       <c r="P102" s="67" t="s">
-        <v>8719</v>
+        <v>8717</v>
       </c>
       <c r="Q102" s="67" t="s">
-        <v>8720</v>
+        <v>8718</v>
       </c>
       <c r="R102" s="67" t="s">
         <v>8364</v>
@@ -41155,7 +41499,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>8575</v>
+        <v>8573</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>$A$2</f>
@@ -41191,7 +41535,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>8576</v>
+        <v>8574</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>$A$2</f>
@@ -41662,61 +42006,61 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>8577</v>
+        <v>8575</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>8578</v>
+        <v>8576</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>8579</v>
+        <v>8577</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>8580</v>
+        <v>8578</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>8581</v>
+        <v>8579</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>8582</v>
+        <v>8580</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>8584</v>
+        <v>8582</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="63" t="s">
-        <v>8585</v>
+        <v>8583</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>8586</v>
+        <v>8584</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="63" t="s">
-        <v>8587</v>
+        <v>8585</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>8588</v>
+        <v>8586</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="63" t="s">
-        <v>8589</v>
+        <v>8587</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>8590</v>
+        <v>8588</v>
       </c>
     </row>
   </sheetData>
@@ -41738,7 +42082,7 @@
   <dimension ref="A1:K6104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -41754,16 +42098,6 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J4" s="35" t="s">
-        <v>8565</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J5" s="35" t="s">
-        <v>8564</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J6" s="35" t="s">
         <v>8563</v>
       </c>
     </row>
@@ -41784,7 +42118,7 @@
         <v>7522</v>
       </c>
       <c r="H15" s="62" t="s">
-        <v>8574</v>
+        <v>8572</v>
       </c>
       <c r="I15" s="62" t="s">
         <v>7898</v>
@@ -41801,16 +42135,16 @@
         <v>7521</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>8573</v>
+        <v>8571</v>
       </c>
       <c r="I16" s="35" t="s">
-        <v>8572</v>
+        <v>8570</v>
       </c>
       <c r="J16" s="35" t="s">
-        <v>8571</v>
+        <v>8569</v>
       </c>
       <c r="K16" s="35" t="s">
-        <v>8570</v>
+        <v>8568</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -41818,16 +42152,16 @@
         <v>7520</v>
       </c>
       <c r="H17" s="62" t="s">
-        <v>8569</v>
+        <v>8567</v>
       </c>
       <c r="I17" s="62" t="s">
-        <v>8568</v>
+        <v>8566</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>8567</v>
+        <v>8565</v>
       </c>
       <c r="K17" s="62" t="s">
-        <v>8566</v>
+        <v>8564</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -84875,10 +85209,10 @@
   <dimension ref="A1:N193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="A1:N119"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="A1:N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -90670,7 +91004,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8723</v>
+        <v>8721</v>
       </c>
     </row>
   </sheetData>
@@ -90692,7 +91026,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E3" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added PlasticChest (+) and Industrial Oven (!) and Flow Regulator (!)
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16830" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="18390" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="17" r:id="rId1"/>
@@ -37786,7 +37786,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed Bouncing on edges, molding bricks, upcycling
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18390" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="19950" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="17" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9097" uniqueCount="8722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9100" uniqueCount="8724">
   <si>
     <t>Uuo</t>
   </si>
@@ -26924,6 +26924,12 @@
   </si>
   <si>
     <t>OilField</t>
+  </si>
+  <si>
+    <t>Cr2O3-Al2O3</t>
+  </si>
+  <si>
+    <t>Chromia Alumina</t>
   </si>
 </sst>
 </file>
@@ -27690,11 +27696,11 @@
   </sheetPr>
   <dimension ref="A1:J338"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C152" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C305" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C169" sqref="A1:H337"/>
+      <selection pane="bottomRight" activeCell="B341" sqref="B341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35170,7 +35176,7 @@
         <v>Liquid</v>
       </c>
     </row>
-    <row r="337" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
@@ -35182,8 +35188,24 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D338" s="12"/>
+    <row r="338" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>8723</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>8722</v>
+      </c>
+      <c r="D338" s="12" t="str">
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
+      </c>
+      <c r="G338" s="12" t="s">
+        <v>266</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37785,8 +37807,8 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37903,10 +37925,10 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -37931,10 +37953,10 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>540</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -37959,10 +37981,10 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>720</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -37987,10 +38009,10 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>720</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -38015,10 +38037,10 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>720</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -38043,10 +38065,10 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>240</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -38071,10 +38093,10 @@
         <v>8</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>240</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -38099,10 +38121,10 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>540</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -38127,10 +38149,10 @@
         <v>10</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>540</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -38155,10 +38177,10 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>1200</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -38183,10 +38205,10 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>1200</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -38211,10 +38233,10 @@
         <v>13</v>
       </c>
       <c r="F15">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="G15">
-        <v>900</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -38239,10 +38261,10 @@
         <v>14</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -38267,10 +38289,10 @@
         <v>15</v>
       </c>
       <c r="F17">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>300</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -38295,10 +38317,10 @@
         <v>16</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G18">
-        <v>200</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -41455,7 +41477,7 @@
   </sheetPr>
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
@@ -42082,7 +42104,7 @@
   <dimension ref="A1:K6104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a Condenser, Potash, Tin and Many Bug Fixes
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19950" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="23070" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="17" r:id="rId1"/>
@@ -26,9 +26,6 @@
     <sheet name="Polymer Objects" sheetId="9" r:id="rId12"/>
     <sheet name="Fuel" sheetId="16" r:id="rId13"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId14"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Items (MC)'!$B$2:$I$193</definedName>
   </definedNames>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9100" uniqueCount="8724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9092" uniqueCount="8721">
   <si>
     <t>Uuo</t>
   </si>
@@ -25965,9 +25962,6 @@
     <t>Bale Of Alfalfa</t>
   </si>
   <si>
-    <t>Temp Items</t>
-  </si>
-  <si>
     <t>transportation</t>
   </si>
   <si>
@@ -26449,36 +26443,18 @@
     <t>State</t>
   </si>
   <si>
-    <t>59</t>
-  </si>
-  <si>
     <t>1Y</t>
   </si>
   <si>
     <t>4i</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>1Z</t>
-  </si>
-  <si>
     <t>4m</t>
   </si>
   <si>
     <t>4l</t>
   </si>
   <si>
-    <t>4k</t>
-  </si>
-  <si>
-    <t>4j</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Bag</t>
   </si>
   <si>
@@ -26930,6 +26906,18 @@
   </si>
   <si>
     <t>Chromia Alumina</t>
+  </si>
+  <si>
+    <t>Acrylonitrile</t>
+  </si>
+  <si>
+    <t>C3H3N</t>
+  </si>
+  <si>
+    <t>Acetonitrile</t>
+  </si>
+  <si>
+    <t>CH3CN</t>
   </si>
 </sst>
 </file>
@@ -27313,54 +27301,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TODO"/>
-      <sheetName val="Notes"/>
-      <sheetName val="Enums"/>
-      <sheetName val="Game IDs"/>
-      <sheetName val="Items (MC)"/>
-      <sheetName val="Blocks (MC)"/>
-      <sheetName val="Elements"/>
-      <sheetName val="Minerals"/>
-      <sheetName val="Alloys"/>
-      <sheetName val="Compounds"/>
-      <sheetName val="Polymers"/>
-      <sheetName val="Polymer Objects"/>
-      <sheetName val="Fuel"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>polyvinyl</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94" t="str">
-            <v>1.0.0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -27661,22 +27601,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8522</v>
+        <v>8521</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8523</v>
+        <v>8522</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8524</v>
+        <v>8523</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8525</v>
+        <v>8524</v>
       </c>
     </row>
   </sheetData>
@@ -27694,13 +27634,13 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:J338"/>
+  <dimension ref="A1:J339"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C305" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C218" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B341" sqref="B341"/>
+      <selection pane="bottomRight" activeCell="B228" sqref="A1:H339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29318,10 +29258,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>8504</v>
+        <v>8503</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>8502</v>
+        <v>8501</v>
       </c>
       <c r="D70" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -29333,7 +29273,7 @@
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12" t="s">
-        <v>8505</v>
+        <v>8504</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -31097,10 +31037,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B151" s="17" t="s">
+        <v>8536</v>
+      </c>
+      <c r="C151" s="18" t="s">
         <v>8537</v>
-      </c>
-      <c r="C151" s="18" t="s">
-        <v>8538</v>
       </c>
       <c r="D151" s="18" t="str">
         <f>Enums!$A$3</f>
@@ -31781,10 +31721,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B181" s="1" t="s">
+        <v>8538</v>
+      </c>
+      <c r="C181" s="12" t="s">
         <v>8539</v>
-      </c>
-      <c r="C181" s="12" t="s">
-        <v>8540</v>
       </c>
       <c r="D181" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31801,10 +31741,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>8541</v>
+        <v>8540</v>
       </c>
       <c r="C182" t="s">
-        <v>8548</v>
+        <v>8547</v>
       </c>
       <c r="D182" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31812,7 +31752,7 @@
       </c>
       <c r="E182" s="12"/>
       <c r="F182" s="12" t="s">
-        <v>8555</v>
+        <v>8554</v>
       </c>
       <c r="G182" s="12"/>
       <c r="H182" s="12"/>
@@ -31823,10 +31763,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>8542</v>
+        <v>8541</v>
       </c>
       <c r="C183" t="s">
-        <v>8549</v>
+        <v>8548</v>
       </c>
       <c r="D183" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31834,7 +31774,7 @@
       </c>
       <c r="E183" s="12"/>
       <c r="F183" s="12" t="s">
-        <v>8556</v>
+        <v>8555</v>
       </c>
       <c r="G183" s="12"/>
       <c r="H183" s="12"/>
@@ -31845,10 +31785,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>8547</v>
+        <v>8546</v>
       </c>
       <c r="C184" t="s">
-        <v>8550</v>
+        <v>8549</v>
       </c>
       <c r="D184" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31856,7 +31796,7 @@
       </c>
       <c r="E184" s="12"/>
       <c r="F184" s="12" t="s">
-        <v>8557</v>
+        <v>8556</v>
       </c>
       <c r="G184" s="12"/>
       <c r="H184" s="12"/>
@@ -31867,10 +31807,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>8546</v>
+        <v>8545</v>
       </c>
       <c r="C185" t="s">
-        <v>8551</v>
+        <v>8550</v>
       </c>
       <c r="D185" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31878,7 +31818,7 @@
       </c>
       <c r="E185" s="12"/>
       <c r="F185" s="12" t="s">
-        <v>8558</v>
+        <v>8557</v>
       </c>
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
@@ -31889,10 +31829,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>8545</v>
+        <v>8544</v>
       </c>
       <c r="C186" t="s">
-        <v>8552</v>
+        <v>8551</v>
       </c>
       <c r="D186" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31900,7 +31840,7 @@
       </c>
       <c r="E186" s="12"/>
       <c r="F186" s="12" t="s">
-        <v>8559</v>
+        <v>8558</v>
       </c>
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
@@ -31911,10 +31851,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>8544</v>
+        <v>8543</v>
       </c>
       <c r="C187" t="s">
-        <v>8553</v>
+        <v>8552</v>
       </c>
       <c r="D187" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31922,7 +31862,7 @@
       </c>
       <c r="E187" s="12"/>
       <c r="F187" s="12" t="s">
-        <v>8560</v>
+        <v>8559</v>
       </c>
       <c r="G187" s="12"/>
       <c r="H187" s="12"/>
@@ -31933,10 +31873,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>8543</v>
+        <v>8542</v>
       </c>
       <c r="C188" t="s">
-        <v>8554</v>
+        <v>8553</v>
       </c>
       <c r="D188" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31944,7 +31884,7 @@
       </c>
       <c r="E188" s="12"/>
       <c r="F188" s="12" t="s">
-        <v>8561</v>
+        <v>8560</v>
       </c>
       <c r="G188" s="12"/>
       <c r="H188" s="12"/>
@@ -32878,8 +32818,8 @@
         <v>546</v>
       </c>
       <c r="D231" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E231" s="12"/>
       <c r="F231" s="12" t="s">
@@ -32902,8 +32842,8 @@
         <v>542</v>
       </c>
       <c r="D232" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E232" s="12"/>
       <c r="F232" s="12" t="s">
@@ -32926,8 +32866,8 @@
         <v>538</v>
       </c>
       <c r="D233" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E233" s="12"/>
       <c r="F233" s="12" t="s">
@@ -32950,8 +32890,8 @@
         <v>536</v>
       </c>
       <c r="D234" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E234" s="12"/>
       <c r="F234" s="12" t="s">
@@ -32974,8 +32914,8 @@
         <v>532</v>
       </c>
       <c r="D235" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E235" s="12"/>
       <c r="F235" s="12" t="s">
@@ -32998,8 +32938,8 @@
         <v>528</v>
       </c>
       <c r="D236" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E236" s="12"/>
       <c r="F236" s="12" t="s">
@@ -33022,8 +32962,8 @@
         <v>525</v>
       </c>
       <c r="D237" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E237" s="12"/>
       <c r="F237" s="12" t="s">
@@ -33046,8 +32986,8 @@
         <v>295</v>
       </c>
       <c r="D238" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E238" s="12"/>
       <c r="F238" s="12" t="s">
@@ -33070,8 +33010,8 @@
         <v>520</v>
       </c>
       <c r="D239" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E239" s="12"/>
       <c r="F239" s="12" t="s">
@@ -33094,8 +33034,8 @@
         <v>516</v>
       </c>
       <c r="D240" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E240" s="12"/>
       <c r="F240" s="12" t="s">
@@ -33118,8 +33058,8 @@
         <v>512</v>
       </c>
       <c r="D241" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E241" s="12"/>
       <c r="F241" s="12" t="s">
@@ -33142,8 +33082,8 @@
         <v>509</v>
       </c>
       <c r="D242" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E242" s="12"/>
       <c r="F242" s="12" t="s">
@@ -33166,8 +33106,8 @@
         <v>505</v>
       </c>
       <c r="D243" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E243" s="12"/>
       <c r="F243" s="12" t="s">
@@ -33190,8 +33130,8 @@
         <v>501</v>
       </c>
       <c r="D244" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E244" s="13"/>
       <c r="F244" s="12"/>
@@ -33210,8 +33150,8 @@
         <v>499</v>
       </c>
       <c r="D245" s="12" t="str">
-        <f>Enums!$A$3</f>
-        <v>Liquid</v>
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
       </c>
       <c r="E245" s="12"/>
       <c r="F245" s="12" t="s">
@@ -33273,7 +33213,7 @@
         <v>492</v>
       </c>
       <c r="C248" s="57" t="s">
-        <v>8500</v>
+        <v>8499</v>
       </c>
       <c r="D248" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -33281,11 +33221,11 @@
       </c>
       <c r="E248" s="12"/>
       <c r="F248" s="12" t="s">
-        <v>8503</v>
+        <v>8502</v>
       </c>
       <c r="G248" s="12"/>
       <c r="H248" s="12" t="s">
-        <v>8501</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -33998,7 +33938,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>8534</v>
+        <v>8533</v>
       </c>
       <c r="C279" s="12"/>
       <c r="D279" s="12" t="str">
@@ -34016,7 +33956,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>8535</v>
+        <v>8534</v>
       </c>
       <c r="C280" s="12"/>
       <c r="D280" s="12" t="str">
@@ -34034,7 +33974,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>8536</v>
+        <v>8535</v>
       </c>
       <c r="C281" s="12"/>
       <c r="D281" s="12" t="str">
@@ -34739,11 +34679,11 @@
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B313" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C313" s="14" t="s">
-        <v>295</v>
+      <c r="B313" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C313" s="13" t="s">
+        <v>293</v>
       </c>
       <c r="D313" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34761,22 +34701,23 @@
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B314" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C314" s="13" t="s">
-        <v>293</v>
+      <c r="B314" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C314" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="D314" s="12" t="str">
         <f>Enums!$A$2</f>
         <v>Solid</v>
       </c>
-      <c r="E314" s="12"/>
       <c r="F314" s="12"/>
       <c r="G314" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="H314" s="12"/>
+      <c r="H314" s="12" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="315" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="str">
@@ -34784,10 +34725,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C315" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D315" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34807,10 +34748,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C316" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D316" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34830,50 +34771,49 @@
         <v>1.0.0</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C317" s="14" t="s">
-        <v>287</v>
-      </c>
+        <v>8574</v>
+      </c>
+      <c r="C317" s="14"/>
       <c r="D317" s="12" t="str">
         <f>Enums!$A$2</f>
         <v>Solid</v>
       </c>
       <c r="F317" s="12"/>
-      <c r="G317" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="H317" s="12" t="s">
-        <v>286</v>
-      </c>
+      <c r="G317" s="12"/>
+      <c r="H317" s="12"/>
     </row>
     <row r="318" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B318" s="8" t="s">
-        <v>8581</v>
-      </c>
-      <c r="C318" s="14"/>
+      <c r="B318" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C318" s="14" t="s">
+        <v>284</v>
+      </c>
       <c r="D318" s="12" t="str">
         <f>Enums!$A$2</f>
         <v>Solid</v>
       </c>
-      <c r="F318" s="12"/>
-      <c r="G318" s="12"/>
-      <c r="H318" s="12"/>
+      <c r="G318" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="H318" s="12" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="319" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="str">
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B319" s="1" t="s">
-        <v>285</v>
+      <c r="B319" s="8" t="s">
+        <v>283</v>
       </c>
       <c r="C319" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D319" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34891,11 +34831,11 @@
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B320" s="8" t="s">
-        <v>283</v>
+      <c r="B320" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="C320" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D320" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34914,10 +34854,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C321" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D321" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34936,10 +34876,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C322" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
+      </c>
+      <c r="C322" s="16" t="s">
+        <v>276</v>
       </c>
       <c r="D322" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34958,10 +34898,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C323" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
+      </c>
+      <c r="C323" s="15" t="s">
+        <v>273</v>
       </c>
       <c r="D323" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34970,9 +34910,6 @@
       <c r="G323" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="H323" s="12" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="324" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="str">
@@ -34980,10 +34917,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C324" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="C324" s="14" t="s">
+        <v>271</v>
       </c>
       <c r="D324" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -34999,15 +34936,16 @@
         <v>1.0.0</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C325" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+      <c r="C325" s="13" t="s">
+        <v>269</v>
       </c>
       <c r="D325" s="12" t="str">
         <f>Enums!$A$2</f>
         <v>Solid</v>
       </c>
+      <c r="E325" s="12"/>
       <c r="G325" s="12" t="s">
         <v>266</v>
       </c>
@@ -35017,11 +34955,11 @@
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B326" s="1" t="s">
-        <v>270</v>
+      <c r="B326" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="C326" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D326" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -35037,19 +34975,13 @@
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B327" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C327" s="13" t="s">
-        <v>267</v>
+      <c r="B327" s="53" t="str">
+        <f>Enums!$B$66</f>
+        <v>Fruit Brandy</v>
       </c>
       <c r="D327" s="12" t="str">
-        <f>Enums!$A$2</f>
-        <v>Solid</v>
-      </c>
-      <c r="E327" s="12"/>
-      <c r="G327" s="12" t="s">
-        <v>266</v>
+        <f>Enums!$A$3</f>
+        <v>Liquid</v>
       </c>
     </row>
     <row r="328" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -35058,8 +34990,8 @@
         <v>1.0.0</v>
       </c>
       <c r="B328" s="53" t="str">
-        <f>Enums!$B$66</f>
-        <v>Fruit Brandy</v>
+        <f>Enums!$B$67</f>
+        <v>Vodka</v>
       </c>
       <c r="D328" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35072,8 +35004,8 @@
         <v>1.0.0</v>
       </c>
       <c r="B329" s="53" t="str">
-        <f>Enums!$B$67</f>
-        <v>Vodka</v>
+        <f>Enums!$B$68</f>
+        <v>Gin</v>
       </c>
       <c r="D329" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35086,8 +35018,8 @@
         <v>1.0.0</v>
       </c>
       <c r="B330" s="53" t="str">
-        <f>Enums!$B$68</f>
-        <v>Gin</v>
+        <f>Enums!$B$69</f>
+        <v>Tequila</v>
       </c>
       <c r="D330" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35100,8 +35032,8 @@
         <v>1.0.0</v>
       </c>
       <c r="B331" s="53" t="str">
-        <f>Enums!$B$69</f>
-        <v>Tequila</v>
+        <f>Enums!$B$70</f>
+        <v>Rum</v>
       </c>
       <c r="D331" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35114,8 +35046,8 @@
         <v>1.0.0</v>
       </c>
       <c r="B332" s="53" t="str">
-        <f>Enums!$B$70</f>
-        <v>Rum</v>
+        <f>Enums!$B$71</f>
+        <v>Whiskey</v>
       </c>
       <c r="D332" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35128,8 +35060,8 @@
         <v>1.0.0</v>
       </c>
       <c r="B333" s="53" t="str">
-        <f>Enums!$B$71</f>
-        <v>Whiskey</v>
+        <f>Enums!$B$72</f>
+        <v>Carrot Wine</v>
       </c>
       <c r="D333" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35141,9 +35073,8 @@
         <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
-      <c r="B334" s="53" t="str">
-        <f>Enums!$B$72</f>
-        <v>Carrot Wine</v>
+      <c r="B334" s="1" t="s">
+        <v>8435</v>
       </c>
       <c r="D334" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35156,7 +35087,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>8435</v>
+        <v>8436</v>
       </c>
       <c r="D335" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35169,42 +35100,61 @@
         <v>1.0.0</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>8436</v>
-      </c>
-      <c r="D336" s="12" t="str">
+        <v>8495</v>
+      </c>
+      <c r="D336" s="12" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>8716</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>8715</v>
+      </c>
+      <c r="D337" s="12" t="str">
+        <f>Enums!$A$2</f>
+        <v>Solid</v>
+      </c>
+      <c r="G337" s="12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>8717</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>8718</v>
+      </c>
+      <c r="D338" s="12" t="str">
         <f>Enums!$A$3</f>
         <v>Liquid</v>
       </c>
     </row>
-    <row r="337" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A337" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B337" s="1" t="s">
-        <v>8496</v>
-      </c>
-      <c r="D337" s="12" t="s">
-        <v>1431</v>
-      </c>
-    </row>
-    <row r="338" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A338" s="1" t="str">
-        <f>Enums!$A$94</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B338" s="1" t="s">
-        <v>8723</v>
-      </c>
-      <c r="C338" s="1" t="s">
-        <v>8722</v>
-      </c>
-      <c r="D338" s="12" t="str">
-        <f>Enums!$A$2</f>
-        <v>Solid</v>
-      </c>
-      <c r="G338" s="12" t="s">
-        <v>266</v>
+    <row r="339" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>8719</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>8720</v>
+      </c>
+      <c r="D339" s="12" t="str">
+        <f>Enums!$A$3</f>
+        <v>Liquid</v>
       </c>
     </row>
   </sheetData>
@@ -35226,7 +35176,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B109" sqref="A1:N115"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="A1:N115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35291,7 +35241,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -35316,7 +35266,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B3" s="33" t="s">
@@ -35337,7 +35287,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B4" s="33" t="s">
@@ -35359,7 +35309,7 @@
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B5" s="33" t="s">
@@ -35379,7 +35329,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -35399,7 +35349,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B7" s="33" t="s">
@@ -35419,7 +35369,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B8" s="33" t="s">
@@ -35439,7 +35389,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B9" s="33" t="s">
@@ -35458,7 +35408,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B10" s="33" t="s">
@@ -35479,7 +35429,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B11" s="33" t="s">
@@ -35499,7 +35449,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B12" s="33" t="s">
@@ -35519,7 +35469,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B13" s="33" t="s">
@@ -35541,7 +35491,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B14" s="33" t="s">
@@ -35561,7 +35511,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B15" s="33" t="s">
@@ -35581,7 +35531,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B16" s="33" t="s">
@@ -35605,7 +35555,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B17" s="33" t="s">
@@ -35625,7 +35575,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B18" s="33" t="s">
@@ -35646,7 +35596,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B19" s="33" t="s">
@@ -35666,7 +35616,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B20" s="33" t="s">
@@ -35685,7 +35635,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B21" s="33" t="s">
@@ -35705,7 +35655,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B22" s="33" t="s">
@@ -35729,7 +35679,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B23" s="33" t="s">
@@ -35750,11 +35700,11 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>8526</v>
+        <v>8525</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>1326</v>
@@ -35771,7 +35721,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B25" s="33" t="s">
@@ -35795,7 +35745,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B26" s="33" t="s">
@@ -35816,7 +35766,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B27" s="33" t="s">
@@ -35836,7 +35786,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B28" s="33" t="s">
@@ -35857,7 +35807,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B29" s="33" t="s">
@@ -35878,7 +35828,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -35898,7 +35848,7 @@
     </row>
     <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B31" s="33" t="s">
@@ -35923,7 +35873,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B32" s="33" t="s">
@@ -35944,7 +35894,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B33" s="33" t="s">
@@ -35965,7 +35915,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B34" s="33" t="s">
@@ -35986,7 +35936,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B35" s="33" t="s">
@@ -36006,11 +35956,11 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>8528</v>
+        <v>8527</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>1304</v>
@@ -36027,7 +35977,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B37" s="33" t="s">
@@ -36048,7 +35998,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B38" s="33" t="s">
@@ -36069,7 +36019,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B39" s="33" t="s">
@@ -36089,7 +36039,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B40" s="33" t="s">
@@ -36109,7 +36059,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B41" s="33" t="s">
@@ -36130,7 +36080,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B42" s="33" t="s">
@@ -36150,7 +36100,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B43" s="33" t="s">
@@ -36170,7 +36120,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B44" s="33" t="s">
@@ -36190,7 +36140,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="str">
-        <f>[1]Enums!$A$94</f>
+        <f>Enums!$A$94</f>
         <v>1.0.0</v>
       </c>
       <c r="B45" s="33" t="s">
@@ -37269,7 +37219,7 @@
         <v>0</v>
       </c>
       <c r="H97" s="8" t="str">
-        <f>[1]Enums!$A$47</f>
+        <f>Enums!$A$47</f>
         <v>polyvinyl</v>
       </c>
     </row>
@@ -37350,7 +37300,7 @@
         <v>0</v>
       </c>
       <c r="H101" s="8" t="str">
-        <f>[1]Enums!$A$47</f>
+        <f>Enums!$A$47</f>
         <v>polyvinyl</v>
       </c>
     </row>
@@ -37370,7 +37320,7 @@
         <v>0</v>
       </c>
       <c r="H102" s="8" t="str">
-        <f>[1]Enums!$A$47</f>
+        <f>Enums!$A$47</f>
         <v>polyvinyl</v>
       </c>
     </row>
@@ -37390,7 +37340,7 @@
         <v>0</v>
       </c>
       <c r="H103" s="8" t="str">
-        <f>[1]Enums!$A$47</f>
+        <f>Enums!$A$47</f>
         <v>polyvinyl</v>
       </c>
     </row>
@@ -37628,10 +37578,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>8720</v>
+        <v>8713</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>8719</v>
+        <v>8712</v>
       </c>
       <c r="F115" s="1" t="b">
         <v>0</v>
@@ -37676,7 +37626,7 @@
         <v>Version</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>8521</v>
+        <v>8520</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -37775,7 +37725,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8499</v>
+        <v>8498</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -37784,7 +37734,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8533</v>
+        <v>8532</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -37827,25 +37777,25 @@
         <v>Version</v>
       </c>
       <c r="B1" s="58" t="s">
+        <v>8512</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>8513</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="D1" s="58" t="s">
         <v>8514</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="E1" s="58" t="s">
+        <v>8531</v>
+      </c>
+      <c r="F1" s="60" t="s">
         <v>8515</v>
       </c>
-      <c r="E1" s="58" t="s">
-        <v>8532</v>
-      </c>
-      <c r="F1" s="60" t="s">
+      <c r="G1" s="61" t="s">
         <v>8516</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="H1" s="61" t="s">
         <v>8517</v>
-      </c>
-      <c r="H1" s="61" t="s">
-        <v>8518</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -38335,10 +38285,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN393"/>
+  <dimension ref="A1:AJ393"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A85" sqref="A85"/>
+      <selection pane="topRight" activeCell="D85" sqref="D85"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomRight" activeCell="U102" sqref="U102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39051,7 +39005,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>8527</v>
+        <v>8526</v>
       </c>
       <c r="D78" s="8"/>
     </row>
@@ -39067,7 +39021,7 @@
       </c>
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>5</v>
       </c>
@@ -39076,7 +39030,7 @@
       </c>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>5</v>
       </c>
@@ -39084,7 +39038,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="83" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>5</v>
       </c>
@@ -39092,24 +39046,24 @@
         <v>8299</v>
       </c>
     </row>
-    <row r="84" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>5</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>8530</v>
-      </c>
-    </row>
-    <row r="85" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+        <v>8529</v>
+      </c>
+    </row>
+    <row r="85" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>5</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>8531</v>
+        <v>8530</v>
       </c>
       <c r="E85" s="8"/>
     </row>
-    <row r="86" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -39117,7 +39071,7 @@
         <v>8298</v>
       </c>
     </row>
-    <row r="87" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>5</v>
       </c>
@@ -39126,197 +39080,199 @@
       </c>
       <c r="E87" s="8"/>
     </row>
-    <row r="88" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="12"/>
       <c r="E88" s="8"/>
     </row>
-    <row r="89" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B89" s="12"/>
     </row>
-    <row r="90" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="12"/>
       <c r="E90" s="8"/>
     </row>
-    <row r="91" spans="1:40" ht="15" x14ac:dyDescent="0.25">
-      <c r="B91" s="12"/>
+    <row r="91" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A91" s="64" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B91" s="64" t="s">
+        <v>8582</v>
+      </c>
+      <c r="C91" s="64" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D91" s="64" t="s">
+        <v>1414</v>
+      </c>
       <c r="E91" s="64" t="s">
-        <v>1375</v>
+        <v>8583</v>
       </c>
       <c r="F91" s="64" t="s">
+        <v>8584</v>
+      </c>
+      <c r="G91" s="64" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H91" s="64" t="s">
+        <v>8585</v>
+      </c>
+      <c r="I91" s="64" t="s">
+        <v>1373</v>
+      </c>
+      <c r="J91" s="64" t="s">
+        <v>8586</v>
+      </c>
+      <c r="K91" s="64" t="s">
+        <v>8587</v>
+      </c>
+      <c r="L91" s="64" t="s">
+        <v>1372</v>
+      </c>
+      <c r="M91" s="64" t="s">
+        <v>1371</v>
+      </c>
+      <c r="N91" s="64" t="s">
+        <v>1370</v>
+      </c>
+      <c r="O91" s="64" t="s">
+        <v>1369</v>
+      </c>
+      <c r="P91" s="64" t="s">
+        <v>8588</v>
+      </c>
+      <c r="Q91" s="64" t="s">
         <v>8589</v>
       </c>
-      <c r="G91" s="64" t="s">
-        <v>1377</v>
-      </c>
-      <c r="H91" s="64" t="s">
-        <v>1414</v>
-      </c>
-      <c r="I91" s="64" t="s">
+      <c r="R91" s="64" t="s">
         <v>8590</v>
       </c>
-      <c r="J91" s="64" t="s">
+      <c r="S91" s="64" t="s">
         <v>8591</v>
       </c>
-      <c r="K91" s="64" t="s">
-        <v>1374</v>
-      </c>
-      <c r="L91" s="64" t="s">
+      <c r="T91" s="64" t="s">
         <v>8592</v>
       </c>
-      <c r="M91" s="64" t="s">
-        <v>1373</v>
-      </c>
-      <c r="N91" s="64" t="s">
+      <c r="U91" s="64" t="s">
         <v>8593</v>
       </c>
-      <c r="O91" s="64" t="s">
+      <c r="V91" s="64" t="s">
         <v>8594</v>
       </c>
-      <c r="P91" s="64" t="s">
-        <v>1372</v>
-      </c>
-      <c r="Q91" s="64" t="s">
-        <v>1371</v>
-      </c>
-      <c r="R91" s="64" t="s">
-        <v>1370</v>
-      </c>
-      <c r="S91" s="64" t="s">
-        <v>1369</v>
-      </c>
-      <c r="T91" s="64" t="s">
+      <c r="W91" s="64" t="s">
         <v>8595</v>
       </c>
-      <c r="U91" s="64" t="s">
+      <c r="X91" s="64" t="s">
         <v>8596</v>
       </c>
-      <c r="V91" s="64" t="s">
+      <c r="Y91" s="64" t="s">
         <v>8597</v>
       </c>
-      <c r="W91" s="64" t="s">
+      <c r="Z91" s="64" t="s">
         <v>8598</v>
       </c>
-      <c r="X91" s="64" t="s">
+      <c r="AA91" s="64" t="s">
         <v>8599</v>
       </c>
-      <c r="Y91" s="64" t="s">
+      <c r="AB91" s="64" t="s">
         <v>8600</v>
       </c>
-      <c r="Z91" s="64" t="s">
+      <c r="AC91" s="64" t="s">
         <v>8601</v>
       </c>
-      <c r="AA91" s="64" t="s">
+      <c r="AD91" s="64" t="s">
         <v>8602</v>
       </c>
-      <c r="AB91" s="64" t="s">
+      <c r="AE91" s="64" t="s">
         <v>8603</v>
       </c>
-      <c r="AC91" s="64" t="s">
+      <c r="AF91" s="64" t="s">
         <v>8604</v>
       </c>
-      <c r="AD91" s="64" t="s">
+      <c r="AG91" s="64" t="s">
         <v>8605</v>
       </c>
-      <c r="AE91" s="64" t="s">
+      <c r="AH91" s="64" t="s">
         <v>8606</v>
       </c>
-      <c r="AF91" s="64" t="s">
+      <c r="AI91" s="64" t="s">
         <v>8607</v>
       </c>
-      <c r="AG91" s="64" t="s">
+      <c r="AJ91" s="64" t="s">
         <v>8608</v>
       </c>
-      <c r="AH91" s="64" t="s">
+    </row>
+    <row r="92" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A92" s="65">
+        <v>1</v>
+      </c>
+      <c r="B92" s="66" t="s">
         <v>8609</v>
       </c>
-      <c r="AI91" s="64" t="s">
+      <c r="C92" s="67" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D92" s="67" t="s">
         <v>8610</v>
       </c>
-      <c r="AJ91" s="64" t="s">
+      <c r="E92" s="66" t="str">
+        <f>"Fiber ("&amp;B92&amp;")"</f>
+        <v>Fiber (PolyEthylene Terephthalate )</v>
+      </c>
+      <c r="F92" s="66" t="str">
+        <f t="shared" ref="F92:F102" si="0">"Pellets ("&amp;B92&amp;")"</f>
+        <v>Pellets (PolyEthylene Terephthalate )</v>
+      </c>
+      <c r="G92" s="67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92" t="b">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>4</v>
+      </c>
+      <c r="L92" s="67" t="s">
         <v>8611</v>
       </c>
-      <c r="AK91" s="64" t="s">
+      <c r="M92" s="67" t="s">
         <v>8612</v>
       </c>
-      <c r="AL91" s="64" t="s">
+      <c r="N92" s="67" t="s">
         <v>8613</v>
       </c>
-      <c r="AM91" s="64" t="s">
+      <c r="O92" s="67" t="s">
         <v>8614</v>
       </c>
-      <c r="AN91" s="64" t="s">
+      <c r="P92" s="67" t="s">
         <v>8615</v>
       </c>
-    </row>
-    <row r="92" spans="1:40" ht="39" x14ac:dyDescent="0.25">
-      <c r="B92" s="12"/>
-      <c r="E92" s="65">
-        <v>1</v>
-      </c>
-      <c r="F92" s="66" t="s">
+      <c r="Q92" s="67" t="s">
         <v>8616</v>
       </c>
-      <c r="G92" s="67" t="s">
-        <v>1265</v>
-      </c>
-      <c r="H92" s="67" t="s">
+      <c r="R92" s="67" t="s">
         <v>8617</v>
       </c>
-      <c r="I92" s="66" t="str">
-        <f>"Fiber ("&amp;F92&amp;")"</f>
-        <v>Fiber (PolyEthylene Terephthalate )</v>
-      </c>
-      <c r="J92" s="66" t="str">
-        <f t="shared" ref="J92:J102" si="0">"Pellets ("&amp;F92&amp;")"</f>
-        <v>Pellets (PolyEthylene Terephthalate )</v>
-      </c>
-      <c r="K92" s="67" t="b">
-        <v>0</v>
-      </c>
-      <c r="L92"/>
-      <c r="M92"/>
-      <c r="N92" t="b">
-        <v>1</v>
-      </c>
-      <c r="O92">
-        <v>4</v>
-      </c>
-      <c r="P92" s="67" t="s">
+      <c r="S92" s="67" t="s">
         <v>8618</v>
       </c>
-      <c r="Q92" s="67" t="s">
+      <c r="T92" s="67" t="s">
         <v>8619</v>
       </c>
-      <c r="R92" s="67" t="s">
+      <c r="U92" s="67" t="s">
         <v>8620</v>
       </c>
-      <c r="S92" s="67" t="s">
+      <c r="V92" s="67" t="s">
         <v>8621</v>
       </c>
-      <c r="T92" s="67" t="s">
+      <c r="W92" s="67" t="s">
         <v>8622</v>
       </c>
-      <c r="U92" s="67" t="s">
-        <v>8623</v>
-      </c>
-      <c r="V92" s="67" t="s">
-        <v>8624</v>
-      </c>
-      <c r="W92" s="67" t="s">
-        <v>8625</v>
-      </c>
-      <c r="X92" s="67" t="s">
-        <v>8626</v>
-      </c>
-      <c r="Y92" s="67" t="s">
-        <v>8627</v>
-      </c>
-      <c r="Z92" s="67" t="s">
-        <v>8628</v>
-      </c>
-      <c r="AA92" s="67" t="s">
-        <v>8629</v>
-      </c>
+      <c r="X92"/>
+      <c r="Y92"/>
+      <c r="Z92"/>
+      <c r="AA92"/>
       <c r="AB92"/>
       <c r="AC92"/>
       <c r="AD92"/>
@@ -39326,74 +39282,73 @@
       <c r="AH92"/>
       <c r="AI92"/>
       <c r="AJ92"/>
-      <c r="AK92"/>
-      <c r="AL92"/>
-      <c r="AM92"/>
-      <c r="AN92"/>
-    </row>
-    <row r="93" spans="1:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B93" s="12"/>
-      <c r="E93" s="67">
+    </row>
+    <row r="93" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A93" s="67">
         <v>2</v>
       </c>
-      <c r="F93" s="66" t="s">
-        <v>8630</v>
-      </c>
-      <c r="G93" s="67" t="s">
+      <c r="B93" s="66" t="s">
+        <v>8623</v>
+      </c>
+      <c r="C93" s="67" t="s">
         <v>1339</v>
       </c>
-      <c r="H93" s="67" t="s">
-        <v>8631</v>
-      </c>
-      <c r="I93" s="66" t="str">
-        <f t="shared" ref="I93:I102" si="1">"Fiber ("&amp;F93&amp;")"</f>
+      <c r="D93" s="67" t="s">
+        <v>8624</v>
+      </c>
+      <c r="E93" s="66" t="str">
+        <f t="shared" ref="E93:E102" si="1">"Fiber ("&amp;B93&amp;")"</f>
         <v>Fiber (High-Density PolyEthylene)</v>
       </c>
-      <c r="J93" s="66" t="str">
+      <c r="F93" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (High-Density PolyEthylene)</v>
       </c>
-      <c r="K93" s="67" t="b">
+      <c r="G93" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L93"/>
-      <c r="M93"/>
-      <c r="N93" t="b">
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93" t="b">
         <v>1</v>
       </c>
-      <c r="O93">
+      <c r="K93">
         <v>4</v>
       </c>
+      <c r="L93" s="67" t="s">
+        <v>8625</v>
+      </c>
+      <c r="M93" s="67" t="s">
+        <v>8626</v>
+      </c>
+      <c r="N93" s="67" t="s">
+        <v>8627</v>
+      </c>
+      <c r="O93" s="67" t="s">
+        <v>8628</v>
+      </c>
       <c r="P93" s="67" t="s">
+        <v>8629</v>
+      </c>
+      <c r="Q93" s="67" t="s">
+        <v>8630</v>
+      </c>
+      <c r="R93" s="67" t="s">
+        <v>8631</v>
+      </c>
+      <c r="S93" s="67" t="s">
         <v>8632</v>
       </c>
-      <c r="Q93" s="67" t="s">
+      <c r="T93" s="67" t="s">
         <v>8633</v>
       </c>
-      <c r="R93" s="67" t="s">
+      <c r="U93" s="67" t="s">
         <v>8634</v>
       </c>
-      <c r="S93" s="67" t="s">
-        <v>8635</v>
-      </c>
-      <c r="T93" s="67" t="s">
-        <v>8636</v>
-      </c>
-      <c r="U93" s="67" t="s">
-        <v>8637</v>
-      </c>
-      <c r="V93" s="67" t="s">
-        <v>8638</v>
-      </c>
-      <c r="W93" s="67" t="s">
-        <v>8639</v>
-      </c>
-      <c r="X93" s="67" t="s">
-        <v>8640</v>
-      </c>
-      <c r="Y93" s="67" t="s">
-        <v>8641</v>
-      </c>
+      <c r="V93"/>
+      <c r="W93"/>
+      <c r="X93"/>
+      <c r="Y93"/>
       <c r="Z93"/>
       <c r="AA93"/>
       <c r="AB93"/>
@@ -39405,74 +39360,73 @@
       <c r="AH93"/>
       <c r="AI93"/>
       <c r="AJ93"/>
-      <c r="AK93"/>
-      <c r="AL93"/>
-      <c r="AM93"/>
-      <c r="AN93"/>
-    </row>
-    <row r="94" spans="1:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B94" s="12"/>
-      <c r="E94" s="67">
+    </row>
+    <row r="94" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A94" s="67">
         <v>3</v>
       </c>
-      <c r="F94" s="66" t="s">
+      <c r="B94" s="66" t="s">
         <v>1182</v>
       </c>
-      <c r="G94" s="67" t="s">
+      <c r="C94" s="67" t="s">
         <v>1181</v>
       </c>
-      <c r="H94" s="67" t="s">
-        <v>8631</v>
-      </c>
-      <c r="I94" s="66" t="str">
+      <c r="D94" s="67" t="s">
+        <v>8624</v>
+      </c>
+      <c r="E94" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (PolyVinyl Chloride)</v>
       </c>
-      <c r="J94" s="66" t="str">
+      <c r="F94" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (PolyVinyl Chloride)</v>
       </c>
-      <c r="K94" s="67" t="b">
+      <c r="G94" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L94"/>
-      <c r="M94"/>
-      <c r="N94" t="b">
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94" t="b">
         <v>1</v>
       </c>
-      <c r="O94">
+      <c r="K94">
         <v>4</v>
       </c>
+      <c r="L94" s="67" t="s">
+        <v>8635</v>
+      </c>
+      <c r="M94" s="67" t="s">
+        <v>8636</v>
+      </c>
+      <c r="N94" s="67" t="s">
+        <v>8637</v>
+      </c>
+      <c r="O94" s="67" t="s">
+        <v>8638</v>
+      </c>
       <c r="P94" s="67" t="s">
+        <v>8639</v>
+      </c>
+      <c r="Q94" s="67" t="s">
+        <v>8640</v>
+      </c>
+      <c r="R94" s="67" t="s">
+        <v>8641</v>
+      </c>
+      <c r="S94" s="67" t="s">
         <v>8642</v>
       </c>
-      <c r="Q94" s="67" t="s">
+      <c r="T94" s="67" t="s">
         <v>8643</v>
       </c>
-      <c r="R94" s="67" t="s">
+      <c r="U94" s="67" t="s">
         <v>8644</v>
       </c>
-      <c r="S94" s="67" t="s">
-        <v>8645</v>
-      </c>
-      <c r="T94" s="67" t="s">
-        <v>8646</v>
-      </c>
-      <c r="U94" s="67" t="s">
-        <v>8647</v>
-      </c>
-      <c r="V94" s="67" t="s">
-        <v>8648</v>
-      </c>
-      <c r="W94" s="67" t="s">
-        <v>8649</v>
-      </c>
-      <c r="X94" s="67" t="s">
-        <v>8650</v>
-      </c>
-      <c r="Y94" s="67" t="s">
-        <v>8651</v>
-      </c>
+      <c r="V94"/>
+      <c r="W94"/>
+      <c r="X94"/>
+      <c r="Y94"/>
       <c r="Z94"/>
       <c r="AA94"/>
       <c r="AB94"/>
@@ -39484,62 +39438,61 @@
       <c r="AH94"/>
       <c r="AI94"/>
       <c r="AJ94"/>
-      <c r="AK94"/>
-      <c r="AL94"/>
-      <c r="AM94"/>
-      <c r="AN94"/>
-    </row>
-    <row r="95" spans="1:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B95" s="12"/>
-      <c r="E95" s="67">
+    </row>
+    <row r="95" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A95" s="67">
         <v>4</v>
       </c>
-      <c r="F95" s="66" t="s">
-        <v>8652</v>
-      </c>
-      <c r="G95" s="67" t="s">
+      <c r="B95" s="66" t="s">
+        <v>8645</v>
+      </c>
+      <c r="C95" s="67" t="s">
         <v>1327</v>
       </c>
-      <c r="H95" s="67" t="s">
-        <v>8631</v>
-      </c>
-      <c r="I95" s="66" t="str">
+      <c r="D95" s="67" t="s">
+        <v>8624</v>
+      </c>
+      <c r="E95" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (Low-Density PolyEthylene)</v>
       </c>
-      <c r="J95" s="66" t="str">
+      <c r="F95" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (Low-Density PolyEthylene)</v>
       </c>
-      <c r="K95" s="67" t="b">
+      <c r="G95" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L95"/>
-      <c r="M95"/>
-      <c r="N95" t="b">
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95" t="b">
         <v>1</v>
       </c>
-      <c r="O95">
+      <c r="K95">
         <v>4</v>
       </c>
+      <c r="L95" s="67" t="s">
+        <v>8445</v>
+      </c>
+      <c r="M95" s="67" t="s">
+        <v>8646</v>
+      </c>
+      <c r="N95" s="67" t="s">
+        <v>8647</v>
+      </c>
+      <c r="O95" s="67" t="s">
+        <v>8648</v>
+      </c>
       <c r="P95" s="67" t="s">
-        <v>8445</v>
+        <v>8471</v>
       </c>
       <c r="Q95" s="67" t="s">
-        <v>8653</v>
-      </c>
-      <c r="R95" s="67" t="s">
-        <v>8654</v>
-      </c>
-      <c r="S95" s="67" t="s">
-        <v>8655</v>
-      </c>
-      <c r="T95" s="67" t="s">
-        <v>8471</v>
-      </c>
-      <c r="U95" s="67" t="s">
-        <v>8656</v>
-      </c>
+        <v>8649</v>
+      </c>
+      <c r="R95"/>
+      <c r="S95"/>
+      <c r="T95"/>
+      <c r="U95"/>
       <c r="V95"/>
       <c r="W95"/>
       <c r="X95"/>
@@ -39555,167 +39508,165 @@
       <c r="AH95"/>
       <c r="AI95"/>
       <c r="AJ95"/>
-      <c r="AK95"/>
-      <c r="AL95"/>
-      <c r="AM95"/>
-      <c r="AN95"/>
-    </row>
-    <row r="96" spans="1:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B96" s="12"/>
-      <c r="E96" s="67">
+    </row>
+    <row r="96" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A96" s="67">
         <v>5</v>
       </c>
-      <c r="F96" s="66" t="s">
+      <c r="B96" s="66" t="s">
         <v>1210</v>
       </c>
-      <c r="G96" s="67" t="s">
+      <c r="C96" s="67" t="s">
         <v>1209</v>
       </c>
-      <c r="H96" s="67" t="s">
-        <v>8631</v>
-      </c>
-      <c r="I96" s="66" t="str">
+      <c r="D96" s="67" t="s">
+        <v>8624</v>
+      </c>
+      <c r="E96" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (PolyPropylene)</v>
       </c>
-      <c r="J96" s="66" t="str">
+      <c r="F96" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (PolyPropylene)</v>
       </c>
-      <c r="K96" s="67" t="b">
+      <c r="G96" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L96"/>
-      <c r="M96"/>
-      <c r="N96" t="b">
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96" t="b">
         <v>1</v>
       </c>
-      <c r="O96">
+      <c r="K96">
         <v>4</v>
       </c>
+      <c r="L96" s="67" t="s">
+        <v>8638</v>
+      </c>
+      <c r="M96" s="67" t="s">
+        <v>8445</v>
+      </c>
+      <c r="N96" s="67" t="s">
+        <v>8647</v>
+      </c>
+      <c r="O96" s="67" t="s">
+        <v>8650</v>
+      </c>
       <c r="P96" s="67" t="s">
-        <v>8645</v>
+        <v>8651</v>
       </c>
       <c r="Q96" s="67" t="s">
-        <v>8445</v>
+        <v>8652</v>
       </c>
       <c r="R96" s="67" t="s">
+        <v>8653</v>
+      </c>
+      <c r="S96" s="67" t="s">
         <v>8654</v>
       </c>
-      <c r="S96" s="67" t="s">
+      <c r="T96" s="67" t="s">
+        <v>8655</v>
+      </c>
+      <c r="U96" s="67" t="s">
+        <v>8656</v>
+      </c>
+      <c r="V96" s="67" t="s">
         <v>8657</v>
       </c>
-      <c r="T96" s="67" t="s">
+      <c r="W96" s="67" t="s">
         <v>8658</v>
       </c>
-      <c r="U96" s="67" t="s">
+      <c r="X96" s="67" t="s">
         <v>8659</v>
       </c>
-      <c r="V96" s="67" t="s">
+      <c r="Y96" s="67" t="s">
         <v>8660</v>
       </c>
-      <c r="W96" s="67" t="s">
+      <c r="Z96" s="67" t="s">
         <v>8661</v>
       </c>
-      <c r="X96" s="67" t="s">
+      <c r="AA96" s="67" t="s">
         <v>8662</v>
       </c>
-      <c r="Y96" s="67" t="s">
+      <c r="AB96" s="67" t="s">
         <v>8663</v>
       </c>
-      <c r="Z96" s="67" t="s">
+      <c r="AC96" s="67" t="s">
         <v>8664</v>
       </c>
-      <c r="AA96" s="67" t="s">
+      <c r="AD96" s="67" t="s">
         <v>8665</v>
       </c>
-      <c r="AB96" s="67" t="s">
-        <v>8666</v>
-      </c>
-      <c r="AC96" s="67" t="s">
-        <v>8667</v>
-      </c>
-      <c r="AD96" s="67" t="s">
-        <v>8668</v>
-      </c>
-      <c r="AE96" s="67" t="s">
-        <v>8669</v>
-      </c>
-      <c r="AF96" s="67" t="s">
-        <v>8670</v>
-      </c>
-      <c r="AG96" s="67" t="s">
-        <v>8671</v>
-      </c>
-      <c r="AH96" s="67" t="s">
-        <v>8672</v>
-      </c>
+      <c r="AE96"/>
+      <c r="AF96"/>
+      <c r="AG96"/>
+      <c r="AH96"/>
       <c r="AI96"/>
       <c r="AJ96"/>
-      <c r="AK96"/>
-      <c r="AL96"/>
-      <c r="AM96"/>
-      <c r="AN96"/>
-    </row>
-    <row r="97" spans="2:40" ht="15" x14ac:dyDescent="0.25">
-      <c r="B97" s="12"/>
-      <c r="E97" s="67">
+    </row>
+    <row r="97" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="67">
         <v>6</v>
       </c>
-      <c r="F97" s="66" t="s">
+      <c r="B97" s="66" t="s">
         <v>1204</v>
       </c>
-      <c r="G97" s="67" t="s">
+      <c r="C97" s="67" t="s">
         <v>1203</v>
       </c>
-      <c r="H97" s="67" t="s">
-        <v>8631</v>
-      </c>
-      <c r="I97" s="66" t="str">
+      <c r="D97" s="67" t="s">
+        <v>8624</v>
+      </c>
+      <c r="E97" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (PolyStyrene)</v>
       </c>
-      <c r="J97" s="66" t="str">
+      <c r="F97" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (PolyStyrene)</v>
       </c>
-      <c r="K97" s="67" t="b">
+      <c r="G97" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L97" s="67" t="b">
+      <c r="H97" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="M97"/>
-      <c r="N97" t="b">
+      <c r="I97"/>
+      <c r="J97" t="b">
         <v>1</v>
       </c>
-      <c r="O97">
+      <c r="K97">
         <v>4</v>
       </c>
+      <c r="L97" s="67" t="s">
+        <v>8666</v>
+      </c>
+      <c r="M97" s="67" t="s">
+        <v>8667</v>
+      </c>
+      <c r="N97" s="67" t="s">
+        <v>8457</v>
+      </c>
+      <c r="O97" s="67" t="s">
+        <v>8668</v>
+      </c>
       <c r="P97" s="67" t="s">
-        <v>8673</v>
+        <v>8669</v>
       </c>
       <c r="Q97" s="67" t="s">
-        <v>8674</v>
+        <v>8670</v>
       </c>
       <c r="R97" s="67" t="s">
-        <v>8457</v>
+        <v>8671</v>
       </c>
       <c r="S97" s="67" t="s">
-        <v>8675</v>
-      </c>
-      <c r="T97" s="67" t="s">
-        <v>8676</v>
-      </c>
-      <c r="U97" s="67" t="s">
-        <v>8677</v>
-      </c>
-      <c r="V97" s="67" t="s">
-        <v>8678</v>
-      </c>
-      <c r="W97" s="67" t="s">
-        <v>8679</v>
-      </c>
+        <v>8672</v>
+      </c>
+      <c r="T97"/>
+      <c r="U97"/>
+      <c r="V97"/>
+      <c r="W97"/>
       <c r="X97"/>
       <c r="Y97"/>
       <c r="Z97"/>
@@ -39729,160 +39680,158 @@
       <c r="AH97"/>
       <c r="AI97"/>
       <c r="AJ97"/>
-      <c r="AK97"/>
-      <c r="AL97"/>
-      <c r="AM97"/>
-      <c r="AN97"/>
-    </row>
-    <row r="98" spans="2:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B98" s="12"/>
-      <c r="E98" s="67">
+    </row>
+    <row r="98" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="67">
         <v>7</v>
       </c>
-      <c r="F98" s="66" t="s">
+      <c r="B98" s="66" t="s">
         <v>1291</v>
       </c>
-      <c r="G98" s="67" t="s">
+      <c r="C98" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="H98" s="67" t="s">
-        <v>8680</v>
-      </c>
-      <c r="I98" s="66" t="str">
+      <c r="D98" s="67" t="s">
+        <v>8673</v>
+      </c>
+      <c r="E98" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (PolyCarbonate)</v>
       </c>
-      <c r="J98" s="66" t="str">
+      <c r="F98" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (PolyCarbonate)</v>
       </c>
-      <c r="K98" s="67" t="b">
+      <c r="G98" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L98" s="67" t="b">
+      <c r="H98" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="M98"/>
-      <c r="N98" t="b">
+      <c r="I98"/>
+      <c r="J98" t="b">
         <v>1</v>
       </c>
-      <c r="O98">
+      <c r="K98">
         <v>4</v>
       </c>
-      <c r="P98" s="67" t="s">
+      <c r="L98" s="67" t="s">
+        <v>8674</v>
+      </c>
+      <c r="M98" s="67" t="s">
+        <v>8675</v>
+      </c>
+      <c r="N98" s="67" t="s">
+        <v>8676</v>
+      </c>
+      <c r="O98" s="67" t="s">
+        <v>8677</v>
+      </c>
+      <c r="P98" s="67"/>
+      <c r="Q98" s="67" t="s">
+        <v>8678</v>
+      </c>
+      <c r="R98" s="67" t="s">
+        <v>8679</v>
+      </c>
+      <c r="S98" s="67" t="s">
+        <v>8680</v>
+      </c>
+      <c r="T98" s="67" t="s">
         <v>8681</v>
       </c>
-      <c r="Q98" s="67" t="s">
+      <c r="U98" s="67" t="s">
         <v>8682</v>
       </c>
-      <c r="R98" s="67" t="s">
+      <c r="V98" s="67" t="s">
         <v>8683</v>
       </c>
-      <c r="S98" s="67" t="s">
+      <c r="W98" s="67" t="s">
         <v>8684</v>
       </c>
-      <c r="T98" s="67"/>
-      <c r="U98" s="67" t="s">
+      <c r="X98" s="67" t="s">
         <v>8685</v>
       </c>
-      <c r="V98" s="67" t="s">
+      <c r="Y98" s="67" t="s">
         <v>8686</v>
       </c>
-      <c r="W98" s="67" t="s">
+      <c r="Z98" s="67" t="s">
         <v>8687</v>
       </c>
-      <c r="X98" s="67" t="s">
+      <c r="AA98" s="67" t="s">
         <v>8688</v>
       </c>
-      <c r="Y98" s="67" t="s">
-        <v>8689</v>
-      </c>
-      <c r="Z98" s="67" t="s">
-        <v>8690</v>
-      </c>
-      <c r="AA98" s="67" t="s">
-        <v>8691</v>
-      </c>
-      <c r="AB98" s="67" t="s">
-        <v>8692</v>
-      </c>
-      <c r="AC98" s="67" t="s">
-        <v>8693</v>
-      </c>
-      <c r="AD98" s="67" t="s">
-        <v>8694</v>
-      </c>
-      <c r="AE98" s="67" t="s">
-        <v>8695</v>
-      </c>
+      <c r="AB98"/>
+      <c r="AC98"/>
+      <c r="AD98"/>
+      <c r="AE98"/>
       <c r="AF98"/>
       <c r="AG98"/>
       <c r="AH98"/>
       <c r="AI98"/>
       <c r="AJ98"/>
-      <c r="AK98"/>
-      <c r="AL98"/>
-      <c r="AM98"/>
-      <c r="AN98"/>
-    </row>
-    <row r="99" spans="2:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B99" s="12"/>
-      <c r="E99" s="67">
+    </row>
+    <row r="99" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="67">
         <v>7</v>
       </c>
-      <c r="F99" s="66" t="s">
+      <c r="B99" s="66" t="s">
         <v>1365</v>
       </c>
-      <c r="G99" s="67" t="s">
+      <c r="C99" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="H99" s="67" t="s">
-        <v>8696</v>
-      </c>
-      <c r="I99" s="66" t="str">
+      <c r="D99" s="67" t="s">
+        <v>8689</v>
+      </c>
+      <c r="E99" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (ABS)</v>
       </c>
-      <c r="J99" s="66" t="str">
+      <c r="F99" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (ABS)</v>
       </c>
-      <c r="K99" s="67" t="b">
+      <c r="G99" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L99"/>
-      <c r="M99"/>
-      <c r="N99" t="b">
+      <c r="H99"/>
+      <c r="I99"/>
+      <c r="J99" t="b">
         <v>1</v>
       </c>
-      <c r="O99">
+      <c r="K99">
         <v>4</v>
       </c>
+      <c r="L99" s="67" t="s">
+        <v>8690</v>
+      </c>
+      <c r="M99" s="67" t="s">
+        <v>8691</v>
+      </c>
+      <c r="N99" s="67" t="s">
+        <v>8692</v>
+      </c>
+      <c r="O99" s="67" t="s">
+        <v>8693</v>
+      </c>
       <c r="P99" s="67" t="s">
+        <v>8694</v>
+      </c>
+      <c r="Q99" s="67" t="s">
+        <v>8695</v>
+      </c>
+      <c r="R99" s="67" t="s">
+        <v>8696</v>
+      </c>
+      <c r="S99" s="67"/>
+      <c r="T99" s="67" t="s">
         <v>8697</v>
       </c>
-      <c r="Q99" s="67" t="s">
-        <v>8698</v>
-      </c>
-      <c r="R99" s="67" t="s">
-        <v>8699</v>
-      </c>
-      <c r="S99" s="67" t="s">
-        <v>8700</v>
-      </c>
-      <c r="T99" s="67" t="s">
-        <v>8701</v>
-      </c>
-      <c r="U99" s="67" t="s">
-        <v>8702</v>
-      </c>
-      <c r="V99" s="67" t="s">
-        <v>8703</v>
-      </c>
-      <c r="W99" s="67"/>
-      <c r="X99" s="67" t="s">
-        <v>8704</v>
-      </c>
+      <c r="U99"/>
+      <c r="V99"/>
+      <c r="W99"/>
+      <c r="X99"/>
       <c r="Y99"/>
       <c r="Z99"/>
       <c r="AA99"/>
@@ -39895,65 +39844,64 @@
       <c r="AH99"/>
       <c r="AI99"/>
       <c r="AJ99"/>
-      <c r="AK99"/>
-      <c r="AL99"/>
-      <c r="AM99"/>
-      <c r="AN99"/>
-    </row>
-    <row r="100" spans="2:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B100" s="12"/>
-      <c r="E100" s="67">
+    </row>
+    <row r="100" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A100" s="67">
         <v>0</v>
       </c>
-      <c r="F100" s="66" t="s">
-        <v>8705</v>
-      </c>
-      <c r="G100" s="67" t="s">
+      <c r="B100" s="66" t="s">
+        <v>8698</v>
+      </c>
+      <c r="C100" s="67" t="s">
         <v>7529</v>
       </c>
-      <c r="H100" s="67" t="s">
-        <v>8706</v>
-      </c>
-      <c r="I100" s="66" t="str">
+      <c r="D100" s="67" t="s">
+        <v>8699</v>
+      </c>
+      <c r="E100" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (Specialty Polymers)</v>
       </c>
-      <c r="J100" s="66" t="str">
+      <c r="F100" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (Specialty Polymers)</v>
       </c>
-      <c r="K100" s="67" t="b">
+      <c r="G100" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L100"/>
-      <c r="M100"/>
-      <c r="N100" t="b">
+      <c r="H100"/>
+      <c r="I100"/>
+      <c r="J100" t="b">
         <v>1</v>
       </c>
-      <c r="O100">
+      <c r="K100">
         <v>4</v>
       </c>
+      <c r="L100" s="67" t="s">
+        <v>8700</v>
+      </c>
+      <c r="M100" s="67" t="s">
+        <v>8701</v>
+      </c>
+      <c r="N100" s="67" t="s">
+        <v>8702</v>
+      </c>
+      <c r="O100" s="67" t="s">
+        <v>8703</v>
+      </c>
       <c r="P100" s="67" t="s">
-        <v>8707</v>
+        <v>8704</v>
       </c>
       <c r="Q100" s="67" t="s">
-        <v>8708</v>
+        <v>8705</v>
       </c>
       <c r="R100" s="67" t="s">
-        <v>8709</v>
-      </c>
-      <c r="S100" s="67" t="s">
-        <v>8710</v>
-      </c>
-      <c r="T100" s="67" t="s">
-        <v>8711</v>
-      </c>
-      <c r="U100" s="67" t="s">
-        <v>8712</v>
-      </c>
-      <c r="V100" s="67" t="s">
-        <v>8713</v>
-      </c>
+        <v>8706</v>
+      </c>
+      <c r="S100"/>
+      <c r="T100"/>
+      <c r="U100"/>
+      <c r="V100"/>
       <c r="W100"/>
       <c r="X100"/>
       <c r="Y100"/>
@@ -39968,45 +39916,44 @@
       <c r="AH100"/>
       <c r="AI100"/>
       <c r="AJ100"/>
-      <c r="AK100"/>
-      <c r="AL100"/>
-      <c r="AM100"/>
-      <c r="AN100"/>
-    </row>
-    <row r="101" spans="2:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B101" s="12"/>
-      <c r="E101" s="67">
+    </row>
+    <row r="101" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A101" s="67">
         <v>10</v>
       </c>
-      <c r="F101" s="66" t="s">
-        <v>8714</v>
-      </c>
-      <c r="G101" s="67" t="s">
+      <c r="B101" s="66" t="s">
+        <v>8707</v>
+      </c>
+      <c r="C101" s="67" t="s">
         <v>7530</v>
       </c>
-      <c r="H101" s="67" t="s">
-        <v>8706</v>
-      </c>
-      <c r="I101" s="66" t="str">
+      <c r="D101" s="67" t="s">
+        <v>8699</v>
+      </c>
+      <c r="E101" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (Natural Polymers)</v>
       </c>
-      <c r="J101" s="66" t="str">
+      <c r="F101" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (Natural Polymers)</v>
       </c>
-      <c r="K101" s="67" t="b">
+      <c r="G101" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="L101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101" t="b">
+        <v>1</v>
+      </c>
+      <c r="K101">
+        <v>4</v>
+      </c>
+      <c r="L101" s="67"/>
       <c r="M101"/>
-      <c r="N101" t="b">
-        <v>1</v>
-      </c>
-      <c r="O101">
-        <v>4</v>
-      </c>
-      <c r="P101" s="67"/>
+      <c r="N101"/>
+      <c r="O101"/>
+      <c r="P101"/>
       <c r="Q101"/>
       <c r="R101"/>
       <c r="S101"/>
@@ -40027,59 +39974,55 @@
       <c r="AH101"/>
       <c r="AI101"/>
       <c r="AJ101"/>
-      <c r="AK101"/>
-      <c r="AL101"/>
-      <c r="AM101"/>
-      <c r="AN101"/>
-    </row>
-    <row r="102" spans="2:40" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B102" s="12"/>
-      <c r="D102" s="6" t="s">
-        <v>8494</v>
-      </c>
-      <c r="E102" s="67">
+    </row>
+    <row r="102" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A102" s="67">
         <v>0</v>
       </c>
-      <c r="F102" s="66" t="s">
-        <v>8715</v>
-      </c>
-      <c r="G102" s="67" t="s">
-        <v>8716</v>
-      </c>
-      <c r="H102" s="67" t="s">
-        <v>8715</v>
-      </c>
-      <c r="I102" s="66" t="str">
+      <c r="B102" s="66" t="s">
+        <v>8708</v>
+      </c>
+      <c r="C102" s="67" t="s">
+        <v>8709</v>
+      </c>
+      <c r="D102" s="67" t="s">
+        <v>8708</v>
+      </c>
+      <c r="E102" s="66" t="str">
         <f t="shared" si="1"/>
         <v>Fiber (Rubber)</v>
       </c>
-      <c r="J102" s="66" t="str">
+      <c r="F102" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Pellets (Rubber)</v>
       </c>
-      <c r="K102" s="67" t="b">
+      <c r="G102" s="67" t="b">
         <v>0</v>
       </c>
-      <c r="L102"/>
-      <c r="M102"/>
-      <c r="N102" t="b">
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102" t="b">
         <v>1</v>
       </c>
-      <c r="O102">
+      <c r="K102">
         <v>4</v>
       </c>
-      <c r="P102" s="67" t="s">
-        <v>8717</v>
-      </c>
-      <c r="Q102" s="67" t="s">
-        <v>8718</v>
-      </c>
-      <c r="R102" s="67" t="s">
+      <c r="L102" s="67" t="s">
+        <v>8710</v>
+      </c>
+      <c r="M102" s="67" t="s">
+        <v>8711</v>
+      </c>
+      <c r="N102" s="67" t="s">
         <v>8364</v>
       </c>
-      <c r="S102" s="67" t="s">
+      <c r="O102" s="67" t="s">
         <v>8362</v>
       </c>
+      <c r="P102"/>
+      <c r="Q102"/>
+      <c r="R102"/>
+      <c r="S102"/>
       <c r="T102"/>
       <c r="U102"/>
       <c r="V102"/>
@@ -40097,15 +40040,11 @@
       <c r="AH102"/>
       <c r="AI102"/>
       <c r="AJ102"/>
-      <c r="AK102"/>
-      <c r="AL102"/>
-      <c r="AM102"/>
-      <c r="AN102"/>
-    </row>
-    <row r="103" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B103" s="12"/>
       <c r="D103" s="53" t="s">
-        <v>8498</v>
+        <v>8497</v>
       </c>
       <c r="E103" s="54" t="s">
         <v>8440</v>
@@ -40115,10 +40054,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B104" s="12"/>
       <c r="D104" s="53" t="s">
-        <v>8497</v>
+        <v>8496</v>
       </c>
       <c r="E104" s="53" t="s">
         <v>8442</v>
@@ -40128,23 +40067,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B105" s="12"/>
       <c r="D105" s="56" t="s">
-        <v>8496</v>
+        <v>8495</v>
       </c>
       <c r="E105" s="54" t="s">
-        <v>8495</v>
+        <v>8494</v>
       </c>
       <c r="F105" s="53"/>
       <c r="G105" s="54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" s="12"/>
     </row>
-    <row r="107" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="12"/>
       <c r="D107" s="53" t="s">
         <v>8493</v>
@@ -40157,7 +40096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="12"/>
       <c r="D108" s="53" t="s">
         <v>8492</v>
@@ -40170,7 +40109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="12"/>
       <c r="D109" s="53" t="s">
         <v>8491</v>
@@ -40183,7 +40122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="12"/>
       <c r="D110" s="53" t="s">
         <v>8490</v>
@@ -40196,7 +40135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="12"/>
       <c r="D111" s="53" t="s">
         <v>8489</v>
@@ -40209,7 +40148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:40" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:36" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="12"/>
       <c r="D112" s="53" t="s">
         <v>8488</v>
@@ -41510,7 +41449,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>8508</v>
+        <v>8507</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1429</v>
@@ -41521,7 +41460,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>8573</v>
+        <v>8566</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>$A$2</f>
@@ -41557,7 +41496,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>8574</v>
+        <v>8567</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>$A$2</f>
@@ -41593,7 +41532,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>8529</v>
+        <v>8528</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>$A$2</f>
@@ -41665,7 +41604,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>8509</v>
+        <v>8508</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -41899,7 +41838,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>8510</v>
+        <v>8509</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -41960,22 +41899,22 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>8511</v>
+        <v>8510</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>8506</v>
+        <v>8505</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>8507</v>
+        <v>8506</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>8512</v>
+        <v>8511</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -42028,61 +41967,61 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>8575</v>
+        <v>8568</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>8576</v>
+        <v>8569</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>8577</v>
+        <v>8570</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>8578</v>
+        <v>8571</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>8579</v>
+        <v>8572</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>8580</v>
+        <v>8573</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>8582</v>
+        <v>8575</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="63" t="s">
-        <v>8583</v>
+        <v>8576</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>8584</v>
+        <v>8577</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="63" t="s">
-        <v>8585</v>
+        <v>8578</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>8586</v>
+        <v>8579</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="63" t="s">
-        <v>8587</v>
+        <v>8580</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>8588</v>
+        <v>8581</v>
       </c>
     </row>
   </sheetData>
@@ -42103,8 +42042,8 @@
   </sheetPr>
   <dimension ref="A1:K6104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42119,9 +42058,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J4" s="35" t="s">
-        <v>8563</v>
-      </c>
+      <c r="J4" s="35"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H11" s="35"/>
@@ -42135,55 +42072,31 @@
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>7522</v>
-      </c>
-      <c r="H15" s="62" t="s">
-        <v>8572</v>
-      </c>
-      <c r="I15" s="62" t="s">
-        <v>7898</v>
-      </c>
-      <c r="J15" s="62" t="s">
-        <v>7895</v>
-      </c>
-      <c r="K15" s="62" t="s">
-        <v>7892</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>7521</v>
       </c>
-      <c r="H16" s="35" t="s">
-        <v>8571</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>8570</v>
-      </c>
       <c r="J16" s="35" t="s">
-        <v>8569</v>
+        <v>8565</v>
       </c>
       <c r="K16" s="35" t="s">
-        <v>8568</v>
+        <v>8564</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>7520</v>
       </c>
-      <c r="H17" s="62" t="s">
-        <v>8567</v>
-      </c>
-      <c r="I17" s="62" t="s">
-        <v>8566</v>
-      </c>
       <c r="J17" s="35" t="s">
-        <v>8565</v>
+        <v>8563</v>
       </c>
       <c r="K17" s="62" t="s">
-        <v>8564</v>
+        <v>8562</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -72663,7 +72576,7 @@
         <v>Version</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>8519</v>
+        <v>8518</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -79182,7 +79095,7 @@
         <v>Version</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>8520</v>
+        <v>8519</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -85231,7 +85144,7 @@
   <dimension ref="A1:N193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G26" sqref="A1:N119"/>
@@ -85265,7 +85178,7 @@
         <v>246</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>8562</v>
+        <v>8561</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>245</v>
@@ -90944,10 +90857,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B5" sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -91026,7 +90939,16 @@
         <v>1.0.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8721</v>
+        <v>8714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="str">
+        <f>Enums!$A$94</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pre 1.0.3 Updates - added heated knife
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26190" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="27750" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="17" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9092" uniqueCount="8721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9135" uniqueCount="8756">
   <si>
     <t>Uuo</t>
   </si>
@@ -26040,18 +26040,6 @@
     <t>Polymer Object</t>
   </si>
   <si>
-    <t>Craft 6 slabs when you craft them from plastic blocks</t>
-  </si>
-  <si>
-    <t>Hold shift should allow you to stop jumping on blocks and not conserve momentum</t>
-  </si>
-  <si>
-    <t>Make it so 1 vial of pellets  = 1 block or it takes 4 vials during smelting</t>
-  </si>
-  <si>
-    <t>when a pogo stick is fully damaged, make it disappear</t>
-  </si>
-  <si>
     <t>Medium Density PolyEthylene</t>
   </si>
   <si>
@@ -26918,6 +26906,123 @@
   </si>
   <si>
     <t>Glycerol</t>
+  </si>
+  <si>
+    <t>Deionized Water</t>
+  </si>
+  <si>
+    <t>Tungsten Carbide</t>
+  </si>
+  <si>
+    <t>Industrial Oven</t>
+  </si>
+  <si>
+    <t>Metal Nuggets</t>
+  </si>
+  <si>
+    <t>Pipes and Piping</t>
+  </si>
+  <si>
+    <t>Pumps and Pumping</t>
+  </si>
+  <si>
+    <t>Metal Extruder</t>
+  </si>
+  <si>
+    <t>New Alloys and Uses</t>
+  </si>
+  <si>
+    <t>Feedwater heater</t>
+  </si>
+  <si>
+    <t>Rectifier</t>
+  </si>
+  <si>
+    <t>Boiler</t>
+  </si>
+  <si>
+    <t>Internal Combustion Engine</t>
+  </si>
+  <si>
+    <t>Concept of a Cleanroom</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>Vacuum Pump</t>
+  </si>
+  <si>
+    <t>Addition</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Sputtering Tool</t>
+  </si>
+  <si>
+    <t>Mask Writer</t>
+  </si>
+  <si>
+    <t>Spin Coater</t>
+  </si>
+  <si>
+    <t>Atomic Force Microscope</t>
+  </si>
+  <si>
+    <t>Scanning Electron Microscope</t>
+  </si>
+  <si>
+    <t>Transmission Electron Microscope</t>
+  </si>
+  <si>
+    <t>Focused Ion Beam</t>
+  </si>
+  <si>
+    <t>Contact Printer</t>
+  </si>
+  <si>
+    <t>Acid Hood</t>
+  </si>
+  <si>
+    <t>Base Hood</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Pickup Items bug (NTTB Tag)</t>
+  </si>
+  <si>
+    <t>Code to export TSV files</t>
+  </si>
+  <si>
+    <t>Adding in Kevlar</t>
+  </si>
+  <si>
+    <t>Plastic Block durability and heated knife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiki Maker GameID -&gt; Page </t>
+  </si>
+  <si>
+    <t>Plastic Chests to AutoUpCycle Bitumen and Ore and Ingots into Compressed Blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machining Mill Sucks Wrong </t>
+  </si>
+  <si>
+    <t>Pellets to 128 and bust in IM and extruder</t>
+  </si>
+  <si>
+    <t>Wiki help about yellow side of Inventories</t>
+  </si>
+  <si>
+    <t>Lag delays on Flamethrower and Jetpack on big servers</t>
+  </si>
+  <si>
+    <t>Flip Derrick upside down</t>
   </si>
 </sst>
 </file>
@@ -27147,7 +27252,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -27282,6 +27387,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -27588,39 +27694,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="79.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8520</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8521</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8522</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8523</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
+        <v>8733</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>8744</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>8732</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8719</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8724</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8723</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8726</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8727</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8456</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8728</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8729</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8730</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8731</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8734</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8735</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8736</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8737</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8738</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8739</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8740</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8741</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8742</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8743</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8745</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8746</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8747</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8748</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8749</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8752</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>8753</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8754</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8755</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -27637,10 +28081,10 @@
   <dimension ref="A1:J339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C269" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B149" sqref="B149"/>
+      <selection pane="bottomRight" activeCell="B273" sqref="A1:H339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30883,7 +31327,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>8720</v>
+        <v>8716</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>751</v>
@@ -31037,10 +31481,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B151" s="17" t="s">
-        <v>8535</v>
+        <v>8531</v>
       </c>
       <c r="C151" s="18" t="s">
-        <v>8536</v>
+        <v>8532</v>
       </c>
       <c r="D151" s="18" t="str">
         <f>Enums!$A$3</f>
@@ -31721,10 +32165,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>8537</v>
+        <v>8533</v>
       </c>
       <c r="C181" s="12" t="s">
-        <v>8538</v>
+        <v>8534</v>
       </c>
       <c r="D181" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31741,10 +32185,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>8539</v>
+        <v>8535</v>
       </c>
       <c r="C182" t="s">
-        <v>8546</v>
+        <v>8542</v>
       </c>
       <c r="D182" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31752,7 +32196,7 @@
       </c>
       <c r="E182" s="12"/>
       <c r="F182" s="12" t="s">
-        <v>8553</v>
+        <v>8549</v>
       </c>
       <c r="G182" s="12"/>
       <c r="H182" s="12"/>
@@ -31763,10 +32207,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>8540</v>
+        <v>8536</v>
       </c>
       <c r="C183" t="s">
-        <v>8547</v>
+        <v>8543</v>
       </c>
       <c r="D183" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31774,7 +32218,7 @@
       </c>
       <c r="E183" s="12"/>
       <c r="F183" s="12" t="s">
-        <v>8554</v>
+        <v>8550</v>
       </c>
       <c r="G183" s="12"/>
       <c r="H183" s="12"/>
@@ -31785,10 +32229,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>8545</v>
+        <v>8541</v>
       </c>
       <c r="C184" t="s">
-        <v>8548</v>
+        <v>8544</v>
       </c>
       <c r="D184" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31796,7 +32240,7 @@
       </c>
       <c r="E184" s="12"/>
       <c r="F184" s="12" t="s">
-        <v>8555</v>
+        <v>8551</v>
       </c>
       <c r="G184" s="12"/>
       <c r="H184" s="12"/>
@@ -31807,10 +32251,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>8544</v>
+        <v>8540</v>
       </c>
       <c r="C185" t="s">
-        <v>8549</v>
+        <v>8545</v>
       </c>
       <c r="D185" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31818,7 +32262,7 @@
       </c>
       <c r="E185" s="12"/>
       <c r="F185" s="12" t="s">
-        <v>8556</v>
+        <v>8552</v>
       </c>
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
@@ -31829,10 +32273,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>8543</v>
+        <v>8539</v>
       </c>
       <c r="C186" t="s">
-        <v>8550</v>
+        <v>8546</v>
       </c>
       <c r="D186" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31840,7 +32284,7 @@
       </c>
       <c r="E186" s="12"/>
       <c r="F186" s="12" t="s">
-        <v>8557</v>
+        <v>8553</v>
       </c>
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
@@ -31851,10 +32295,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>8542</v>
+        <v>8538</v>
       </c>
       <c r="C187" t="s">
-        <v>8551</v>
+        <v>8547</v>
       </c>
       <c r="D187" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31862,7 +32306,7 @@
       </c>
       <c r="E187" s="12"/>
       <c r="F187" s="12" t="s">
-        <v>8558</v>
+        <v>8554</v>
       </c>
       <c r="G187" s="12"/>
       <c r="H187" s="12"/>
@@ -31873,10 +32317,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>8541</v>
+        <v>8537</v>
       </c>
       <c r="C188" t="s">
-        <v>8552</v>
+        <v>8548</v>
       </c>
       <c r="D188" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -31884,7 +32328,7 @@
       </c>
       <c r="E188" s="12"/>
       <c r="F188" s="12" t="s">
-        <v>8559</v>
+        <v>8555</v>
       </c>
       <c r="G188" s="12"/>
       <c r="H188" s="12"/>
@@ -33938,7 +34382,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>8532</v>
+        <v>8528</v>
       </c>
       <c r="C279" s="12"/>
       <c r="D279" s="12" t="str">
@@ -33956,7 +34400,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>8533</v>
+        <v>8529</v>
       </c>
       <c r="C280" s="12"/>
       <c r="D280" s="12" t="str">
@@ -33974,7 +34418,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>8534</v>
+        <v>8530</v>
       </c>
       <c r="C281" s="12"/>
       <c r="D281" s="12" t="str">
@@ -34430,7 +34874,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B302" s="17" t="s">
-        <v>328</v>
+        <v>8717</v>
       </c>
       <c r="C302" s="18" t="s">
         <v>327</v>
@@ -34771,7 +35215,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>8573</v>
+        <v>8569</v>
       </c>
       <c r="C317" s="14"/>
       <c r="D317" s="12" t="str">
@@ -35112,10 +35556,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>8715</v>
+        <v>8711</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>8714</v>
+        <v>8710</v>
       </c>
       <c r="D337" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -35131,10 +35575,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>8716</v>
+        <v>8712</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>8717</v>
+        <v>8713</v>
       </c>
       <c r="D338" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35147,10 +35591,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>8718</v>
+        <v>8714</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>8719</v>
+        <v>8715</v>
       </c>
       <c r="D339" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35176,7 +35620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B106" sqref="A1:N115"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35704,7 +36148,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>8524</v>
+        <v>8520</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>1325</v>
@@ -35960,7 +36404,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>8526</v>
+        <v>8522</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>1303</v>
@@ -37578,10 +38022,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>8712</v>
+        <v>8708</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>8711</v>
+        <v>8707</v>
       </c>
       <c r="F115" s="1" t="b">
         <v>0</v>
@@ -37734,7 +38178,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8531</v>
+        <v>8527</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -37758,7 +38202,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37786,7 +38230,7 @@
         <v>8513</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>8530</v>
+        <v>8526</v>
       </c>
       <c r="F1" s="60" t="s">
         <v>8514</v>
@@ -37819,10 +38263,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -37875,10 +38319,10 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -37906,7 +38350,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -37931,10 +38375,10 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -37959,10 +38403,10 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -37987,10 +38431,10 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -38018,7 +38462,7 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -38046,7 +38490,7 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -38071,10 +38515,10 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>60</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -38099,10 +38543,10 @@
         <v>10</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>60</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -38127,10 +38571,10 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G13">
-        <v>60</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -38155,10 +38599,10 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>60</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -38183,10 +38627,10 @@
         <v>13</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -38211,10 +38655,10 @@
         <v>14</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G16">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -38242,7 +38686,7 @@
         <v>3</v>
       </c>
       <c r="G17">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -38270,7 +38714,7 @@
         <v>3</v>
       </c>
       <c r="G18">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -38287,12 +38731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ393"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A85" sqref="A85"/>
-      <selection pane="topRight" activeCell="D85" sqref="D85"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
-      <selection pane="bottomRight" activeCell="U102" sqref="U102"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39005,7 +39445,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>8525</v>
+        <v>8521</v>
       </c>
       <c r="D78" s="8"/>
     </row>
@@ -39051,7 +39491,7 @@
         <v>5</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>8528</v>
+        <v>8524</v>
       </c>
     </row>
     <row r="85" spans="1:36" ht="15" x14ac:dyDescent="0.25">
@@ -39059,7 +39499,7 @@
         <v>5</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>8529</v>
+        <v>8525</v>
       </c>
       <c r="E85" s="8"/>
     </row>
@@ -39096,7 +39536,7 @@
         <v>1374</v>
       </c>
       <c r="B91" s="64" t="s">
-        <v>8581</v>
+        <v>8577</v>
       </c>
       <c r="C91" s="64" t="s">
         <v>1376</v>
@@ -39105,25 +39545,25 @@
         <v>1413</v>
       </c>
       <c r="E91" s="64" t="s">
-        <v>8582</v>
+        <v>8578</v>
       </c>
       <c r="F91" s="64" t="s">
-        <v>8583</v>
+        <v>8579</v>
       </c>
       <c r="G91" s="64" t="s">
         <v>1373</v>
       </c>
       <c r="H91" s="64" t="s">
-        <v>8584</v>
+        <v>8580</v>
       </c>
       <c r="I91" s="64" t="s">
         <v>1372</v>
       </c>
       <c r="J91" s="64" t="s">
-        <v>8585</v>
+        <v>8581</v>
       </c>
       <c r="K91" s="64" t="s">
-        <v>8586</v>
+        <v>8582</v>
       </c>
       <c r="L91" s="64" t="s">
         <v>1371</v>
@@ -39138,67 +39578,67 @@
         <v>1368</v>
       </c>
       <c r="P91" s="64" t="s">
+        <v>8583</v>
+      </c>
+      <c r="Q91" s="64" t="s">
+        <v>8584</v>
+      </c>
+      <c r="R91" s="64" t="s">
+        <v>8585</v>
+      </c>
+      <c r="S91" s="64" t="s">
+        <v>8586</v>
+      </c>
+      <c r="T91" s="64" t="s">
         <v>8587</v>
       </c>
-      <c r="Q91" s="64" t="s">
+      <c r="U91" s="64" t="s">
         <v>8588</v>
       </c>
-      <c r="R91" s="64" t="s">
+      <c r="V91" s="64" t="s">
         <v>8589</v>
       </c>
-      <c r="S91" s="64" t="s">
+      <c r="W91" s="64" t="s">
         <v>8590</v>
       </c>
-      <c r="T91" s="64" t="s">
+      <c r="X91" s="64" t="s">
         <v>8591</v>
       </c>
-      <c r="U91" s="64" t="s">
+      <c r="Y91" s="64" t="s">
         <v>8592</v>
       </c>
-      <c r="V91" s="64" t="s">
+      <c r="Z91" s="64" t="s">
         <v>8593</v>
       </c>
-      <c r="W91" s="64" t="s">
+      <c r="AA91" s="64" t="s">
         <v>8594</v>
       </c>
-      <c r="X91" s="64" t="s">
+      <c r="AB91" s="64" t="s">
         <v>8595</v>
       </c>
-      <c r="Y91" s="64" t="s">
+      <c r="AC91" s="64" t="s">
         <v>8596</v>
       </c>
-      <c r="Z91" s="64" t="s">
+      <c r="AD91" s="64" t="s">
         <v>8597</v>
       </c>
-      <c r="AA91" s="64" t="s">
+      <c r="AE91" s="64" t="s">
         <v>8598</v>
       </c>
-      <c r="AB91" s="64" t="s">
+      <c r="AF91" s="64" t="s">
         <v>8599</v>
       </c>
-      <c r="AC91" s="64" t="s">
+      <c r="AG91" s="64" t="s">
         <v>8600</v>
       </c>
-      <c r="AD91" s="64" t="s">
+      <c r="AH91" s="64" t="s">
         <v>8601</v>
       </c>
-      <c r="AE91" s="64" t="s">
+      <c r="AI91" s="64" t="s">
         <v>8602</v>
       </c>
-      <c r="AF91" s="64" t="s">
+      <c r="AJ91" s="64" t="s">
         <v>8603</v>
-      </c>
-      <c r="AG91" s="64" t="s">
-        <v>8604</v>
-      </c>
-      <c r="AH91" s="64" t="s">
-        <v>8605</v>
-      </c>
-      <c r="AI91" s="64" t="s">
-        <v>8606</v>
-      </c>
-      <c r="AJ91" s="64" t="s">
-        <v>8607</v>
       </c>
     </row>
     <row r="92" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
@@ -39206,13 +39646,13 @@
         <v>1</v>
       </c>
       <c r="B92" s="66" t="s">
-        <v>8608</v>
+        <v>8604</v>
       </c>
       <c r="C92" s="67" t="s">
         <v>1264</v>
       </c>
       <c r="D92" s="67" t="s">
-        <v>8609</v>
+        <v>8605</v>
       </c>
       <c r="E92" s="66" t="str">
         <f>"Fiber ("&amp;B92&amp;")"</f>
@@ -39234,40 +39674,40 @@
         <v>4</v>
       </c>
       <c r="L92" s="67" t="s">
+        <v>8606</v>
+      </c>
+      <c r="M92" s="67" t="s">
+        <v>8607</v>
+      </c>
+      <c r="N92" s="67" t="s">
+        <v>8608</v>
+      </c>
+      <c r="O92" s="67" t="s">
+        <v>8609</v>
+      </c>
+      <c r="P92" s="67" t="s">
         <v>8610</v>
       </c>
-      <c r="M92" s="67" t="s">
+      <c r="Q92" s="67" t="s">
         <v>8611</v>
       </c>
-      <c r="N92" s="67" t="s">
+      <c r="R92" s="67" t="s">
         <v>8612</v>
       </c>
-      <c r="O92" s="67" t="s">
+      <c r="S92" s="67" t="s">
         <v>8613</v>
       </c>
-      <c r="P92" s="67" t="s">
+      <c r="T92" s="67" t="s">
         <v>8614</v>
       </c>
-      <c r="Q92" s="67" t="s">
+      <c r="U92" s="67" t="s">
         <v>8615</v>
       </c>
-      <c r="R92" s="67" t="s">
+      <c r="V92" s="67" t="s">
         <v>8616</v>
       </c>
-      <c r="S92" s="67" t="s">
+      <c r="W92" s="67" t="s">
         <v>8617</v>
-      </c>
-      <c r="T92" s="67" t="s">
-        <v>8618</v>
-      </c>
-      <c r="U92" s="67" t="s">
-        <v>8619</v>
-      </c>
-      <c r="V92" s="67" t="s">
-        <v>8620</v>
-      </c>
-      <c r="W92" s="67" t="s">
-        <v>8621</v>
       </c>
       <c r="X92"/>
       <c r="Y92"/>
@@ -39288,13 +39728,13 @@
         <v>2</v>
       </c>
       <c r="B93" s="66" t="s">
-        <v>8622</v>
+        <v>8618</v>
       </c>
       <c r="C93" s="67" t="s">
         <v>1338</v>
       </c>
       <c r="D93" s="67" t="s">
-        <v>8623</v>
+        <v>8619</v>
       </c>
       <c r="E93" s="66" t="str">
         <f t="shared" ref="E93:E102" si="1">"Fiber ("&amp;B93&amp;")"</f>
@@ -39316,34 +39756,34 @@
         <v>4</v>
       </c>
       <c r="L93" s="67" t="s">
+        <v>8620</v>
+      </c>
+      <c r="M93" s="67" t="s">
+        <v>8621</v>
+      </c>
+      <c r="N93" s="67" t="s">
+        <v>8622</v>
+      </c>
+      <c r="O93" s="67" t="s">
+        <v>8623</v>
+      </c>
+      <c r="P93" s="67" t="s">
         <v>8624</v>
       </c>
-      <c r="M93" s="67" t="s">
+      <c r="Q93" s="67" t="s">
         <v>8625</v>
       </c>
-      <c r="N93" s="67" t="s">
+      <c r="R93" s="67" t="s">
         <v>8626</v>
       </c>
-      <c r="O93" s="67" t="s">
+      <c r="S93" s="67" t="s">
         <v>8627</v>
       </c>
-      <c r="P93" s="67" t="s">
+      <c r="T93" s="67" t="s">
         <v>8628</v>
       </c>
-      <c r="Q93" s="67" t="s">
+      <c r="U93" s="67" t="s">
         <v>8629</v>
-      </c>
-      <c r="R93" s="67" t="s">
-        <v>8630</v>
-      </c>
-      <c r="S93" s="67" t="s">
-        <v>8631</v>
-      </c>
-      <c r="T93" s="67" t="s">
-        <v>8632</v>
-      </c>
-      <c r="U93" s="67" t="s">
-        <v>8633</v>
       </c>
       <c r="V93"/>
       <c r="W93"/>
@@ -39372,7 +39812,7 @@
         <v>1180</v>
       </c>
       <c r="D94" s="67" t="s">
-        <v>8623</v>
+        <v>8619</v>
       </c>
       <c r="E94" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39394,34 +39834,34 @@
         <v>4</v>
       </c>
       <c r="L94" s="67" t="s">
+        <v>8630</v>
+      </c>
+      <c r="M94" s="67" t="s">
+        <v>8631</v>
+      </c>
+      <c r="N94" s="67" t="s">
+        <v>8632</v>
+      </c>
+      <c r="O94" s="67" t="s">
+        <v>8633</v>
+      </c>
+      <c r="P94" s="67" t="s">
         <v>8634</v>
       </c>
-      <c r="M94" s="67" t="s">
+      <c r="Q94" s="67" t="s">
         <v>8635</v>
       </c>
-      <c r="N94" s="67" t="s">
+      <c r="R94" s="67" t="s">
         <v>8636</v>
       </c>
-      <c r="O94" s="67" t="s">
+      <c r="S94" s="67" t="s">
         <v>8637</v>
       </c>
-      <c r="P94" s="67" t="s">
+      <c r="T94" s="67" t="s">
         <v>8638</v>
       </c>
-      <c r="Q94" s="67" t="s">
+      <c r="U94" s="67" t="s">
         <v>8639</v>
-      </c>
-      <c r="R94" s="67" t="s">
-        <v>8640</v>
-      </c>
-      <c r="S94" s="67" t="s">
-        <v>8641</v>
-      </c>
-      <c r="T94" s="67" t="s">
-        <v>8642</v>
-      </c>
-      <c r="U94" s="67" t="s">
-        <v>8643</v>
       </c>
       <c r="V94"/>
       <c r="W94"/>
@@ -39444,13 +39884,13 @@
         <v>4</v>
       </c>
       <c r="B95" s="66" t="s">
-        <v>8644</v>
+        <v>8640</v>
       </c>
       <c r="C95" s="67" t="s">
         <v>1326</v>
       </c>
       <c r="D95" s="67" t="s">
-        <v>8623</v>
+        <v>8619</v>
       </c>
       <c r="E95" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39475,19 +39915,19 @@
         <v>8444</v>
       </c>
       <c r="M95" s="67" t="s">
-        <v>8645</v>
+        <v>8641</v>
       </c>
       <c r="N95" s="67" t="s">
-        <v>8646</v>
+        <v>8642</v>
       </c>
       <c r="O95" s="67" t="s">
-        <v>8647</v>
+        <v>8643</v>
       </c>
       <c r="P95" s="67" t="s">
         <v>8470</v>
       </c>
       <c r="Q95" s="67" t="s">
-        <v>8648</v>
+        <v>8644</v>
       </c>
       <c r="R95"/>
       <c r="S95"/>
@@ -39520,7 +39960,7 @@
         <v>1208</v>
       </c>
       <c r="D96" s="67" t="s">
-        <v>8623</v>
+        <v>8619</v>
       </c>
       <c r="E96" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39542,61 +39982,61 @@
         <v>4</v>
       </c>
       <c r="L96" s="67" t="s">
-        <v>8637</v>
+        <v>8633</v>
       </c>
       <c r="M96" s="67" t="s">
         <v>8444</v>
       </c>
       <c r="N96" s="67" t="s">
+        <v>8642</v>
+      </c>
+      <c r="O96" s="67" t="s">
+        <v>8645</v>
+      </c>
+      <c r="P96" s="67" t="s">
         <v>8646</v>
       </c>
-      <c r="O96" s="67" t="s">
+      <c r="Q96" s="67" t="s">
+        <v>8647</v>
+      </c>
+      <c r="R96" s="67" t="s">
+        <v>8648</v>
+      </c>
+      <c r="S96" s="67" t="s">
         <v>8649</v>
       </c>
-      <c r="P96" s="67" t="s">
+      <c r="T96" s="67" t="s">
         <v>8650</v>
       </c>
-      <c r="Q96" s="67" t="s">
+      <c r="U96" s="67" t="s">
         <v>8651</v>
       </c>
-      <c r="R96" s="67" t="s">
+      <c r="V96" s="67" t="s">
         <v>8652</v>
       </c>
-      <c r="S96" s="67" t="s">
+      <c r="W96" s="67" t="s">
         <v>8653</v>
       </c>
-      <c r="T96" s="67" t="s">
+      <c r="X96" s="67" t="s">
         <v>8654</v>
       </c>
-      <c r="U96" s="67" t="s">
+      <c r="Y96" s="67" t="s">
         <v>8655</v>
       </c>
-      <c r="V96" s="67" t="s">
+      <c r="Z96" s="67" t="s">
         <v>8656</v>
       </c>
-      <c r="W96" s="67" t="s">
+      <c r="AA96" s="67" t="s">
         <v>8657</v>
       </c>
-      <c r="X96" s="67" t="s">
+      <c r="AB96" s="67" t="s">
         <v>8658</v>
       </c>
-      <c r="Y96" s="67" t="s">
+      <c r="AC96" s="67" t="s">
         <v>8659</v>
       </c>
-      <c r="Z96" s="67" t="s">
+      <c r="AD96" s="67" t="s">
         <v>8660</v>
-      </c>
-      <c r="AA96" s="67" t="s">
-        <v>8661</v>
-      </c>
-      <c r="AB96" s="67" t="s">
-        <v>8662</v>
-      </c>
-      <c r="AC96" s="67" t="s">
-        <v>8663</v>
-      </c>
-      <c r="AD96" s="67" t="s">
-        <v>8664</v>
       </c>
       <c r="AE96"/>
       <c r="AF96"/>
@@ -39616,7 +40056,7 @@
         <v>1202</v>
       </c>
       <c r="D97" s="67" t="s">
-        <v>8623</v>
+        <v>8619</v>
       </c>
       <c r="E97" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39640,28 +40080,28 @@
         <v>4</v>
       </c>
       <c r="L97" s="67" t="s">
-        <v>8665</v>
+        <v>8661</v>
       </c>
       <c r="M97" s="67" t="s">
-        <v>8666</v>
+        <v>8662</v>
       </c>
       <c r="N97" s="67" t="s">
         <v>8456</v>
       </c>
       <c r="O97" s="67" t="s">
+        <v>8663</v>
+      </c>
+      <c r="P97" s="67" t="s">
+        <v>8664</v>
+      </c>
+      <c r="Q97" s="67" t="s">
+        <v>8665</v>
+      </c>
+      <c r="R97" s="67" t="s">
+        <v>8666</v>
+      </c>
+      <c r="S97" s="67" t="s">
         <v>8667</v>
-      </c>
-      <c r="P97" s="67" t="s">
-        <v>8668</v>
-      </c>
-      <c r="Q97" s="67" t="s">
-        <v>8669</v>
-      </c>
-      <c r="R97" s="67" t="s">
-        <v>8670</v>
-      </c>
-      <c r="S97" s="67" t="s">
-        <v>8671</v>
       </c>
       <c r="T97"/>
       <c r="U97"/>
@@ -39692,7 +40132,7 @@
         <v>220</v>
       </c>
       <c r="D98" s="67" t="s">
-        <v>8672</v>
+        <v>8668</v>
       </c>
       <c r="E98" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39716,50 +40156,50 @@
         <v>4</v>
       </c>
       <c r="L98" s="67" t="s">
-        <v>8673</v>
+        <v>8669</v>
       </c>
       <c r="M98" s="67" t="s">
-        <v>8674</v>
+        <v>8670</v>
       </c>
       <c r="N98" s="67" t="s">
-        <v>8675</v>
+        <v>8671</v>
       </c>
       <c r="O98" s="67" t="s">
-        <v>8676</v>
+        <v>8672</v>
       </c>
       <c r="P98" s="67"/>
       <c r="Q98" s="67" t="s">
+        <v>8673</v>
+      </c>
+      <c r="R98" s="67" t="s">
+        <v>8674</v>
+      </c>
+      <c r="S98" s="67" t="s">
+        <v>8675</v>
+      </c>
+      <c r="T98" s="67" t="s">
+        <v>8676</v>
+      </c>
+      <c r="U98" s="67" t="s">
         <v>8677</v>
       </c>
-      <c r="R98" s="67" t="s">
+      <c r="V98" s="67" t="s">
         <v>8678</v>
       </c>
-      <c r="S98" s="67" t="s">
+      <c r="W98" s="67" t="s">
         <v>8679</v>
       </c>
-      <c r="T98" s="67" t="s">
+      <c r="X98" s="67" t="s">
         <v>8680</v>
       </c>
-      <c r="U98" s="67" t="s">
+      <c r="Y98" s="67" t="s">
         <v>8681</v>
       </c>
-      <c r="V98" s="67" t="s">
+      <c r="Z98" s="67" t="s">
         <v>8682</v>
       </c>
-      <c r="W98" s="67" t="s">
+      <c r="AA98" s="67" t="s">
         <v>8683</v>
-      </c>
-      <c r="X98" s="67" t="s">
-        <v>8684</v>
-      </c>
-      <c r="Y98" s="67" t="s">
-        <v>8685</v>
-      </c>
-      <c r="Z98" s="67" t="s">
-        <v>8686</v>
-      </c>
-      <c r="AA98" s="67" t="s">
-        <v>8687</v>
       </c>
       <c r="AB98"/>
       <c r="AC98"/>
@@ -39782,7 +40222,7 @@
         <v>220</v>
       </c>
       <c r="D99" s="67" t="s">
-        <v>8688</v>
+        <v>8684</v>
       </c>
       <c r="E99" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39804,29 +40244,29 @@
         <v>4</v>
       </c>
       <c r="L99" s="67" t="s">
+        <v>8685</v>
+      </c>
+      <c r="M99" s="67" t="s">
+        <v>8686</v>
+      </c>
+      <c r="N99" s="67" t="s">
+        <v>8687</v>
+      </c>
+      <c r="O99" s="67" t="s">
+        <v>8688</v>
+      </c>
+      <c r="P99" s="67" t="s">
         <v>8689</v>
       </c>
-      <c r="M99" s="67" t="s">
+      <c r="Q99" s="67" t="s">
         <v>8690</v>
       </c>
-      <c r="N99" s="67" t="s">
+      <c r="R99" s="67" t="s">
         <v>8691</v>
-      </c>
-      <c r="O99" s="67" t="s">
-        <v>8692</v>
-      </c>
-      <c r="P99" s="67" t="s">
-        <v>8693</v>
-      </c>
-      <c r="Q99" s="67" t="s">
-        <v>8694</v>
-      </c>
-      <c r="R99" s="67" t="s">
-        <v>8695</v>
       </c>
       <c r="S99" s="67"/>
       <c r="T99" s="67" t="s">
-        <v>8696</v>
+        <v>8692</v>
       </c>
       <c r="U99"/>
       <c r="V99"/>
@@ -39850,13 +40290,13 @@
         <v>0</v>
       </c>
       <c r="B100" s="66" t="s">
-        <v>8697</v>
+        <v>8693</v>
       </c>
       <c r="C100" s="67" t="s">
         <v>7528</v>
       </c>
       <c r="D100" s="67" t="s">
-        <v>8698</v>
+        <v>8694</v>
       </c>
       <c r="E100" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39878,25 +40318,25 @@
         <v>4</v>
       </c>
       <c r="L100" s="67" t="s">
+        <v>8695</v>
+      </c>
+      <c r="M100" s="67" t="s">
+        <v>8696</v>
+      </c>
+      <c r="N100" s="67" t="s">
+        <v>8697</v>
+      </c>
+      <c r="O100" s="67" t="s">
+        <v>8698</v>
+      </c>
+      <c r="P100" s="67" t="s">
         <v>8699</v>
       </c>
-      <c r="M100" s="67" t="s">
+      <c r="Q100" s="67" t="s">
         <v>8700</v>
       </c>
-      <c r="N100" s="67" t="s">
+      <c r="R100" s="67" t="s">
         <v>8701</v>
-      </c>
-      <c r="O100" s="67" t="s">
-        <v>8702</v>
-      </c>
-      <c r="P100" s="67" t="s">
-        <v>8703</v>
-      </c>
-      <c r="Q100" s="67" t="s">
-        <v>8704</v>
-      </c>
-      <c r="R100" s="67" t="s">
-        <v>8705</v>
       </c>
       <c r="S100"/>
       <c r="T100"/>
@@ -39922,13 +40362,13 @@
         <v>10</v>
       </c>
       <c r="B101" s="66" t="s">
-        <v>8706</v>
+        <v>8702</v>
       </c>
       <c r="C101" s="67" t="s">
         <v>7529</v>
       </c>
       <c r="D101" s="67" t="s">
-        <v>8698</v>
+        <v>8694</v>
       </c>
       <c r="E101" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39980,13 +40420,13 @@
         <v>0</v>
       </c>
       <c r="B102" s="66" t="s">
-        <v>8707</v>
+        <v>8703</v>
       </c>
       <c r="C102" s="67" t="s">
-        <v>8708</v>
+        <v>8704</v>
       </c>
       <c r="D102" s="67" t="s">
-        <v>8707</v>
+        <v>8703</v>
       </c>
       <c r="E102" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40008,10 +40448,10 @@
         <v>4</v>
       </c>
       <c r="L102" s="67" t="s">
-        <v>8709</v>
+        <v>8705</v>
       </c>
       <c r="M102" s="67" t="s">
-        <v>8710</v>
+        <v>8706</v>
       </c>
       <c r="N102" s="67" t="s">
         <v>8363</v>
@@ -41460,7 +41900,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>8565</v>
+        <v>8561</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>$A$2</f>
@@ -41496,7 +41936,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>8566</v>
+        <v>8562</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>$A$2</f>
@@ -41532,7 +41972,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>8527</v>
+        <v>8523</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>$A$2</f>
@@ -41967,61 +42407,61 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>8567</v>
+        <v>8563</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>8568</v>
+        <v>8564</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>8569</v>
+        <v>8565</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>8570</v>
+        <v>8566</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>8571</v>
+        <v>8567</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>8572</v>
+        <v>8568</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>8574</v>
+        <v>8570</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="63" t="s">
-        <v>8575</v>
+        <v>8571</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>8576</v>
+        <v>8572</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="63" t="s">
-        <v>8577</v>
+        <v>8573</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>8578</v>
+        <v>8574</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="63" t="s">
-        <v>8579</v>
+        <v>8575</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>8580</v>
+        <v>8576</v>
       </c>
     </row>
   </sheetData>
@@ -42082,10 +42522,10 @@
         <v>7520</v>
       </c>
       <c r="J16" s="35" t="s">
-        <v>8564</v>
+        <v>8560</v>
       </c>
       <c r="K16" s="35" t="s">
-        <v>8563</v>
+        <v>8559</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -42093,10 +42533,10 @@
         <v>7519</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>8562</v>
+        <v>8558</v>
       </c>
       <c r="K17" s="62" t="s">
-        <v>8561</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -72561,7 +73001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -85144,10 +85584,10 @@
   <dimension ref="A1:N193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -85178,7 +85618,7 @@
         <v>246</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>8560</v>
+        <v>8556</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>245</v>
@@ -90939,7 +91379,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8713</v>
+        <v>8709</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -90967,10 +91407,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="A1:G5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -91087,6 +91527,14 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8575</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8718</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="decimal" sqref="C2:E3">

</xml_diff>

<commit_message>
Tweaks to Polycraft 1.0.4 to fix lang file and update fuels
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\GitHub\polycraft1.0.0-1.7.2-10.12.2.1121\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\GitHub\polycraft-1.7.10\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27750" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" activeTab="3"/>
+    <workbookView xWindow="29310" yWindow="0" windowWidth="19560" windowHeight="9120" tabRatio="729" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="17" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9127" uniqueCount="8748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="8749">
   <si>
     <t>Uuo</t>
   </si>
@@ -26407,12 +26407,6 @@
     <t>4i</t>
   </si>
   <si>
-    <t>4m</t>
-  </si>
-  <si>
-    <t>4l</t>
-  </si>
-  <si>
     <t>Bag</t>
   </si>
   <si>
@@ -26999,6 +26993,15 @@
   </si>
   <si>
     <t>Heated Knife Handle</t>
+  </si>
+  <si>
+    <t>1.0.4</t>
+  </si>
+  <si>
+    <t>Sweet Kerosene</t>
+  </si>
+  <si>
+    <t>Sweet Diesel</t>
   </si>
 </sst>
 </file>
@@ -27685,13 +27688,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
-        <v>8721</v>
+        <v>8719</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>8732</v>
+        <v>8730</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>8720</v>
+        <v>8718</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -27699,7 +27702,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8706</v>
+        <v>8704</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -27710,7 +27713,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8707</v>
+        <v>8705</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -27718,7 +27721,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8712</v>
+        <v>8710</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -27726,7 +27729,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>8708</v>
+        <v>8706</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -27737,7 +27740,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8709</v>
+        <v>8707</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -27745,7 +27748,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8710</v>
+        <v>8708</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -27769,7 +27772,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>8711</v>
+        <v>8709</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -27801,7 +27804,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>8713</v>
+        <v>8711</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -27817,7 +27820,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>8714</v>
+        <v>8712</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -27825,7 +27828,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>8715</v>
+        <v>8713</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -27841,7 +27844,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>8716</v>
+        <v>8714</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -27849,7 +27852,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>8717</v>
+        <v>8715</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -27857,7 +27860,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>8718</v>
+        <v>8716</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -27865,7 +27868,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>8719</v>
+        <v>8717</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -27873,7 +27876,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>8722</v>
+        <v>8720</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -27881,7 +27884,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>8723</v>
+        <v>8721</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -27889,7 +27892,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>8724</v>
+        <v>8722</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -27897,7 +27900,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>8725</v>
+        <v>8723</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -27905,7 +27908,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>8726</v>
+        <v>8724</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -27913,7 +27916,7 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>8727</v>
+        <v>8725</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -27921,7 +27924,7 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>8728</v>
+        <v>8726</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -27929,7 +27932,7 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>8729</v>
+        <v>8727</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -27937,7 +27940,7 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>8730</v>
+        <v>8728</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -27945,7 +27948,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>8731</v>
+        <v>8729</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -27953,7 +27956,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>8733</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -27964,7 +27967,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>8734</v>
+        <v>8732</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -27975,7 +27978,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>8735</v>
+        <v>8733</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -27983,7 +27986,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>8736</v>
+        <v>8734</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -27991,7 +27994,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>8737</v>
+        <v>8735</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -27999,7 +28002,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>8738</v>
+        <v>8736</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -28007,7 +28010,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>8739</v>
+        <v>8737</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -28015,12 +28018,12 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>8740</v>
+        <v>8738</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>8741</v>
+        <v>8739</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -28028,7 +28031,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>8742</v>
+        <v>8740</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -28036,7 +28039,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>8743</v>
+        <v>8741</v>
       </c>
     </row>
   </sheetData>
@@ -28055,13 +28058,13 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:J339"/>
+  <dimension ref="A1:J341"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C269" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C261" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B273" sqref="A1:H339"/>
+      <selection pane="bottomRight" activeCell="B271" sqref="A1:H341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31304,7 +31307,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>8704</v>
+        <v>8702</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>751</v>
@@ -34399,8 +34402,8 @@
       </c>
       <c r="C281" s="12"/>
       <c r="D281" s="12" t="str">
-        <f>Enums!$A$4</f>
-        <v>Gas</v>
+        <f>Enums!$A$3</f>
+        <v>Liquid</v>
       </c>
       <c r="E281" s="12"/>
       <c r="F281" s="12"/>
@@ -34851,7 +34854,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B302" s="17" t="s">
-        <v>8705</v>
+        <v>8703</v>
       </c>
       <c r="C302" s="18" t="s">
         <v>327</v>
@@ -35192,7 +35195,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>8560</v>
+        <v>8558</v>
       </c>
       <c r="C317" s="14"/>
       <c r="D317" s="12" t="str">
@@ -35533,10 +35536,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>8699</v>
+        <v>8697</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>8698</v>
+        <v>8696</v>
       </c>
       <c r="D337" s="12" t="str">
         <f>Enums!$A$2</f>
@@ -35552,10 +35555,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>8700</v>
+        <v>8698</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>8701</v>
+        <v>8699</v>
       </c>
       <c r="D338" s="12" t="str">
         <f>Enums!$A$3</f>
@@ -35568,12 +35571,41 @@
         <v>1.0.0</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>8702</v>
+        <v>8700</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>8703</v>
+        <v>8701</v>
       </c>
       <c r="D339" s="12" t="str">
+        <f>Enums!$A$3</f>
+        <v>Liquid</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>8747</v>
+      </c>
+      <c r="C340" s="12" t="s">
+        <v>700</v>
+      </c>
+      <c r="D340" s="12" t="str">
+        <f>Enums!$A$3</f>
+        <v>Liquid</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>8748</v>
+      </c>
+      <c r="D341" s="12" t="str">
         <f>Enums!$A$3</f>
         <v>Liquid</v>
       </c>
@@ -37999,10 +38031,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>8696</v>
+        <v>8694</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>8695</v>
+        <v>8693</v>
       </c>
       <c r="F115" s="1" t="b">
         <v>0</v>
@@ -38164,7 +38196,7 @@
         <v>1.0.3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8747</v>
+        <v>8745</v>
       </c>
     </row>
   </sheetData>
@@ -38182,10 +38214,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D42" sqref="A1:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38274,7 +38306,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>240</v>
@@ -38302,7 +38334,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>180</v>
@@ -38314,7 +38346,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" ref="B5:B18" si="1">D5</f>
+        <f t="shared" ref="B5:B51" si="1">D5</f>
         <v>Methane</v>
       </c>
       <c r="C5" t="str">
@@ -38326,11 +38358,11 @@
         <v>Methane</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E18" si="2" xml:space="preserve"> E4 + 1</f>
+        <f t="shared" ref="E5:E51" si="2" xml:space="preserve"> E4 + 1</f>
         <v>3</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <v>240</v>
@@ -38386,7 +38418,7 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <v>360</v>
@@ -38414,7 +38446,7 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <v>240</v>
@@ -38442,7 +38474,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>120</v>
@@ -38498,7 +38530,7 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <v>240</v>
@@ -38526,7 +38558,7 @@
         <v>10</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>240</v>
@@ -38554,7 +38586,7 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>360</v>
@@ -38698,6 +38730,930 @@
       </c>
       <c r="G18">
         <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>Butane Isomers</v>
+      </c>
+      <c r="C19" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D19" t="str">
+        <f>Compounds!B68</f>
+        <v>Butane Isomers</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="1"/>
+        <v>Sweet Kerosene</v>
+      </c>
+      <c r="C20" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D20" t="str">
+        <f>Compounds!B340</f>
+        <v>Sweet Kerosene</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="1"/>
+        <v>Sweet Diesel</v>
+      </c>
+      <c r="C21" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D21" t="str">
+        <f>Compounds!B341</f>
+        <v>Sweet Diesel</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="1"/>
+        <v>Benzene-Toluene-Xylene</v>
+      </c>
+      <c r="C22" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D22" t="str">
+        <f>Compounds!B60</f>
+        <v>Benzene-Toluene-Xylene</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>Ethanol</v>
+      </c>
+      <c r="C23" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D23" t="str">
+        <f>Compounds!B126</f>
+        <v>Ethanol</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>Butanol</v>
+      </c>
+      <c r="C24" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D24" t="str">
+        <f>Compounds!B69</f>
+        <v>Butanol</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>Heavy Naphtha</v>
+      </c>
+      <c r="C25" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D25" t="str">
+        <f>Compounds!B147</f>
+        <v>Heavy Naphtha</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>Hydrogen Gas</v>
+      </c>
+      <c r="C26" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D26" t="str">
+        <f>Compounds!B154</f>
+        <v>Hydrogen Gas</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoButane</v>
+      </c>
+      <c r="C27" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D27" t="str">
+        <f>Compounds!B160</f>
+        <v>IsoButane</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoPentane</v>
+      </c>
+      <c r="C28" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D28" t="str">
+        <f>Compounds!B161</f>
+        <v>IsoPentane</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="1"/>
+        <v>Light Olefins</v>
+      </c>
+      <c r="C29" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D29" t="str">
+        <f>Compounds!B169</f>
+        <v>Light Olefins</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="1"/>
+        <v>Light Parrafins</v>
+      </c>
+      <c r="C30" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D30" t="str">
+        <f>Compounds!B170</f>
+        <v>Light Parrafins</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="1"/>
+        <v>Methanol</v>
+      </c>
+      <c r="C31" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D31" t="str">
+        <f>Compounds!B194</f>
+        <v>Methanol</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="1"/>
+        <v>Meta-Xylene</v>
+      </c>
+      <c r="C32" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D32" t="str">
+        <f>Compounds!B190</f>
+        <v>Meta-Xylene</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="1"/>
+        <v>N-Butane</v>
+      </c>
+      <c r="C33" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D33" t="str">
+        <f>Compounds!B204</f>
+        <v>N-Butane</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="1"/>
+        <v>N-Hexane</v>
+      </c>
+      <c r="C34" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D34" t="str">
+        <f>Compounds!B206</f>
+        <v>N-Hexane</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="1"/>
+        <v>N-Pentane</v>
+      </c>
+      <c r="C35" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D35" t="str">
+        <f>Compounds!B207</f>
+        <v>N-Pentane</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="1"/>
+        <v>NeoPentane</v>
+      </c>
+      <c r="C36" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D36" t="str">
+        <f>Compounds!B212</f>
+        <v>NeoPentane</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="1"/>
+        <v>Olefins</v>
+      </c>
+      <c r="C37" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D37" t="str">
+        <f>Compounds!B215</f>
+        <v>Olefins</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="1"/>
+        <v>Ortho-Xylene</v>
+      </c>
+      <c r="C38" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D38" t="str">
+        <f>Compounds!B217</f>
+        <v>Ortho-Xylene</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="1"/>
+        <v>Para-Xylene</v>
+      </c>
+      <c r="C39" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D39" t="str">
+        <f>Compounds!B221</f>
+        <v>Para-Xylene</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="1"/>
+        <v>Paraffin</v>
+      </c>
+      <c r="C40" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D40" t="str">
+        <f>Compounds!B222</f>
+        <v>Paraffin</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="1"/>
+        <v>Pentane Isomers</v>
+      </c>
+      <c r="C41" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D41" t="str">
+        <f>Compounds!B223</f>
+        <v>Pentane Isomers</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="F41">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="1"/>
+        <v>Propanol</v>
+      </c>
+      <c r="C42" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D42" t="str">
+        <f>Compounds!B247</f>
+        <v>Propanol</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="1"/>
+        <v>Xylene</v>
+      </c>
+      <c r="C43" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D43" t="str">
+        <f>Compounds!B303</f>
+        <v>Xylene</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="1"/>
+        <v>Toluene</v>
+      </c>
+      <c r="C44" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D44" t="str">
+        <f>Compounds!B290</f>
+        <v>Toluene</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="1"/>
+        <v>Benzene</v>
+      </c>
+      <c r="C45" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D45" t="str">
+        <f>Compounds!B59</f>
+        <v>Benzene</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="1"/>
+        <v>Fruit Brandy</v>
+      </c>
+      <c r="C46" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D46" t="str">
+        <f>Compounds!B327</f>
+        <v>Fruit Brandy</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="1"/>
+        <v>Vodka</v>
+      </c>
+      <c r="C47" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D47" t="str">
+        <f>Compounds!B328</f>
+        <v>Vodka</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="1"/>
+        <v>Gin</v>
+      </c>
+      <c r="C48" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D48" t="str">
+        <f>Compounds!B329</f>
+        <v>Gin</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="1"/>
+        <v>Tequila</v>
+      </c>
+      <c r="C49" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D49" t="str">
+        <f>Compounds!B330</f>
+        <v>Tequila</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="1"/>
+        <v>Rum</v>
+      </c>
+      <c r="C50" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D50" t="str">
+        <f>Compounds!B331</f>
+        <v>Rum</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>Enums!$A$98</f>
+        <v>1.0.4</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="1"/>
+        <v>Whiskey</v>
+      </c>
+      <c r="C51" t="str">
+        <f xml:space="preserve"> Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="D51" t="str">
+        <f>Compounds!B332</f>
+        <v>Whiskey</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -39519,7 +40475,7 @@
         <v>1374</v>
       </c>
       <c r="B91" s="64" t="s">
-        <v>8565</v>
+        <v>8563</v>
       </c>
       <c r="C91" s="64" t="s">
         <v>1376</v>
@@ -39528,25 +40484,25 @@
         <v>1413</v>
       </c>
       <c r="E91" s="64" t="s">
-        <v>8566</v>
+        <v>8564</v>
       </c>
       <c r="F91" s="64" t="s">
-        <v>8567</v>
+        <v>8565</v>
       </c>
       <c r="G91" s="64" t="s">
         <v>1373</v>
       </c>
       <c r="H91" s="64" t="s">
-        <v>8568</v>
+        <v>8566</v>
       </c>
       <c r="I91" s="64" t="s">
         <v>1372</v>
       </c>
       <c r="J91" s="64" t="s">
-        <v>8569</v>
+        <v>8567</v>
       </c>
       <c r="K91" s="64" t="s">
-        <v>8570</v>
+        <v>8568</v>
       </c>
       <c r="L91" s="64" t="s">
         <v>1371</v>
@@ -39561,67 +40517,67 @@
         <v>1368</v>
       </c>
       <c r="P91" s="64" t="s">
+        <v>8569</v>
+      </c>
+      <c r="Q91" s="64" t="s">
+        <v>8570</v>
+      </c>
+      <c r="R91" s="64" t="s">
         <v>8571</v>
       </c>
-      <c r="Q91" s="64" t="s">
+      <c r="S91" s="64" t="s">
         <v>8572</v>
       </c>
-      <c r="R91" s="64" t="s">
+      <c r="T91" s="64" t="s">
         <v>8573</v>
       </c>
-      <c r="S91" s="64" t="s">
+      <c r="U91" s="64" t="s">
         <v>8574</v>
       </c>
-      <c r="T91" s="64" t="s">
+      <c r="V91" s="64" t="s">
         <v>8575</v>
       </c>
-      <c r="U91" s="64" t="s">
+      <c r="W91" s="64" t="s">
         <v>8576</v>
       </c>
-      <c r="V91" s="64" t="s">
+      <c r="X91" s="64" t="s">
         <v>8577</v>
       </c>
-      <c r="W91" s="64" t="s">
+      <c r="Y91" s="64" t="s">
         <v>8578</v>
       </c>
-      <c r="X91" s="64" t="s">
+      <c r="Z91" s="64" t="s">
         <v>8579</v>
       </c>
-      <c r="Y91" s="64" t="s">
+      <c r="AA91" s="64" t="s">
         <v>8580</v>
       </c>
-      <c r="Z91" s="64" t="s">
+      <c r="AB91" s="64" t="s">
         <v>8581</v>
       </c>
-      <c r="AA91" s="64" t="s">
+      <c r="AC91" s="64" t="s">
         <v>8582</v>
       </c>
-      <c r="AB91" s="64" t="s">
+      <c r="AD91" s="64" t="s">
         <v>8583</v>
       </c>
-      <c r="AC91" s="64" t="s">
+      <c r="AE91" s="64" t="s">
         <v>8584</v>
       </c>
-      <c r="AD91" s="64" t="s">
+      <c r="AF91" s="64" t="s">
         <v>8585</v>
       </c>
-      <c r="AE91" s="64" t="s">
+      <c r="AG91" s="64" t="s">
         <v>8586</v>
       </c>
-      <c r="AF91" s="64" t="s">
+      <c r="AH91" s="64" t="s">
         <v>8587</v>
       </c>
-      <c r="AG91" s="64" t="s">
+      <c r="AI91" s="64" t="s">
         <v>8588</v>
       </c>
-      <c r="AH91" s="64" t="s">
+      <c r="AJ91" s="64" t="s">
         <v>8589</v>
-      </c>
-      <c r="AI91" s="64" t="s">
-        <v>8590</v>
-      </c>
-      <c r="AJ91" s="64" t="s">
-        <v>8591</v>
       </c>
     </row>
     <row r="92" spans="1:36" ht="26.25" x14ac:dyDescent="0.25">
@@ -39629,13 +40585,13 @@
         <v>1</v>
       </c>
       <c r="B92" s="66" t="s">
-        <v>8592</v>
+        <v>8590</v>
       </c>
       <c r="C92" s="67" t="s">
         <v>1264</v>
       </c>
       <c r="D92" s="67" t="s">
-        <v>8593</v>
+        <v>8591</v>
       </c>
       <c r="E92" s="66" t="str">
         <f>"Fiber ("&amp;B92&amp;")"</f>
@@ -39657,40 +40613,40 @@
         <v>4</v>
       </c>
       <c r="L92" s="67" t="s">
+        <v>8592</v>
+      </c>
+      <c r="M92" s="67" t="s">
+        <v>8593</v>
+      </c>
+      <c r="N92" s="67" t="s">
         <v>8594</v>
       </c>
-      <c r="M92" s="67" t="s">
+      <c r="O92" s="67" t="s">
         <v>8595</v>
       </c>
-      <c r="N92" s="67" t="s">
+      <c r="P92" s="67" t="s">
         <v>8596</v>
       </c>
-      <c r="O92" s="67" t="s">
+      <c r="Q92" s="67" t="s">
         <v>8597</v>
       </c>
-      <c r="P92" s="67" t="s">
+      <c r="R92" s="67" t="s">
         <v>8598</v>
       </c>
-      <c r="Q92" s="67" t="s">
+      <c r="S92" s="67" t="s">
         <v>8599</v>
       </c>
-      <c r="R92" s="67" t="s">
+      <c r="T92" s="67" t="s">
         <v>8600</v>
       </c>
-      <c r="S92" s="67" t="s">
+      <c r="U92" s="67" t="s">
         <v>8601</v>
       </c>
-      <c r="T92" s="67" t="s">
+      <c r="V92" s="67" t="s">
         <v>8602</v>
       </c>
-      <c r="U92" s="67" t="s">
+      <c r="W92" s="67" t="s">
         <v>8603</v>
-      </c>
-      <c r="V92" s="67" t="s">
-        <v>8604</v>
-      </c>
-      <c r="W92" s="67" t="s">
-        <v>8605</v>
       </c>
       <c r="X92"/>
       <c r="Y92"/>
@@ -39711,13 +40667,13 @@
         <v>2</v>
       </c>
       <c r="B93" s="66" t="s">
-        <v>8606</v>
+        <v>8604</v>
       </c>
       <c r="C93" s="67" t="s">
         <v>1338</v>
       </c>
       <c r="D93" s="67" t="s">
-        <v>8607</v>
+        <v>8605</v>
       </c>
       <c r="E93" s="66" t="str">
         <f t="shared" ref="E93:E102" si="1">"Fiber ("&amp;B93&amp;")"</f>
@@ -39739,34 +40695,34 @@
         <v>4</v>
       </c>
       <c r="L93" s="67" t="s">
+        <v>8606</v>
+      </c>
+      <c r="M93" s="67" t="s">
+        <v>8607</v>
+      </c>
+      <c r="N93" s="67" t="s">
         <v>8608</v>
       </c>
-      <c r="M93" s="67" t="s">
+      <c r="O93" s="67" t="s">
         <v>8609</v>
       </c>
-      <c r="N93" s="67" t="s">
+      <c r="P93" s="67" t="s">
         <v>8610</v>
       </c>
-      <c r="O93" s="67" t="s">
+      <c r="Q93" s="67" t="s">
         <v>8611</v>
       </c>
-      <c r="P93" s="67" t="s">
+      <c r="R93" s="67" t="s">
         <v>8612</v>
       </c>
-      <c r="Q93" s="67" t="s">
+      <c r="S93" s="67" t="s">
         <v>8613</v>
       </c>
-      <c r="R93" s="67" t="s">
+      <c r="T93" s="67" t="s">
         <v>8614</v>
       </c>
-      <c r="S93" s="67" t="s">
+      <c r="U93" s="67" t="s">
         <v>8615</v>
-      </c>
-      <c r="T93" s="67" t="s">
-        <v>8616</v>
-      </c>
-      <c r="U93" s="67" t="s">
-        <v>8617</v>
       </c>
       <c r="V93"/>
       <c r="W93"/>
@@ -39795,7 +40751,7 @@
         <v>1180</v>
       </c>
       <c r="D94" s="67" t="s">
-        <v>8607</v>
+        <v>8605</v>
       </c>
       <c r="E94" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39817,34 +40773,34 @@
         <v>4</v>
       </c>
       <c r="L94" s="67" t="s">
+        <v>8616</v>
+      </c>
+      <c r="M94" s="67" t="s">
+        <v>8617</v>
+      </c>
+      <c r="N94" s="67" t="s">
         <v>8618</v>
       </c>
-      <c r="M94" s="67" t="s">
+      <c r="O94" s="67" t="s">
         <v>8619</v>
       </c>
-      <c r="N94" s="67" t="s">
+      <c r="P94" s="67" t="s">
         <v>8620</v>
       </c>
-      <c r="O94" s="67" t="s">
+      <c r="Q94" s="67" t="s">
         <v>8621</v>
       </c>
-      <c r="P94" s="67" t="s">
+      <c r="R94" s="67" t="s">
         <v>8622</v>
       </c>
-      <c r="Q94" s="67" t="s">
+      <c r="S94" s="67" t="s">
         <v>8623</v>
       </c>
-      <c r="R94" s="67" t="s">
+      <c r="T94" s="67" t="s">
         <v>8624</v>
       </c>
-      <c r="S94" s="67" t="s">
+      <c r="U94" s="67" t="s">
         <v>8625</v>
-      </c>
-      <c r="T94" s="67" t="s">
-        <v>8626</v>
-      </c>
-      <c r="U94" s="67" t="s">
-        <v>8627</v>
       </c>
       <c r="V94"/>
       <c r="W94"/>
@@ -39867,13 +40823,13 @@
         <v>4</v>
       </c>
       <c r="B95" s="66" t="s">
-        <v>8628</v>
+        <v>8626</v>
       </c>
       <c r="C95" s="67" t="s">
         <v>1326</v>
       </c>
       <c r="D95" s="67" t="s">
-        <v>8607</v>
+        <v>8605</v>
       </c>
       <c r="E95" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39898,19 +40854,19 @@
         <v>8435</v>
       </c>
       <c r="M95" s="67" t="s">
+        <v>8627</v>
+      </c>
+      <c r="N95" s="67" t="s">
+        <v>8628</v>
+      </c>
+      <c r="O95" s="67" t="s">
         <v>8629</v>
-      </c>
-      <c r="N95" s="67" t="s">
-        <v>8630</v>
-      </c>
-      <c r="O95" s="67" t="s">
-        <v>8631</v>
       </c>
       <c r="P95" s="67" t="s">
         <v>8461</v>
       </c>
       <c r="Q95" s="67" t="s">
-        <v>8632</v>
+        <v>8630</v>
       </c>
       <c r="R95"/>
       <c r="S95"/>
@@ -39943,7 +40899,7 @@
         <v>1208</v>
       </c>
       <c r="D96" s="67" t="s">
-        <v>8607</v>
+        <v>8605</v>
       </c>
       <c r="E96" s="66" t="str">
         <f t="shared" si="1"/>
@@ -39965,61 +40921,61 @@
         <v>4</v>
       </c>
       <c r="L96" s="67" t="s">
-        <v>8621</v>
+        <v>8619</v>
       </c>
       <c r="M96" s="67" t="s">
         <v>8435</v>
       </c>
       <c r="N96" s="67" t="s">
-        <v>8630</v>
+        <v>8628</v>
       </c>
       <c r="O96" s="67" t="s">
+        <v>8631</v>
+      </c>
+      <c r="P96" s="67" t="s">
+        <v>8632</v>
+      </c>
+      <c r="Q96" s="67" t="s">
         <v>8633</v>
       </c>
-      <c r="P96" s="67" t="s">
+      <c r="R96" s="67" t="s">
         <v>8634</v>
       </c>
-      <c r="Q96" s="67" t="s">
+      <c r="S96" s="67" t="s">
         <v>8635</v>
       </c>
-      <c r="R96" s="67" t="s">
+      <c r="T96" s="67" t="s">
         <v>8636</v>
       </c>
-      <c r="S96" s="67" t="s">
+      <c r="U96" s="67" t="s">
         <v>8637</v>
       </c>
-      <c r="T96" s="67" t="s">
+      <c r="V96" s="67" t="s">
         <v>8638</v>
       </c>
-      <c r="U96" s="67" t="s">
+      <c r="W96" s="67" t="s">
         <v>8639</v>
       </c>
-      <c r="V96" s="67" t="s">
+      <c r="X96" s="67" t="s">
         <v>8640</v>
       </c>
-      <c r="W96" s="67" t="s">
+      <c r="Y96" s="67" t="s">
         <v>8641</v>
       </c>
-      <c r="X96" s="67" t="s">
+      <c r="Z96" s="67" t="s">
         <v>8642</v>
       </c>
-      <c r="Y96" s="67" t="s">
+      <c r="AA96" s="67" t="s">
         <v>8643</v>
       </c>
-      <c r="Z96" s="67" t="s">
+      <c r="AB96" s="67" t="s">
         <v>8644</v>
       </c>
-      <c r="AA96" s="67" t="s">
+      <c r="AC96" s="67" t="s">
         <v>8645</v>
       </c>
-      <c r="AB96" s="67" t="s">
+      <c r="AD96" s="67" t="s">
         <v>8646</v>
-      </c>
-      <c r="AC96" s="67" t="s">
-        <v>8647</v>
-      </c>
-      <c r="AD96" s="67" t="s">
-        <v>8648</v>
       </c>
       <c r="AE96"/>
       <c r="AF96"/>
@@ -40039,7 +40995,7 @@
         <v>1202</v>
       </c>
       <c r="D97" s="67" t="s">
-        <v>8607</v>
+        <v>8605</v>
       </c>
       <c r="E97" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40063,28 +41019,28 @@
         <v>4</v>
       </c>
       <c r="L97" s="67" t="s">
-        <v>8649</v>
+        <v>8647</v>
       </c>
       <c r="M97" s="67" t="s">
-        <v>8650</v>
+        <v>8648</v>
       </c>
       <c r="N97" s="67" t="s">
         <v>8447</v>
       </c>
       <c r="O97" s="67" t="s">
+        <v>8649</v>
+      </c>
+      <c r="P97" s="67" t="s">
+        <v>8650</v>
+      </c>
+      <c r="Q97" s="67" t="s">
         <v>8651</v>
       </c>
-      <c r="P97" s="67" t="s">
+      <c r="R97" s="67" t="s">
         <v>8652</v>
       </c>
-      <c r="Q97" s="67" t="s">
+      <c r="S97" s="67" t="s">
         <v>8653</v>
-      </c>
-      <c r="R97" s="67" t="s">
-        <v>8654</v>
-      </c>
-      <c r="S97" s="67" t="s">
-        <v>8655</v>
       </c>
       <c r="T97"/>
       <c r="U97"/>
@@ -40115,7 +41071,7 @@
         <v>220</v>
       </c>
       <c r="D98" s="67" t="s">
-        <v>8656</v>
+        <v>8654</v>
       </c>
       <c r="E98" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40139,50 +41095,50 @@
         <v>4</v>
       </c>
       <c r="L98" s="67" t="s">
+        <v>8655</v>
+      </c>
+      <c r="M98" s="67" t="s">
+        <v>8656</v>
+      </c>
+      <c r="N98" s="67" t="s">
         <v>8657</v>
       </c>
-      <c r="M98" s="67" t="s">
+      <c r="O98" s="67" t="s">
         <v>8658</v>
-      </c>
-      <c r="N98" s="67" t="s">
-        <v>8659</v>
-      </c>
-      <c r="O98" s="67" t="s">
-        <v>8660</v>
       </c>
       <c r="P98" s="67"/>
       <c r="Q98" s="67" t="s">
+        <v>8659</v>
+      </c>
+      <c r="R98" s="67" t="s">
+        <v>8660</v>
+      </c>
+      <c r="S98" s="67" t="s">
         <v>8661</v>
       </c>
-      <c r="R98" s="67" t="s">
+      <c r="T98" s="67" t="s">
         <v>8662</v>
       </c>
-      <c r="S98" s="67" t="s">
+      <c r="U98" s="67" t="s">
         <v>8663</v>
       </c>
-      <c r="T98" s="67" t="s">
+      <c r="V98" s="67" t="s">
         <v>8664</v>
       </c>
-      <c r="U98" s="67" t="s">
+      <c r="W98" s="67" t="s">
         <v>8665</v>
       </c>
-      <c r="V98" s="67" t="s">
+      <c r="X98" s="67" t="s">
         <v>8666</v>
       </c>
-      <c r="W98" s="67" t="s">
+      <c r="Y98" s="67" t="s">
         <v>8667</v>
       </c>
-      <c r="X98" s="67" t="s">
+      <c r="Z98" s="67" t="s">
         <v>8668</v>
       </c>
-      <c r="Y98" s="67" t="s">
+      <c r="AA98" s="67" t="s">
         <v>8669</v>
-      </c>
-      <c r="Z98" s="67" t="s">
-        <v>8670</v>
-      </c>
-      <c r="AA98" s="67" t="s">
-        <v>8671</v>
       </c>
       <c r="AB98"/>
       <c r="AC98"/>
@@ -40205,7 +41161,7 @@
         <v>220</v>
       </c>
       <c r="D99" s="67" t="s">
-        <v>8672</v>
+        <v>8670</v>
       </c>
       <c r="E99" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40227,29 +41183,29 @@
         <v>4</v>
       </c>
       <c r="L99" s="67" t="s">
+        <v>8671</v>
+      </c>
+      <c r="M99" s="67" t="s">
+        <v>8672</v>
+      </c>
+      <c r="N99" s="67" t="s">
         <v>8673</v>
       </c>
-      <c r="M99" s="67" t="s">
+      <c r="O99" s="67" t="s">
         <v>8674</v>
       </c>
-      <c r="N99" s="67" t="s">
+      <c r="P99" s="67" t="s">
         <v>8675</v>
       </c>
-      <c r="O99" s="67" t="s">
+      <c r="Q99" s="67" t="s">
         <v>8676</v>
       </c>
-      <c r="P99" s="67" t="s">
+      <c r="R99" s="67" t="s">
         <v>8677</v>
-      </c>
-      <c r="Q99" s="67" t="s">
-        <v>8678</v>
-      </c>
-      <c r="R99" s="67" t="s">
-        <v>8679</v>
       </c>
       <c r="S99" s="67"/>
       <c r="T99" s="67" t="s">
-        <v>8680</v>
+        <v>8678</v>
       </c>
       <c r="U99"/>
       <c r="V99"/>
@@ -40273,13 +41229,13 @@
         <v>0</v>
       </c>
       <c r="B100" s="66" t="s">
-        <v>8681</v>
+        <v>8679</v>
       </c>
       <c r="C100" s="67" t="s">
         <v>7519</v>
       </c>
       <c r="D100" s="67" t="s">
-        <v>8682</v>
+        <v>8680</v>
       </c>
       <c r="E100" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40301,25 +41257,25 @@
         <v>4</v>
       </c>
       <c r="L100" s="67" t="s">
+        <v>8681</v>
+      </c>
+      <c r="M100" s="67" t="s">
+        <v>8682</v>
+      </c>
+      <c r="N100" s="67" t="s">
         <v>8683</v>
       </c>
-      <c r="M100" s="67" t="s">
+      <c r="O100" s="67" t="s">
         <v>8684</v>
       </c>
-      <c r="N100" s="67" t="s">
+      <c r="P100" s="67" t="s">
         <v>8685</v>
       </c>
-      <c r="O100" s="67" t="s">
+      <c r="Q100" s="67" t="s">
         <v>8686</v>
       </c>
-      <c r="P100" s="67" t="s">
+      <c r="R100" s="67" t="s">
         <v>8687</v>
-      </c>
-      <c r="Q100" s="67" t="s">
-        <v>8688</v>
-      </c>
-      <c r="R100" s="67" t="s">
-        <v>8689</v>
       </c>
       <c r="S100"/>
       <c r="T100"/>
@@ -40345,13 +41301,13 @@
         <v>10</v>
       </c>
       <c r="B101" s="66" t="s">
-        <v>8690</v>
+        <v>8688</v>
       </c>
       <c r="C101" s="67" t="s">
         <v>7520</v>
       </c>
       <c r="D101" s="67" t="s">
-        <v>8682</v>
+        <v>8680</v>
       </c>
       <c r="E101" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40403,13 +41359,13 @@
         <v>0</v>
       </c>
       <c r="B102" s="66" t="s">
-        <v>8691</v>
+        <v>8689</v>
       </c>
       <c r="C102" s="67" t="s">
-        <v>8692</v>
+        <v>8690</v>
       </c>
       <c r="D102" s="67" t="s">
-        <v>8691</v>
+        <v>8689</v>
       </c>
       <c r="E102" s="66" t="str">
         <f t="shared" si="1"/>
@@ -40431,10 +41387,10 @@
         <v>4</v>
       </c>
       <c r="L102" s="67" t="s">
-        <v>8693</v>
+        <v>8691</v>
       </c>
       <c r="M102" s="67" t="s">
-        <v>8694</v>
+        <v>8692</v>
       </c>
       <c r="N102" s="67" t="s">
         <v>8354</v>
@@ -41837,10 +42793,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -41883,7 +42839,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>8552</v>
+        <v>8550</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>$A$2</f>
@@ -41919,7 +42875,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>8553</v>
+        <v>8551</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>$A$2</f>
@@ -42390,42 +43346,42 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>8554</v>
+        <v>8552</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>8555</v>
+        <v>8553</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>8556</v>
+        <v>8554</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>8557</v>
+        <v>8555</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>8558</v>
+        <v>8556</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>8559</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>8561</v>
+        <v>8559</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="63" t="s">
-        <v>8562</v>
+        <v>8560</v>
       </c>
       <c r="B94" s="69">
         <v>41804</v>
@@ -42433,7 +43389,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="63" t="s">
-        <v>8563</v>
+        <v>8561</v>
       </c>
       <c r="B95" s="69">
         <v>41805</v>
@@ -42441,7 +43397,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="63" t="s">
-        <v>8745</v>
+        <v>8743</v>
       </c>
       <c r="B96" s="69">
         <v>41806</v>
@@ -42449,7 +43405,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="63" t="s">
-        <v>8744</v>
+        <v>8742</v>
       </c>
       <c r="B97" s="69">
         <v>41813</v>
@@ -42457,10 +43413,18 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="63" t="s">
-        <v>8564</v>
-      </c>
-      <c r="B98" s="1" t="s">
         <v>8746</v>
+      </c>
+      <c r="B98" s="69">
+        <v>41868</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="63" t="s">
+        <v>8562</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>8744</v>
       </c>
     </row>
   </sheetData>
@@ -42481,8 +43445,8 @@
   </sheetPr>
   <dimension ref="A1:J6104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42496,15 +43460,7 @@
         <v>7576</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>8551</v>
-      </c>
-    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
-        <v>8550</v>
-      </c>
       <c r="J4" s="35"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -91268,7 +92224,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -91347,7 +92303,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8697</v>
+        <v>8695</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -91378,7 +92334,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -91497,10 +92453,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8564</v>
+        <v>8562</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8706</v>
+        <v>8704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fuel fix - partway - not stable build
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75945" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="1"/>
+    <workbookView xWindow="75945" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -27284,7 +27284,7 @@
   </sheetPr>
   <dimension ref="A1:C5988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -57197,7 +57197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
@@ -63662,7 +63662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
       <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
@@ -69729,7 +69729,7 @@
   <dimension ref="A1:N193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
@@ -75723,10 +75723,10 @@
   <dimension ref="A1:J352"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C325" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B359" sqref="B359"/>
+      <selection pane="bottomRight" activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed Fuel Bug in 1.1.0
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75945" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="3"/>
+    <workbookView xWindow="75945" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -63662,7 +63662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+    <sheetView topLeftCell="A142" workbookViewId="0">
       <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
@@ -75722,8 +75722,8 @@
   </sheetPr>
   <dimension ref="A1:J352"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C238" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A153" sqref="A153"/>

</xml_diff>

<commit_message>
Added Different Jet Packs and Altitude Limit, some recipe changes
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="83385" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="7"/>
+    <workbookView xWindow="84315" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -73038,7 +73039,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C349" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F369" sqref="F369"/>
+      <selection pane="bottomRight" activeCell="F370" sqref="F370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed major problems with 3D lamps and placing 3d inventories close to each other.
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="85245" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860"/>
+    <workbookView xWindow="85245" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -25063,8 +25063,8 @@
   </sheetPr>
   <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -71899,11 +71899,11 @@
   </sheetPr>
   <dimension ref="A1:J399"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C368" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B402" sqref="B402"/>
+      <selection pane="bottomRight" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -73980,9 +73980,9 @@
         <v>875</v>
       </c>
       <c r="C90" s="12"/>
-      <c r="D90" s="12" t="str">
-        <f>Enums!$A$21</f>
-        <v>Liquid</v>
+      <c r="D90" s="18" t="str">
+        <f>Enums!$A$22</f>
+        <v>Gas</v>
       </c>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>

</xml_diff>

<commit_message>
Added new 3D textures
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="86175" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="7"/>
+    <workbookView xWindow="87105" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -23285,9 +23285,6 @@
     <t>Antifreeze</t>
   </si>
   <si>
-    <t>Large Pipe</t>
-  </si>
-  <si>
     <t>C3H6</t>
   </si>
   <si>
@@ -24338,6 +24335,9 @@
   </si>
   <si>
     <t>1.1.4</t>
+  </si>
+  <si>
+    <t>Pipe Segment</t>
   </si>
 </sst>
 </file>
@@ -25076,12 +25076,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>7729</v>
+        <v>7728</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
-        <v>7730</v>
+        <v>7729</v>
       </c>
       <c r="B2" s="54">
         <v>41804</v>
@@ -25089,7 +25089,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
-        <v>7731</v>
+        <v>7730</v>
       </c>
       <c r="B3" s="54">
         <v>41805</v>
@@ -25097,7 +25097,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
-        <v>7746</v>
+        <v>7745</v>
       </c>
       <c r="B4" s="54">
         <v>41806</v>
@@ -25105,7 +25105,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>7745</v>
+        <v>7744</v>
       </c>
       <c r="B5" s="54">
         <v>41813</v>
@@ -25113,7 +25113,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="53" t="s">
-        <v>7749</v>
+        <v>7748</v>
       </c>
       <c r="B6" s="54">
         <v>41868</v>
@@ -25121,15 +25121,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="53" t="s">
+        <v>7752</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>7753</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>7754</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7752</v>
+        <v>7751</v>
       </c>
       <c r="B8" s="54">
         <v>41930</v>
@@ -25137,7 +25137,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7755</v>
+        <v>7754</v>
       </c>
       <c r="B9" s="54">
         <v>41932</v>
@@ -25145,7 +25145,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7756</v>
+        <v>7755</v>
       </c>
       <c r="B10" s="54">
         <v>41941</v>
@@ -25153,7 +25153,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7757</v>
+        <v>7756</v>
       </c>
       <c r="B11" s="54">
         <v>41998</v>
@@ -25161,7 +25161,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>7732</v>
+        <v>7731</v>
       </c>
       <c r="B12" s="54">
         <v>42002</v>
@@ -25169,7 +25169,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7841</v>
+        <v>7840</v>
       </c>
       <c r="B13" s="54">
         <v>42037</v>
@@ -25177,7 +25177,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>7870</v>
+        <v>7869</v>
       </c>
       <c r="B14" s="54">
         <v>42042</v>
@@ -25185,7 +25185,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>7917</v>
+        <v>7916</v>
       </c>
       <c r="B15" s="54">
         <v>42060</v>
@@ -25193,7 +25193,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>7918</v>
+        <v>7917</v>
       </c>
       <c r="B16" s="54">
         <v>42062</v>
@@ -25201,10 +25201,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>7758</v>
+        <v>7757</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7747</v>
+        <v>7746</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -25232,7 +25232,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>7687</v>
+        <v>7686</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>1387</v>
@@ -25243,7 +25243,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>7720</v>
+        <v>7719</v>
       </c>
       <c r="B25" s="1" t="str">
         <f>$A$20</f>
@@ -25279,7 +25279,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>7721</v>
+        <v>7720</v>
       </c>
       <c r="B28" s="1" t="str">
         <f>$A$20</f>
@@ -25315,7 +25315,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>7695</v>
+        <v>7694</v>
       </c>
       <c r="B31" s="1" t="str">
         <f>$A$20</f>
@@ -25390,7 +25390,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>7688</v>
+        <v>7687</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -25627,7 +25627,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>7689</v>
+        <v>7688</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -25688,22 +25688,22 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>7690</v>
+        <v>7689</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>7685</v>
+        <v>7684</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>7686</v>
+        <v>7685</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>7777</v>
+        <v>7776</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -25780,7 +25780,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>7744</v>
+        <v>7743</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>7656</v>
@@ -25788,7 +25788,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>7774</v>
+        <v>7773</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>7656</v>
@@ -25796,125 +25796,125 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>7779</v>
+        <v>7778</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>7778</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>7760</v>
+        <v>7759</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>7761</v>
+        <v>7760</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>7762</v>
+        <v>7761</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>7763</v>
+        <v>7762</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>7764</v>
+        <v>7763</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>7770</v>
+        <v>7769</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>7771</v>
+        <v>7770</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>7765</v>
+        <v>7764</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>7766</v>
+        <v>7765</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>7767</v>
+        <v>7766</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>7768</v>
+        <v>7767</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>7769</v>
+        <v>7768</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
-        <v>7722</v>
+        <v>7721</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>7723</v>
+        <v>7722</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>7724</v>
+        <v>7723</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>7725</v>
+        <v>7724</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>7726</v>
+        <v>7725</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>7727</v>
+        <v>7726</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
-        <v>7828</v>
+        <v>7827</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>7829</v>
+        <v>7828</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>7830</v>
+        <v>7829</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
-        <v>7890</v>
+        <v>7889</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>7891</v>
+        <v>7890</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
@@ -25924,7 +25924,7 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>7892</v>
+        <v>7891</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
@@ -25945,8 +25945,8 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25962,7 +25962,7 @@
         <v>Version</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7693</v>
+        <v>7692</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -26061,7 +26061,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7678</v>
+        <v>7918</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -26070,7 +26070,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7696</v>
+        <v>7695</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -26079,7 +26079,7 @@
         <v>1.0.3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7748</v>
+        <v>7747</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -26088,7 +26088,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7772</v>
+        <v>7771</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -26097,7 +26097,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7790</v>
+        <v>7789</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -26106,7 +26106,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7801</v>
+        <v>7800</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -26115,7 +26115,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7802</v>
+        <v>7801</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -26124,7 +26124,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7803</v>
+        <v>7802</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -26133,7 +26133,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7804</v>
+        <v>7803</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -26142,7 +26142,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7805</v>
+        <v>7804</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -26151,7 +26151,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7806</v>
+        <v>7805</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -26160,7 +26160,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7807</v>
+        <v>7806</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -26169,7 +26169,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7808</v>
+        <v>7807</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -26178,7 +26178,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7809</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -26187,7 +26187,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>7810</v>
+        <v>7809</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -26196,7 +26196,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7811</v>
+        <v>7810</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -26205,7 +26205,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7812</v>
+        <v>7811</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -26214,7 +26214,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7827</v>
+        <v>7826</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -26223,7 +26223,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7871</v>
+        <v>7870</v>
       </c>
     </row>
   </sheetData>
@@ -26253,7 +26253,7 @@
         <v>6930</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>7759</v>
+        <v>7758</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -53405,7 +53405,7 @@
         <v>Version</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>7691</v>
+        <v>7690</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -59868,7 +59868,7 @@
         <v>Version</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7692</v>
+        <v>7691</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -65946,7 +65946,7 @@
         <v>246</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>7719</v>
+        <v>7718</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>245</v>
@@ -69711,7 +69711,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>7776</v>
+        <v>7775</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>72</v>
@@ -71702,7 +71702,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7735</v>
+        <v>7734</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -71720,7 +71720,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7894</v>
+        <v>7893</v>
       </c>
     </row>
   </sheetData>
@@ -71860,7 +71860,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7744</v>
+        <v>7743</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -71869,7 +71869,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7774</v>
+        <v>7773</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -71878,7 +71878,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7775</v>
+        <v>7774</v>
       </c>
     </row>
   </sheetData>
@@ -71899,7 +71899,7 @@
   </sheetPr>
   <dimension ref="A1:J399"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -72109,7 +72109,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7859</v>
+        <v>7858</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>1108</v>
@@ -72134,7 +72134,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7860</v>
+        <v>7859</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>1106</v>
@@ -72159,7 +72159,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7861</v>
+        <v>7860</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>1104</v>
@@ -73113,10 +73113,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>7876</v>
+        <v>7875</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>7875</v>
+        <v>7874</v>
       </c>
       <c r="D52" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -73519,10 +73519,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>7683</v>
+        <v>7682</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>7681</v>
+        <v>7680</v>
       </c>
       <c r="D70" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -73534,7 +73534,7 @@
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12" t="s">
-        <v>7684</v>
+        <v>7683</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -73867,7 +73867,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>7850</v>
+        <v>7849</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>885</v>
@@ -73933,7 +73933,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>7833</v>
+        <v>7832</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="12" t="str">
@@ -74240,7 +74240,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>7858</v>
+        <v>7857</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>282</v>
@@ -74966,7 +74966,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>7857</v>
+        <v>7856</v>
       </c>
       <c r="C136" s="12" t="s">
         <v>301</v>
@@ -75124,7 +75124,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>7742</v>
+        <v>7741</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>744</v>
@@ -75278,10 +75278,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B150" s="17" t="s">
+        <v>7699</v>
+      </c>
+      <c r="C150" s="18" t="s">
         <v>7700</v>
-      </c>
-      <c r="C150" s="18" t="s">
-        <v>7701</v>
       </c>
       <c r="D150" s="18" t="str">
         <f>Enums!$A$21</f>
@@ -75962,10 +75962,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B180" s="1" t="s">
+        <v>7701</v>
+      </c>
+      <c r="C180" s="12" t="s">
         <v>7702</v>
-      </c>
-      <c r="C180" s="12" t="s">
-        <v>7703</v>
       </c>
       <c r="D180" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -75982,10 +75982,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>7854</v>
+        <v>7853</v>
       </c>
       <c r="C181" t="s">
-        <v>7705</v>
+        <v>7704</v>
       </c>
       <c r="D181" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -75993,7 +75993,7 @@
       </c>
       <c r="E181" s="12"/>
       <c r="F181" s="12" t="s">
-        <v>7712</v>
+        <v>7711</v>
       </c>
       <c r="G181" s="12"/>
       <c r="H181" s="12"/>
@@ -76004,10 +76004,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>7855</v>
+        <v>7854</v>
       </c>
       <c r="C182" t="s">
-        <v>7706</v>
+        <v>7705</v>
       </c>
       <c r="D182" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -76015,7 +76015,7 @@
       </c>
       <c r="E182" s="12"/>
       <c r="F182" s="12" t="s">
-        <v>7713</v>
+        <v>7712</v>
       </c>
       <c r="G182" s="12"/>
       <c r="H182" s="12"/>
@@ -76026,10 +76026,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>7856</v>
+        <v>7855</v>
       </c>
       <c r="C183" t="s">
-        <v>7707</v>
+        <v>7706</v>
       </c>
       <c r="D183" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -76037,7 +76037,7 @@
       </c>
       <c r="E183" s="12"/>
       <c r="F183" s="12" t="s">
-        <v>7714</v>
+        <v>7713</v>
       </c>
       <c r="G183" s="12"/>
       <c r="H183" s="12"/>
@@ -76048,10 +76048,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>7704</v>
+        <v>7703</v>
       </c>
       <c r="C184" t="s">
-        <v>7708</v>
+        <v>7707</v>
       </c>
       <c r="D184" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -76059,7 +76059,7 @@
       </c>
       <c r="E184" s="12"/>
       <c r="F184" s="12" t="s">
-        <v>7715</v>
+        <v>7714</v>
       </c>
       <c r="G184" s="12"/>
       <c r="H184" s="12"/>
@@ -76070,10 +76070,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>7851</v>
+        <v>7850</v>
       </c>
       <c r="C185" t="s">
-        <v>7709</v>
+        <v>7708</v>
       </c>
       <c r="D185" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -76081,7 +76081,7 @@
       </c>
       <c r="E185" s="12"/>
       <c r="F185" s="12" t="s">
-        <v>7716</v>
+        <v>7715</v>
       </c>
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
@@ -76092,10 +76092,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>7852</v>
+        <v>7851</v>
       </c>
       <c r="C186" t="s">
-        <v>7710</v>
+        <v>7709</v>
       </c>
       <c r="D186" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -76103,7 +76103,7 @@
       </c>
       <c r="E186" s="12"/>
       <c r="F186" s="12" t="s">
-        <v>7717</v>
+        <v>7716</v>
       </c>
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
@@ -76114,10 +76114,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>7853</v>
+        <v>7852</v>
       </c>
       <c r="C187" t="s">
-        <v>7711</v>
+        <v>7710</v>
       </c>
       <c r="D187" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -76125,7 +76125,7 @@
       </c>
       <c r="E187" s="12"/>
       <c r="F187" s="12" t="s">
-        <v>7718</v>
+        <v>7717</v>
       </c>
       <c r="G187" s="12"/>
       <c r="H187" s="12"/>
@@ -76156,7 +76156,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B189" s="17" t="s">
-        <v>7865</v>
+        <v>7864</v>
       </c>
       <c r="C189" s="18" t="s">
         <v>323</v>
@@ -76474,7 +76474,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B203" s="17" t="s">
-        <v>7847</v>
+        <v>7846</v>
       </c>
       <c r="C203" s="18" t="s">
         <v>604</v>
@@ -76514,7 +76514,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B205" s="17" t="s">
-        <v>7848</v>
+        <v>7847</v>
       </c>
       <c r="C205" s="18" t="s">
         <v>602</v>
@@ -76536,7 +76536,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B206" s="17" t="s">
-        <v>7849</v>
+        <v>7848</v>
       </c>
       <c r="C206" s="18" t="s">
         <v>565</v>
@@ -76746,7 +76746,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>7846</v>
+        <v>7845</v>
       </c>
       <c r="C216" s="12"/>
       <c r="D216" s="12" t="str">
@@ -76809,7 +76809,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>7844</v>
+        <v>7843</v>
       </c>
       <c r="C219" s="12" t="s">
         <v>572</v>
@@ -76833,7 +76833,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>7845</v>
+        <v>7844</v>
       </c>
       <c r="C220" s="12"/>
       <c r="D220" s="12" t="str">
@@ -77450,7 +77450,7 @@
         <v>492</v>
       </c>
       <c r="C247" s="52" t="s">
-        <v>7679</v>
+        <v>7678</v>
       </c>
       <c r="D247" s="18" t="str">
         <f>Enums!$A$22</f>
@@ -77458,11 +77458,11 @@
       </c>
       <c r="E247" s="12"/>
       <c r="F247" s="12" t="s">
-        <v>7682</v>
+        <v>7681</v>
       </c>
       <c r="G247" s="12"/>
       <c r="H247" s="12" t="s">
-        <v>7680</v>
+        <v>7679</v>
       </c>
     </row>
     <row r="248" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -78175,7 +78175,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>7697</v>
+        <v>7696</v>
       </c>
       <c r="C278" s="12"/>
       <c r="D278" s="12" t="str">
@@ -78193,7 +78193,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>7698</v>
+        <v>7697</v>
       </c>
       <c r="C279" s="12"/>
       <c r="D279" s="12" t="str">
@@ -78211,7 +78211,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>7699</v>
+        <v>7698</v>
       </c>
       <c r="C280" s="12"/>
       <c r="D280" s="12" t="str">
@@ -78667,7 +78667,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B301" s="17" t="s">
-        <v>7743</v>
+        <v>7742</v>
       </c>
       <c r="C301" s="18" t="s">
         <v>327</v>
@@ -79008,7 +79008,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>7728</v>
+        <v>7727</v>
       </c>
       <c r="C316" s="14"/>
       <c r="D316" s="12" t="str">
@@ -79349,10 +79349,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>7737</v>
+        <v>7736</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>7736</v>
+        <v>7735</v>
       </c>
       <c r="D336" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79368,10 +79368,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B337" s="1" t="s">
+        <v>7737</v>
+      </c>
+      <c r="C337" s="1" t="s">
         <v>7738</v>
-      </c>
-      <c r="C337" s="1" t="s">
-        <v>7739</v>
       </c>
       <c r="D337" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79384,10 +79384,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B338" s="1" t="s">
+        <v>7739</v>
+      </c>
+      <c r="C338" s="1" t="s">
         <v>7740</v>
-      </c>
-      <c r="C338" s="1" t="s">
-        <v>7741</v>
       </c>
       <c r="D338" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79400,7 +79400,7 @@
         <v>1.0.4</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>7750</v>
+        <v>7749</v>
       </c>
       <c r="C339" s="12" t="s">
         <v>693</v>
@@ -79416,7 +79416,7 @@
         <v>1.0.4</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>7751</v>
+        <v>7750</v>
       </c>
       <c r="D340" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79429,7 +79429,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>7781</v>
+        <v>7780</v>
       </c>
       <c r="D341" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79442,7 +79442,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>7782</v>
+        <v>7781</v>
       </c>
       <c r="D342" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79455,7 +79455,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>7783</v>
+        <v>7782</v>
       </c>
       <c r="D343" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79468,7 +79468,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>7784</v>
+        <v>7783</v>
       </c>
       <c r="D344" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79481,7 +79481,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>7785</v>
+        <v>7784</v>
       </c>
       <c r="D345" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79494,7 +79494,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>7786</v>
+        <v>7785</v>
       </c>
       <c r="D346" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79507,7 +79507,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>7787</v>
+        <v>7786</v>
       </c>
       <c r="D347" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79520,7 +79520,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>7788</v>
+        <v>7787</v>
       </c>
       <c r="D348" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79533,7 +79533,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>7789</v>
+        <v>7788</v>
       </c>
       <c r="D349" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79549,7 +79549,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>7791</v>
+        <v>7790</v>
       </c>
       <c r="D350" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79565,10 +79565,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B351" s="1" t="s">
+        <v>7791</v>
+      </c>
+      <c r="C351" s="1" t="s">
         <v>7792</v>
-      </c>
-      <c r="C351" s="1" t="s">
-        <v>7793</v>
       </c>
       <c r="D351" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79581,10 +79581,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B352" s="1" t="s">
+        <v>7816</v>
+      </c>
+      <c r="C352" s="1" t="s">
         <v>7817</v>
-      </c>
-      <c r="C352" s="1" t="s">
-        <v>7818</v>
       </c>
       <c r="D352" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79600,10 +79600,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B353" s="1" t="s">
+        <v>7818</v>
+      </c>
+      <c r="C353" s="1" t="s">
         <v>7819</v>
-      </c>
-      <c r="C353" s="1" t="s">
-        <v>7820</v>
       </c>
       <c r="D353" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79619,10 +79619,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>7822</v>
+        <v>7821</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>7821</v>
+        <v>7820</v>
       </c>
       <c r="D354" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79635,10 +79635,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B355" s="1" t="s">
+        <v>7823</v>
+      </c>
+      <c r="C355" t="s">
         <v>7824</v>
-      </c>
-      <c r="C355" t="s">
-        <v>7825</v>
       </c>
       <c r="D355" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79651,7 +79651,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>7834</v>
+        <v>7833</v>
       </c>
       <c r="D356" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79664,7 +79664,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>7835</v>
+        <v>7834</v>
       </c>
       <c r="D357" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79677,7 +79677,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>7836</v>
+        <v>7835</v>
       </c>
       <c r="D358" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79690,7 +79690,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>7837</v>
+        <v>7836</v>
       </c>
       <c r="D359" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79703,7 +79703,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>7838</v>
+        <v>7837</v>
       </c>
       <c r="D360" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79716,7 +79716,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>7839</v>
+        <v>7838</v>
       </c>
       <c r="D361" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79729,7 +79729,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>7840</v>
+        <v>7839</v>
       </c>
       <c r="D362" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79742,7 +79742,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>7842</v>
+        <v>7841</v>
       </c>
       <c r="D363" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79755,7 +79755,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>7843</v>
+        <v>7842</v>
       </c>
       <c r="D364" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79768,7 +79768,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>7862</v>
+        <v>7861</v>
       </c>
       <c r="D365" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79781,7 +79781,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>7863</v>
+        <v>7862</v>
       </c>
       <c r="D366" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79794,7 +79794,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>7864</v>
+        <v>7863</v>
       </c>
       <c r="D367" s="12" t="str">
         <f>Enums!$A$22</f>
@@ -79807,7 +79807,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>7866</v>
+        <v>7865</v>
       </c>
       <c r="D368" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79820,7 +79820,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>7867</v>
+        <v>7866</v>
       </c>
       <c r="D369" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79833,7 +79833,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>7868</v>
+        <v>7867</v>
       </c>
       <c r="D370" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79846,7 +79846,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>7904</v>
+        <v>7903</v>
       </c>
       <c r="D371" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79859,7 +79859,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>7905</v>
+        <v>7904</v>
       </c>
       <c r="D372" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79872,7 +79872,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>7874</v>
+        <v>7873</v>
       </c>
       <c r="D373" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79885,7 +79885,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>7877</v>
+        <v>7876</v>
       </c>
       <c r="D374" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79898,7 +79898,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>7899</v>
+        <v>7898</v>
       </c>
       <c r="D375" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79911,7 +79911,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>7878</v>
+        <v>7877</v>
       </c>
       <c r="D376" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79937,7 +79937,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>7879</v>
+        <v>7878</v>
       </c>
       <c r="D378" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79950,7 +79950,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>7880</v>
+        <v>7879</v>
       </c>
       <c r="D379" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79963,7 +79963,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>7881</v>
+        <v>7880</v>
       </c>
       <c r="D380" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -79976,7 +79976,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>7882</v>
+        <v>7881</v>
       </c>
       <c r="D381" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -79989,7 +79989,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>7883</v>
+        <v>7882</v>
       </c>
       <c r="D382" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80002,7 +80002,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>7884</v>
+        <v>7883</v>
       </c>
       <c r="D383" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80018,7 +80018,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>7885</v>
+        <v>7884</v>
       </c>
       <c r="D384" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80034,7 +80034,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>7886</v>
+        <v>7885</v>
       </c>
       <c r="D385" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80047,7 +80047,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>7887</v>
+        <v>7886</v>
       </c>
       <c r="D386" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80060,7 +80060,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>7888</v>
+        <v>7887</v>
       </c>
       <c r="D387" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80073,7 +80073,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>7889</v>
+        <v>7888</v>
       </c>
       <c r="D388" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80086,7 +80086,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>7895</v>
+        <v>7894</v>
       </c>
       <c r="D389" s="12" t="str">
         <f>Enums!$A$22</f>
@@ -80099,10 +80099,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B390" s="1" t="s">
+        <v>7895</v>
+      </c>
+      <c r="C390" s="1" t="s">
         <v>7896</v>
-      </c>
-      <c r="C390" s="1" t="s">
-        <v>7897</v>
       </c>
       <c r="D390" s="12" t="str">
         <f>Enums!$A$20</f>
@@ -80115,7 +80115,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>7898</v>
+        <v>7897</v>
       </c>
       <c r="D391" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80128,10 +80128,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>7903</v>
+        <v>7902</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>7900</v>
+        <v>7899</v>
       </c>
       <c r="D392" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80144,10 +80144,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B393" s="1" t="s">
+        <v>7900</v>
+      </c>
+      <c r="C393" s="1" t="s">
         <v>7901</v>
-      </c>
-      <c r="C393" s="1" t="s">
-        <v>7902</v>
       </c>
       <c r="D393" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80160,10 +80160,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B394" s="1" t="s">
+        <v>7905</v>
+      </c>
+      <c r="C394" s="1" t="s">
         <v>7906</v>
-      </c>
-      <c r="C394" s="1" t="s">
-        <v>7907</v>
       </c>
       <c r="D394" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80176,7 +80176,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>7908</v>
+        <v>7907</v>
       </c>
       <c r="D395" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80189,7 +80189,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>7909</v>
+        <v>7908</v>
       </c>
       <c r="D396" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80202,7 +80202,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>7910</v>
+        <v>7909</v>
       </c>
       <c r="D397" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80215,7 +80215,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>7911</v>
+        <v>7910</v>
       </c>
       <c r="D398" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80228,7 +80228,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>7912</v>
+        <v>7911</v>
       </c>
       <c r="D399" s="12" t="str">
         <f>Enums!$A$21</f>
@@ -80277,7 +80277,7 @@
         <v>1335</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>7794</v>
+        <v>7793</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>1334</v>
@@ -80322,10 +80322,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>7799</v>
+        <v>7798</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>7798</v>
+        <v>7797</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -80445,10 +80445,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>7826</v>
+        <v>7825</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7826</v>
+        <v>7825</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -80634,7 +80634,7 @@
         <v>1310</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7800</v>
+        <v>7799</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -80728,10 +80728,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>7893</v>
+        <v>7892</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7823</v>
+        <v>7822</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -80847,7 +80847,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>7694</v>
+        <v>7693</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>1295</v>
@@ -80969,7 +80969,7 @@
         <v>1.0.0</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>7773</v>
+        <v>7772</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>1286</v>
@@ -80996,7 +80996,7 @@
         <v>1285</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>7797</v>
+        <v>7796</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -81139,10 +81139,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B36" s="33" t="s">
+        <v>7871</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>7872</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>7873</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -81187,10 +81187,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>7813</v>
+        <v>7812</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>7815</v>
+        <v>7814</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -81211,10 +81211,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>7814</v>
+        <v>7813</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>7816</v>
+        <v>7815</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -81470,7 +81470,7 @@
         <v>1254</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>7831</v>
+        <v>7830</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -81710,7 +81710,7 @@
         <v>1234</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>7832</v>
+        <v>7831</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -81874,7 +81874,7 @@
         <v>1221</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>7795</v>
+        <v>7794</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -82038,7 +82038,7 @@
         <v>1208</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>7869</v>
+        <v>7868</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -82132,7 +82132,7 @@
         <v>1201</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>7796</v>
+        <v>7795</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -82248,7 +82248,7 @@
         <v>1192</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>7780</v>
+        <v>7779</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -82994,10 +82994,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>7734</v>
+        <v>7733</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>7733</v>
+        <v>7732</v>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -83016,10 +83016,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>7913</v>
+        <v>7912</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>7915</v>
+        <v>7914</v>
       </c>
       <c r="D116" t="b">
         <v>0</v>
@@ -83038,10 +83038,10 @@
         <v>1.1.2</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>7914</v>
+        <v>7913</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>7916</v>
+        <v>7915</v>
       </c>
       <c r="D117" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed a loophole to get infinite oil. Removed a wayward distillation recipe.
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="88965" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="1"/>
+    <workbookView xWindow="88965" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -25937,7 +25937,7 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -26230,7 +26230,7 @@
   </sheetPr>
   <dimension ref="A1:E5417"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added improved textures for water cannon and freeze ray
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="88965" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="9"/>
+    <workbookView xWindow="88965" yWindow="555" windowWidth="19125" windowHeight="19395" tabRatio="860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -25937,7 +25937,7 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -59790,7 +59790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
       <selection activeCell="I175" sqref="I175"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1.3.2 Added cleanroom and associated processing
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7990" uniqueCount="7750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7992" uniqueCount="7752">
   <si>
     <t>Uuo</t>
   </si>
@@ -23832,6 +23832,12 @@
   </si>
   <si>
     <t>Cinnabar</t>
+  </si>
+  <si>
+    <t>1bY</t>
+  </si>
+  <si>
+    <t>1bZ</t>
   </si>
 </sst>
 </file>
@@ -25842,7 +25848,7 @@
   <dimension ref="A1:F5241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25865,6 +25871,16 @@
       </c>
       <c r="F5" s="35" t="s">
         <v>6619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="35" t="s">
+        <v>7750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="35" t="s">
+        <v>7751</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update to 1.3.5 - restricted communication, cleanrooms
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="860"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -24463,8 +24463,8 @@
   </sheetPr>
   <dimension ref="A1:C154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25763,8 +25763,8 @@
   </sheetPr>
   <dimension ref="A1:E5201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated recipes to return some catalyst in chemical processor
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\polycraftWorkStuff\PolyCraft_Forge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\polycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7861" uniqueCount="7621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7862" uniqueCount="7622">
   <si>
     <t>Uuo</t>
   </si>
@@ -23444,6 +23444,9 @@
   </si>
   <si>
     <t>1.4.4</t>
+  </si>
+  <si>
+    <t>1.4.5</t>
   </si>
 </sst>
 </file>
@@ -24202,10 +24205,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B164" sqref="B164"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25236,7 +25239,15 @@
       <c r="B163" s="54">
         <v>42917</v>
       </c>
-      <c r="C163" s="1" t="s">
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>7621</v>
+      </c>
+      <c r="B164" s="54">
+        <v>42936</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>7617</v>
       </c>
     </row>
@@ -57510,7 +57521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A155" workbookViewId="0">
+    <sheetView topLeftCell="A161" workbookViewId="0">
       <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added merox treatment unit image and recipe changes
</commit_message>
<xml_diff>
--- a/config/Polycraft Inputs.xlsx
+++ b/config/Polycraft Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17670" yWindow="0" windowWidth="5520" windowHeight="9045" tabRatio="860" activeTab="1"/>
+    <workbookView xWindow="17670" yWindow="0" windowWidth="5520" windowHeight="9045" tabRatio="860" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="10" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7862" uniqueCount="7622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7864" uniqueCount="7623">
   <si>
     <t>Uuo</t>
   </si>
@@ -23447,6 +23447,9 @@
   </si>
   <si>
     <t>1.4.5</t>
+  </si>
+  <si>
+    <t>Heavy Naphthenes</t>
   </si>
 </sst>
 </file>
@@ -25596,7 +25599,7 @@
   </sheetPr>
   <dimension ref="A1:E5088"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -69580,11 +69583,11 @@
   </sheetPr>
   <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C374" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="B404" sqref="B404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -77969,7 +77972,16 @@
       </c>
     </row>
     <row r="404" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D404" s="12"/>
+      <c r="A404" s="1" t="s">
+        <v>7620</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>7622</v>
+      </c>
+      <c r="D404" s="12" t="str">
+        <f>Enums!$A$3</f>
+        <v>Liquid</v>
+      </c>
     </row>
     <row r="405" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D405" s="12"/>

</xml_diff>